<commit_message>
Data now in one excel sheet and tabs are being closed
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\win2k19-dc2.home.lab\home\Angela\Documents\UiPath\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11778270-5441-45B1-9B11-E075267E49FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5647E27-EEED-4B07-8B24-C830B8408FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>The Equalizer 3</t>
   </si>
@@ -295,12 +295,631 @@
   </si>
   <si>
     <t>https://www.boxofficemojo.com/release/rl1303282433/?ref_=bo_md_table_43</t>
+  </si>
+  <si>
+    <t>Antoine Fuqua</t>
+  </si>
+  <si>
+    <t>Columbia PicturesEagle PicturesEscape Artists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Tarak Ben Ammar
+          ...
+            executive producer
+ Todd Black
+          ...
+            producer (produced by) (p.g.a.)
+ David Bloomfield
+          ...
+            executive producer
+ Jason Blumenthal
+          ...
+            producer (produced by) (p.g.a.)
+ Vito Colazzo
+          ...
+            line producer
+ Tony Eldridge
+          ...
+            producer (produced by)
+ Antoine Fuqua
+          ...
+            producer (produced by) (p.g.a.)
+ Andy Mitchell
+          ...
+            executive producer
+ Samir M. Patel
+          ...
+            executive producer (as Samir Patel)
+ Guja Quaranta
+          ...
+            associate producer
+ Kat Samick
+          ...
+            executive producer
+ Alex Siskin
+          ...
+            producer (produced by)
+ Enzo Sisti
+          ...
+            executive producer
+ Michael Sloan
+          ...
+            producer (produced by)
+ Steve Tisch
+          ...
+            producer (produced by)
+ Clayton Townsend
+          ...
+            producer (produced by) (p.g.a.)
+ Denzel Washington
+          ...
+            producer (produced by)
+ Richard Wenk
+          ...
+            co-producer
+    </t>
+  </si>
+  <si>
+    <t>Michael Chaves</t>
+  </si>
+  <si>
+    <t>$38,000,000 (estimated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ John Bernard
+          ...
+            line producer
+ Richard Brener
+          ...
+            executive producer
+ Michael Clear
+          ...
+            executive producer
+ Gary Dauberman
+          ...
+            executive producer
+ Tricia Miles
+          ...
+            associate producer (as Tricia Miles Tharp)
+ Dave Neustadter
+          ...
+            executive producer
+ Victoria Palmeri
+          ...
+            executive producer
+ Michael Polaire
+          ...
+            executive producer
+ Peter Safran
+          ...
+            producer (produced by) (p.g.a.)
+ Judson Scott
+          ...
+            executive producer
+ James Wan
+          ...
+            producer (produced by) (p.g.a.)
+    </t>
+  </si>
+  <si>
+    <t>Kenneth Branagh</t>
+  </si>
+  <si>
+    <t>20th Century StudiosKinberg GenreScott Free Productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Enrico Ballarin
+          ...
+            line producer: Venice
+ Kenneth Branagh
+          ...
+            producer (p.g.a.)
+ Martin Curry
+          ...
+            associate producer
+ Mark Gordon
+          ...
+            executive producer
+ Judy Hofflund
+          ...
+            producer (p.g.a.)
+ Louise Killin
+          ...
+            executive producer
+ Simon Kinberg
+          ...
+            producer
+ James Prichard
+          ...
+            executive producer
+ Ridley Scott
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Nia Vardalos</t>
+  </si>
+  <si>
+    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Paul Brooks
+          ...
+            executive producer
+ Michael P. Flannigan
+          ...
+            executive producer
+ Gary Goetzman
+          ...
+            producer
+ Tom Hanks
+          ...
+            producer
+ Scott Niemeyer
+          ...
+            executive producer
+ Eric Quijano
+          ...
+            associate producer
+ Kostas Raftopoulos
+          ...
+            line producer: Greece
+ Steve Shareshian
+          ...
+            executive producer
+ Julie Shimer
+          ...
+            associate producer (as Julie Shimer Lawrence)
+ Jonathan Shore
+          ...
+            co-producer
+ Nia Vardalos
+          ...
+            executive producer
+ Rita Wilson
+          ...
+            producer (produced by) (p.g.a)
+    </t>
+  </si>
+  <si>
+    <t>Cal Brunker</t>
+  </si>
+  <si>
+    <t>Nickelodeon Animation StudiosNickelodeon MoviesParamount Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Bob Barlen
+          ...
+            associate producer
+ Adam Beder
+          ...
+            executive producer
+ Laura Clunie
+          ...
+            producer (produced by) (p.g.a.)
+ Andre Coutu
+          ...
+            post producer
+ Jennifer Dodge
+          ...
+            producer (produced by) (p.g.a.)
+ Pierre Escande
+          ...
+            executive producer: Mikros Animation
+ Ronnen Harary
+          ...
+            executive producer
+ Julie Marouzé
+          ...
+            line producer: Mikros Animation
+ Peter Schlessel
+          ...
+            executive producer
+ Toni Stevens
+          ...
+            producer (produced by) (p.g.a.)
+ Laurence Vacher
+          ...
+            executive producer: Mikros Animation
+    </t>
+  </si>
+  <si>
+    <t>Kevin Greutert</t>
+  </si>
+  <si>
+    <t>Mexico City, Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Mark Burg
+          ...
+            producer
+ Jason Constantine
+          ...
+            executive producer
+ Daniel J. Heffner
+          ...
+            executive producer (as Daniel Jason Heffner)
+ Gregg Hoffman
+          ...
+            executive producer
+ Ketura Kestin
+          ...
+            executive producer
+ Oren Koules
+          ...
+            producer
+ Ulrich Maier
+          ...
+            producer: mexico
+ Mindy Sheldon
+          ...
+            co-producer
+ Stacey Testro
+          ...
+            executive producer
+ James Wan
+          ...
+            executive producer
+ Leigh Whannell
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Gareth Edwards</t>
+  </si>
+  <si>
+    <t>20th Century StudiosNew Regency ProductionsEntertainment One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Courtney Cunniff
+          ...
+            co-producer (as Courtney L. Cunniff)
+ Gareth Edwards
+          ...
+            producer (p.g.a.)
+ Zev Foreman
+          ...
+            executive producer
+ Greig Fraser
+          ...
+            co-producer
+ Kiri Hart
+          ...
+            producer
+ Natalie Lehmann
+          ...
+            executive producer
+ Nick Meyer
+          ...
+            executive producer
+ Arnon Milchan
+          ...
+            producer
+ Yariv Milchan
+          ...
+            executive producer
+ Galileo Mondol
+          ...
+            producer: Los Angeles unit
+ Chidchanok Plodripu
+          ...
+            line producer: Thailand (as Chidchanok 'Pam' Plodripu)
+ Ace Salvador
+          ...
+            producer: Los Angeles unit
+ Michael Schaefer
+          ...
+            executive producer
+ Nicholas Simon
+          ...
+            co-producer
+ Jim Spencer
+          ...
+            producer (p.g.a.)
+    </t>
+  </si>
+  <si>
+    <t>Atlee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Gauri Khan
+          ...
+            producer
+ Gaurav Verma
+          ...
+            co-producer
+    </t>
+  </si>
+  <si>
+    <t>Scott Waugh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Vessela Banzourkova
+          ...
+            line producer
+ Christa Campbell
+          ...
+            executive producer
+ Guymon Casady
+          ...
+            executive producer
+ Spenser Cohen
+          ...
+            executive producer
+ Michael S. Constable
+          ...
+            executive producer
+ Jason Constantine
+          ...
+            executive producer
+ Allen Dam
+          ...
+            executive producer
+ Boaz Davidson
+          ...
+            executive producer
+ Jon Feltheimer
+          ...
+            executive producer
+ Claiton Fernandes
+          ...
+            co-executive producer
+ Vladimir Fernandes
+          ...
+            co-executive producer
+ Jeffrey Greenstein
+          ...
+            executive producer
+ Lati Grobman
+          ...
+            executive producer
+ Victor Hadida
+          ...
+            co-executive producer
+ Anna Halberg
+          ...
+            executive producer
+ Basil Iwanyk
+          ...
+            executive producer
+ K. Blaine Johnston
+          ...
+            executive producer
+ Eda Kowan
+          ...
+            executive producer
+ Avi Lerner
+          ...
+            executive producer
+ Yariv Lerner
+          ...
+            producer
+ Gisella Marengo
+          ...
+            co-producer
+ Balan Melarkode
+          ...
+            co-executive producer
+ Abby Mills
+          ...
+            co-producer
+ Euzebio Munhoz Jr.
+          ...
+            co-executive producer
+ Matthew O'Toole
+          ...
+            co-producer
+ Stephen Paul
+          ...
+            executive producer
+ Lonnie Ramati
+          ...
+            co-executive producer
+ Trevor Short
+          ...
+            executive producer
+ Jason Statham
+          ...
+            producer
+ Kevin King Templeton
+          ...
+            producer
+ Robert Van Norden
+          ...
+            executive producer
+ Les Weldon
+          ...
+            producer
+ Gareth West
+          ...
+            executive producer
+ Christopher Woodrow
+          ...
+            executive producer
+ Jonathan Yunger
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Craig Gillespie</t>
+  </si>
+  <si>
+    <t>$30,000,000 (estimated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Rebecca Angelo
+          ...
+            executive producer
+ Lauren Schuker Blum
+          ...
+            executive producer
+ Loren Brock
+          ...
+            line producer: LA unit
+ Christopher Casanova
+          ...
+            co-producer
+ John Friedberg
+          ...
+            executive producer
+ Craig Gillespie
+          ...
+            producer
+ Michael Heimler
+          ...
+            executive producer
+ Johnny Holland
+          ...
+            executive producer
+ Ben Mezrich
+          ...
+            executive producer
+ Johnny Pariseau
+          ...
+            co-producer
+ Aaron Ryder
+          ...
+            producer (produced by) (p.g.a.)
+ Teddy Schwarzman
+          ...
+            producer
+ Claire Severance
+          ...
+            associate producer
+ Andrew Swett
+          ...
+            executive producer
+ Kevin Ulrich
+          ...
+            executive producer
+ Cameron Winklevoss
+          ...
+            executive producer
+ Tyler Winklevoss
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Andrew Hyatt</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Dan Campbell
+          ...
+            associate producer
+ Zach Dasher
+          ...
+            producer
+ Troy Duhon
+          ...
+            executive producer
+ Bob Katz
+          ...
+            executive producer
+ Robert Katz
+          ...
+            producer
+ Jason Melton
+          ...
+            executive producer
+ Shelley D. Needham
+          ...
+            line producer
+ Cole Prine
+          ...
+            producer
+ Korie Robertson
+          ...
+            producer
+ Willie Robertson
+          ...
+            executive producer
+ Jeremy John Wells
+          ...
+            executive producer
+ Brittany Yost
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Bishal Dutta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Arielle Boisvert
+          ...
+            executive producer
+ Jeff Deutchman
+          ...
+            executive producer
+ Ryan Friscia
+          ...
+            executive producer
+ Edward H. Hamm Jr.
+          ...
+            executive producer
+ Raymond Mansfield
+          ...
+            producer
+ Sean McKittrick
+          ...
+            producer
+ Jameson Parker
+          ...
+            executive producer
+ Tom Quinn
+          ...
+            executive producer
+ Emily Thomas
+          ...
+            executive producer
+ Shawn Williamson
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Jonathan Demme</t>
+  </si>
+  <si>
+    <t>Talking Heads: Stop Making Sense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Gary Goetzman
+          ...
+            producer
+ Gary Kurfirst
+          ...
+            executive producer
+    </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,8 +949,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,13 +1269,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -662,8 +1285,17 @@
       <c r="C1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -673,8 +1305,17 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -684,8 +1325,17 @@
       <c r="C3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -695,8 +1345,17 @@
       <c r="C4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -706,8 +1365,17 @@
       <c r="C5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -717,8 +1385,17 @@
       <c r="C6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -728,8 +1405,17 @@
       <c r="C7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -739,8 +1425,17 @@
       <c r="C8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="2">
+        <v>14600569</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -750,8 +1445,17 @@
       <c r="C9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="2">
+        <v>13508046</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -761,8 +1465,17 @@
       <c r="C10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -772,8 +1485,17 @@
       <c r="C11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -783,8 +1505,17 @@
       <c r="C12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5102192</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -794,8 +1525,17 @@
       <c r="C13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -806,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -817,7 +1557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
try catch implemented and trying new studio selector
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\win2k19-dc2.home.lab\home\Angela\Documents\UiPath\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5647E27-EEED-4B07-8B24-C830B8408FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD289C3D-D932-41A9-BC23-15AB4A2D6BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="182">
   <si>
     <t>The Equalizer 3</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Antoine Fuqua</t>
-  </si>
-  <si>
-    <t>Columbia PicturesEagle PicturesEscape Artists</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -364,9 +361,6 @@
     <t>Michael Chaves</t>
   </si>
   <si>
-    <t>$38,000,000 (estimated)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  John Bernard
           ...
@@ -407,9 +401,6 @@
     <t>Kenneth Branagh</t>
   </si>
   <si>
-    <t>20th Century StudiosKinberg GenreScott Free Productions</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Enrico Ballarin
           ...
@@ -444,9 +435,6 @@
     <t>Nia Vardalos</t>
   </si>
   <si>
-    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Paul Brooks
           ...
@@ -490,9 +478,6 @@
     <t>Cal Brunker</t>
   </si>
   <si>
-    <t>Nickelodeon Animation StudiosNickelodeon MoviesParamount Animation</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Bob Barlen
           ...
@@ -533,9 +518,6 @@
     <t>Kevin Greutert</t>
   </si>
   <si>
-    <t>Mexico City, Mexico</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Mark Burg
           ...
@@ -576,9 +558,6 @@
     <t>Gareth Edwards</t>
   </si>
   <si>
-    <t>20th Century StudiosNew Regency ProductionsEntertainment One</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Courtney Cunniff
           ...
@@ -756,9 +735,6 @@
     <t>Craig Gillespie</t>
   </si>
   <si>
-    <t>$30,000,000 (estimated)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Rebecca Angelo
           ...
@@ -817,9 +793,6 @@
     <t>Andrew Hyatt</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Dan Campbell
           ...
@@ -900,9 +873,6 @@
     <t>Jonathan Demme</t>
   </si>
   <si>
-    <t>Talking Heads: Stop Making Sense</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Gary Goetzman
           ...
@@ -910,6 +880,1280 @@
  Gary Kurfirst
           ...
             executive producer
+    </t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>No studios found</t>
+  </si>
+  <si>
+    <t>$34,604,229Sep 3, 2023</t>
+  </si>
+  <si>
+    <t>$14,279,529Sep 17, 2023</t>
+  </si>
+  <si>
+    <t>$22,764,354Oct 1, 2023</t>
+  </si>
+  <si>
+    <t>$14,079,512Oct 1, 2023</t>
+  </si>
+  <si>
+    <t>2 hours 49 minutes</t>
+  </si>
+  <si>
+    <t>1 hour 43 minutes</t>
+  </si>
+  <si>
+    <t>2.39:1</t>
+  </si>
+  <si>
+    <t>$1,200,000 (estimated)</t>
+  </si>
+  <si>
+    <t>Matthew Crouch</t>
+  </si>
+  <si>
+    <t>Wuershan</t>
+  </si>
+  <si>
+    <t>Dolby Atmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Yang Du
+          ...
+            executive producer
+ William Kong
+          ...
+            executive producer
+ Barrie M. Osborne
+          ...
+            production consultant
+ Ye Sun
+          ...
+            line producer
+    </t>
+  </si>
+  <si>
+    <t>Sean Olson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Jason Lee Brown
+          ...
+            producer
+ Phillip Glasser
+          ...
+            producer
+ Brad Goen
+          ...
+            associate producer
+ Ashley Greyson
+          ...
+            executive producer
+ Sean Olson
+          ...
+            co-producer
+ Justin Vesci
+          ...
+            executive producer
+ Andy Woolard
+          ...
+            associate producer
+    </t>
+  </si>
+  <si>
+    <t>Miles Joris-Peyrafitte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Luke Daniels
+          ...
+            executive producer
+ Lizzie Friedman
+          ...
+            executive producer
+ Jeffrey Giles
+          ...
+            executive producer
+ Richard Goldberg
+          ...
+            executive producer
+ Peter Jarowey
+          ...
+            executive producer
+ Karen Lauder
+          ...
+            executive producer
+ Greg Little
+          ...
+            executive producer
+ Michael Lurie
+          ...
+            executive producer
+ Siena Oberman
+          ...
+            producer
+ Derek Rubin
+          ...
+            co-producer
+ Shaun Sanghani
+          ...
+            producer
+ Brent Stiefel
+          ...
+            executive producer
+ Hilary Swank
+          ...
+            executive producer
+ Emma Tillinger Koskoff
+          ...
+            producer
+ Peter Winther
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Aitch Alberto</t>
+  </si>
+  <si>
+    <t>1 hour 38 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Aitch Alberto
+          ...
+            executive producer
+ Meredith Bagby
+          ...
+            executive producer
+ David Boies
+          ...
+            executive producer
+ Eugenio Derbez
+          ...
+            producer
+ Nicole Flores
+          ...
+            line producer
+ Lin-Manuel Miranda
+          ...
+            producer
+ Ben Odell
+          ...
+            producer
+ Owen Panettieri
+          ...
+            co-producer
+ Chris Parker
+          ...
+            producer
+ Zack Schiller
+          ...
+            executive producer
+ Kyra Sedgwick
+          ...
+            producer
+ Dylan Sellers
+          ...
+            producer
+ Valerie Stadler
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Rudy Valdez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Carlos Santana
+    </t>
+  </si>
+  <si>
+    <t>Michael Jai White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Elliott 'Lee' Cowart
+          ...
+            co-executive producer
+ Donovan de Boer
+          ...
+            a film produced by
+ Makasha Dorsey
+          ...
+            associate producer
+ Grant Gilmore
+          ...
+            producer
+ Matthew Godbey
+          ...
+            executive producer (as Matthew Grant Godbey)
+ Robert Goldman
+          ...
+            executive producer
+ Kevin Griffo
+          ...
+            executive producer
+ Kalon Jackson
+          ...
+            co-executive producer
+ Herb Kimble
+          ...
+            executive producer
+ Byron Minns
+          ...
+            producer (as Byron Keith Minns)
+ Oscar Torres
+          ...
+            associate producer
+ Gillian White
+          ...
+            associate producer
+ Michael Jai White
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Michael A. Goorjian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Vartan Barsoumian
+          ...
+            executive producer
+ Michael A. Goorjian
+          ...
+            producer
+ Robert Patrick Malkassian
+          ...
+            producer
+ Arman Nshanian
+          ...
+            producer
+ Knarik Sargsyan
+          ...
+            line producer
+ Serj Tankian
+          ...
+            executive producer
+ Sol Tryon
+          ...
+            producer
+ Ani Vorskanyan
+          ...
+            co-producer
+    </t>
+  </si>
+  <si>
+    <t>Jim CapobiancoPierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Kat Alioshin
+          ...
+            executive producer / line producer
+ Ali Baghdadi
+          ...
+            executive producer
+ Olivier Barbier
+          ...
+            executive producer
+ Joshua A. Bevan
+          ...
+            co-executive producer
+ Jay Burnley
+          ...
+            executive producer
+ Ellen Byrne
+          ...
+            co-producer
+ Chris Capobianco
+          ...
+            executive producer
+ Jim Capobianco
+          ...
+            producer (produced by)
+ Carmella Casinelli
+          ...
+            executive producer
+ Justin Chen
+          ...
+            executive producer
+ Ryan Clarkson
+          ...
+            executive producer
+ Lorenz Evans
+          ...
+            co-executive producer
+ Lucas A. Ferrara
+          ...
+            co-executive producer
+ Raymond Fino
+          ...
+            executive producer
+ Nicolas Flory
+          ...
+            executive producer
+ Mimi Polk Gitlin
+          ...
+            executive producer
+ Don Hahn
+          ...
+            executive producer
+ Chris Ihlenfeldt
+          ...
+            co-executive producer
+ Fionnuala Jamison
+          ...
+            executive producer
+ Nathanaël Karmitz
+          ...
+            executive producer
+ David Lyons
+          ...
+            executive producer
+ Christopher Massimine
+          ...
+            executive producer
+ Keanu Mayo
+          ...
+            executive producer
+ Vince McCarthy
+          ...
+            co-producer
+ Rob McGillivray
+          ...
+            executive producer
+ Martin Metz
+          ...
+            producer
+ Steve Muench
+          ...
+            executive producer
+ Habib Paracha
+          ...
+            executive producer
+ Adrian Politowski
+          ...
+            producer
+ Robert Rippberger
+          ...
+            producer (produced by) (p.g.a.)
+ Raymond Sandra
+          ...
+            executive producer
+ Sita Saviolo
+          ...
+            executive producer
+ Laura Schlessinger
+          ...
+            executive producer
+ Jacob Michael Silva
+          ...
+            co-executive producer
+ Ben Stranahan
+          ...
+            executive producer
+ Kyle Stroud
+          ...
+            executive producer
+ Chelsea Tieu
+          ...
+            executive producer
+ Ilan Urroz
+          ...
+            executive producer
+ Phil Viardo
+          ...
+            executive producer
+ Eric Vonfeldt
+          ...
+            executive producer
+ Neuman Vong
+          ...
+            executive producer
+ Katherine Waddell
+          ...
+            executive producer
+ Jeremy Walton
+          ...
+            executive producer
+ Pierce Young
+          ...
+            executive producer
+ J.D. Zacharias
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Tyler Sansom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Cameron Arnett
+          ...
+            producer
+ Ty Carter
+          ...
+            producer
+ Steve Degrasse
+          ...
+            supervising producer
+ Brandon Feller
+          ...
+            producer
+ John French
+          ...
+            producer
+ Mark Hubbard
+          ...
+            producer
+ Will Kramer
+          ...
+            executive producer
+ Paul L. Long
+          ...
+            producer
+ Evan Mitchum
+          ...
+            producer
+ Justen Overlander
+          ...
+            executive producer
+ Eric Pavey
+          ...
+            producer
+ Mark Richt
+          ...
+            associate producer
+ Tyler Sansom
+          ...
+            producer
+ Brad J. Silverman
+          ...
+            producer
+ Chris Skomra
+          ...
+            associate producer
+    </t>
+  </si>
+  <si>
+    <t>Peter FacinelliNick Lyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Beth Bruce
+          ...
+            producer
+ Simon Crowe
+          ...
+            executive producer
+ Peter Facinelli
+          ...
+            producer
+ Joe Fernandez
+          ...
+            executive producer
+ Matthew Joynes
+          ...
+            producer
+ Nick Lyon
+          ...
+            a film by / producer
+ Xander McCabe
+          ...
+            line producer
+ Suzanne Weinert
+          ...
+            producer
+ Peter Winther
+          ...
+            producer
+ Rob Witte
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Peter Lepeniotis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ William Alexander
+          ...
+            associate producer
+ Dan Bernard
+          ...
+            executive producer
+ Yvonne M. Bernard
+          ...
+            executive producer
+ Micheline Blais
+          ...
+            co-producer
+ Victor Elizalde
+          ...
+            executive producer
+ John Gillespie
+          ...
+            executive producer / producer
+ Rakhee Gillespie
+          ...
+            executive producer
+ Mark Holdom
+          ...
+            executive producer
+ P. Jayakumar
+          ...
+            executive producer
+ Mayank Jhalani
+          ...
+            associate producer
+ Mark Kowalsky
+          ...
+            associate producer
+ Brendan McNeill
+          ...
+            associate producer
+ R.L. Stine
+          ...
+            executive producer
+ Paul Weber
+          ...
+            executive producer
+ Robert Wertheimer
+          ...
+            co-producer
+    </t>
+  </si>
+  <si>
+    <t>Kaige Chen</t>
+  </si>
+  <si>
+    <t>$4,000,000 (estimated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Feng Hsu
+          ...
+            producer
+ Jade Hsu
+          ...
+            executive producer
+ Pin Hsu
+          ...
+            executive producer
+ Zhenduo Li
+          ...
+            line producer
+ Donald Ranvaud
+          ...
+            associate producer
+ Sun Ying
+          ...
+            line producer
+ Xia Zhang
+          ...
+            line producer
+    </t>
+  </si>
+  <si>
+    <t>Francesco Tesauro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Harry Manfredini
+    </t>
+  </si>
+  <si>
+    <t>Nicol Paone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Cary Anderson
+          ...
+            executive producer
+ Jordan Beckerman
+          ...
+            producer
+ David J. Bell
+          ...
+            executive producer
+ Stephen Braun
+          ...
+            executive producer
+ Jay Burnley
+          ...
+            executive producer
+ Ash Christian
+          ...
+            executive producer
+ Anne Clements
+          ...
+            producer
+ Neal Cupersmith
+          ...
+            co-executive producer
+ Michael Day
+          ...
+            co-producer / line producer
+ James Di Giacomo
+          ...
+            executive producer
+ Nicholas Donnermeyer
+          ...
+            executive producer
+ Kahil Dotay
+          ...
+            executive producer
+ Kurt Ebner
+          ...
+            co-executive producer
+ Ulf Ek
+          ...
+            executive producer
+ Pedro Luis Cunha Farias
+          ...
+            co-executive producer
+ BK Fulton
+          ...
+            executive producer
+ Marc Fusco
+          ...
+            Creative Producer
+ Naomi George
+          ...
+            executive producer
+ David Gilbery
+          ...
+            executive producer
+ Bill Green
+          ...
+            executive producer
+ Vishwas Hannurkar
+          ...
+            executive producer
+ Matthew Helderman
+          ...
+            executive producer
+ Amanda Homer
+          ...
+            co-producer
+ Phil Hunt
+          ...
+            executive producer
+ Robert Kapp
+          ...
+            executive producer
+ Jon Keeyes
+          ...
+            producer
+ Megan Kelleher
+          ...
+            co-executive producer
+ Bill Kenwright
+          ...
+            producer
+ Tyler W. Konney
+          ...
+            executive producer
+ Bradley J Korman
+          ...
+            co-executive producer
+ Jesse Korman
+          ...
+            co-producer
+ Jason Kringstein
+          ...
+            executive producer
+ Jeffrey B. Larson
+          ...
+            co-executive producer
+ Scott Levenson
+          ...
+            executive producer
+ Jordan Yale Levine
+          ...
+            producer
+ Marina Masowietsky
+          ...
+            executive producer
+ Mark Maxey
+          ...
+            executive producer
+ Kimberly Montini
+          ...
+            co-producer
+ David Nazar
+          ...
+            executive producer
+ Ian Niles
+          ...
+            executive producer
+ Dominic Ottersbach
+          ...
+            co-producer
+ Jackie Palkovicz
+          ...
+            executive producer
+ Michael Palkovicz
+          ...
+            executive producer
+ Nicol Paone
+          ...
+            producer
+ Bradley Pilz
+          ...
+            executive producer
+ Vahik Pirhamzei
+          ...
+            Creative Producer
+ Russ Posternak
+          ...
+            executive producer
+ William Rosenfeld
+          ...
+            producer
+ Compton Ross
+          ...
+            executive producer
+ Michael J. Rothstein
+          ...
+            executive producer
+ Philip W. Shaltz
+          ...
+            executive producer
+ Richard Switzer
+          ...
+            executive producer
+ Luke Taylor
+          ...
+            executive producer
+ Dannielle Thomas
+          ...
+            producer
+ Uma Thurman
+          ...
+            producer
+ Jeffrey Tussi
+          ...
+            executive producer
+ Paul Wedgwood
+          ...
+            executive producer
+ Jason Weinberg
+          ...
+            producer
+ Nicholas Wirth
+          ...
+            executive producer
+ Jason Zibarras
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Bethann HardisonFrédéric Tcheng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Hallee Adelman
+          ...
+            executive producer
+ John Boccardo
+          ...
+            executive producer
+ Naomi Campbell
+          ...
+            executive producer
+ Lisa Cortes
+          ...
+            producer
+ James Paul Dallas
+          ...
+            Archive Producer / co-producer
+ Derek Esplin
+          ...
+            executive producer
+ Ivy Herman
+          ...
+            executive producer
+ Rebecca H. James
+          ...
+            associate producer
+ Robina Riccitiello
+          ...
+            co-executive producer
+ Rick Rosenthal
+          ...
+            executive producer
+ Nancy Stephens
+          ...
+            executive producer
+ Nancy Stephens
+          ...
+            executive producer
+ Chris Stolte
+          ...
+            co-executive producer
+ Heidi Stolte
+          ...
+            co-executive producer
+ Andrea van Beuren
+          ...
+            executive producer
+ Jeff Zimbalist
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Klaus Härö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Kaarle Aho
+          ...
+            producer
+ David Collins
+          ...
+            producer
+ Kai Nordberg
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Danny O'MalleyAlex Rivest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Paul Doucette
+ Jeff Russo
+    </t>
+  </si>
+  <si>
+    <t>Joshua TickellRebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Jan Ellison Baszucki
+          ...
+            executive producer
+ Bill Benenson
+          ...
+            executive producer
+ Laurie Benenson
+          ...
+            executive producer
+ Corinne Bourdeau
+          ...
+            co-producer
+ Rosario Dawson
+          ...
+            executive producer
+ John Paul DeJoria
+          ...
+            executive producer
+ Eric Dillon
+          ...
+            producer
+ Ryland Engelhart
+          ...
+            co-producer / executive producer
+ Pamela B. Green
+          ...
+            executive producer
+ George Gund IV
+          ...
+            executive producer
+ Gloriana Gund
+          ...
+            executive producer
+ Diane Ladd
+          ...
+            executive producer
+ Julian Lennon
+          ...
+            executive producer
+ Adam Lewis
+          ...
+            executive producer
+ Melony Lewis
+          ...
+            executive producer
+ Christopher Lindstrom
+          ...
+            executive producer
+ Christiana Musk
+          ...
+            executive producer
+ Susan Rockefeller
+          ...
+            co-producer
+ Annie Roney
+          ...
+            executive producer
+ Regina K. Scully
+          ...
+            executive producer
+ Ian Somerhalder
+          ...
+            executive producer
+ Joshua Tickell
+          ...
+            producer
+ Rebecca Harrell Tickell
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Stephen Gyllenhaal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Meredith Blake
+          ...
+            executive producer
+ Laura Bretscher
+          ...
+            associate producer
+ Kathleen Man Gyllenhaal
+          ...
+            producer
+ Stephen Gyllenhaal
+          ...
+            producer
+ Lindsay Hadley
+          ...
+            executive producer
+ Melissa Hart
+          ...
+            associate producer
+ Heather Kahlert
+          ...
+            executive producer
+ Eric M. Klein
+          ...
+            co-producer
+ Bri Lageyre
+          ...
+            associate producer
+ Ambika Leigh
+          ...
+            associate producer
+ Dina Rahban
+          ...
+            co-producer
+ Casey Rogers
+          ...
+            co-producer
+    </t>
+  </si>
+  <si>
+    <t>Richard Dewey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Richard Dewey
+          ...
+            producer
+ Nathan Epstein
+          ...
+            executive producer
+ Andy Fortenbacher
+          ...
+            producer
+ Chris Laszlo
+          ...
+            producer
+ David Light
+          ...
+            executive producer
+ Gerry Ohrstrom
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Aristotle Torres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Robert Aguilar
+          ...
+            executive producer
+ Claude Amadeo
+          ...
+            executive producer
+ Martin Cabrera
+          ...
+            executive producer
+ Justin Cirulli
+          ...
+            associate producer
+ Michael D'Alto
+          ...
+            executive producer
+ Gus Deardoff
+          ...
+            executive producer
+ Jamie Foxx
+          ...
+            producer
+ Cemí Guzmán
+          ...
+            executive producer
+ Luis Guzmán
+          ...
+            executive producer
+ Randal Sandler
+          ...
+            executive producer
+ Lizzie Shapiro
+          ...
+            producer
+ Bernie Stern
+          ...
+            line producer
+ Aristotle Torres
+          ...
+            producer
+ Chris Triana
+          ...
+            executive producer
+ Datari Turner
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Luca Balser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Pauline Chalamet
+          ...
+            producer
+ Rachel Walden
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Hiroshi Akabane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Ryuho Okawa
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>John Stalberg Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Adam Beasley
+          ...
+            executive producer
+ Cindy Bru
+          ...
+            executive producer
+ Stephen Chrisanthus
+          ...
+            co-executive producer
+ Ford Corbett
+          ...
+            producer
+ Jatin Desai
+          ...
+            executive producer
+ Arianne Fraser
+          ...
+            executive producer
+ Greg Friedman
+          ...
+            executive producer
+ David Frigerio
+          ...
+            producer
+ David Guglielmo
+          ...
+            executive producer
+ B.D. Gunnell
+          ...
+            line producer / producer
+ Avi Haas
+          ...
+            executive producer
+ Joshua Harris
+          ...
+            executive producer
+ Michael Jefferson
+          ...
+            executive producer
+ Nathan Klingher
+          ...
+            producer
+ Roy Scott MacFarland
+          ...
+            executive producer
+ Tim O'Hair
+          ...
+            executive producer
+ Delphine Perrier
+          ...
+            executive producer
+ Scott Powell
+          ...
+            co-executive producer
+ Kyle Smithson
+          ...
+            executive producer
+ Dallas Sonnier
+          ...
+            executive producer
+ John Stalberg Jr.
+          ...
+            producer
+ Anthony Standberry
+          ...
+            executive producer
+ Caleb Ward
+          ...
+            co-executive producer
+ Michael Weiss
+          ...
+            executive producer
+ Ryan Winterstern
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Jude Okwudiafor Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Carolyn Bird
+          ...
+            executive producer
+ Janice Brathwaite
+          ...
+            executive producer
+ Garfield Bryant
+          ...
+            executive producer
+ Nicole de Meneses
+          ...
+            line producer
+ Adam Okwudiafor Johnson
+          ...
+            executive producer
+ Dee Johnson
+          ...
+            executive producer
+ Joseph Okwudiafor Johnson
+          ...
+            co-producer / executive producer
+ Jude Okwudiafor Johnson
+          ...
+            producer
+ Zina Moore-McGlockton
+          ...
+            executive producer
+ Jite Okoloko
+          ...
+            executive producer
+ Angel Omoruan
+          ...
+            coordinating producer
+ Paresh Raghani
+          ...
+            executive producer
+ Jerry Stallworth
+          ...
+            executive producer
+    </t>
+  </si>
+  <si>
+    <t>Andrea Di Stefano</t>
+  </si>
+  <si>
+    <t>2.35 : 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Marco Cohen
+          ...
+            producer
+ Marco Colombo
+          ...
+            producer
+ Fabrizio Donvito
+          ...
+            producer
+ Benedetto Habib
+          ...
+            producer
+ Fabio Lombardelli
+          ...
+            line producer
+ Alessandro Mascheroni
+          ...
+            executive producer
+ Francesco Melzi d'Eril
+          ...
+            producer
+ Marco Morabito
+          ...
+            executive producer
+ Daniel Campos Pavoncelli
+          ...
+            producer
+    </t>
+  </si>
+  <si>
+    <t>Cru EnnisLee Roy Kunz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Isaac Bauman
+          ...
+            producer
+ Cru Ennis
+          ...
+            producer
+ Kane Kunz
+          ...
+            producer
+ Lee Roy Kunz
+          ...
+            producer
+ Elina Litvinova
+          ...
+            producer
+ Lili Pilt
+          ...
+            line producer
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Marc Missonnier
+          ...
+            producer
     </t>
   </si>
 </sst>
@@ -917,7 +2161,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -949,12 +2194,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,7 +2517,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1288,11 +2536,11 @@
       <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1306,13 +2554,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="3">
+        <v>233100128</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1326,13 +2574,13 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1346,13 +2594,13 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="H4" s="3">
+        <v>34987190</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1366,13 +2614,13 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" t="s">
-        <v>99</v>
+        <v>94</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1386,13 +2634,13 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="H6" s="3">
+        <v>19874313</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1406,13 +2654,13 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" t="s">
-        <v>105</v>
+        <v>98</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1426,13 +2674,13 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" s="2">
-        <v>14600569</v>
+        <v>100</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1446,13 +2694,13 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="2">
-        <v>13508046</v>
+        <v>102</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1466,13 +2714,13 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
-      </c>
-      <c r="H10" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="H10" s="3">
+        <v>8288722</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1486,13 +2734,13 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1506,13 +2754,13 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
-      </c>
-      <c r="H12" s="2">
-        <v>5102192</v>
+        <v>108</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1526,13 +2774,13 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1545,8 +2793,17 @@
       <c r="C14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1556,8 +2813,17 @@
       <c r="C15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1567,8 +2833,17 @@
       <c r="C16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1578,8 +2853,17 @@
       <c r="C17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1589,8 +2873,17 @@
       <c r="C18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1600,8 +2893,17 @@
       <c r="C19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1611,8 +2913,17 @@
       <c r="C20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1622,8 +2933,17 @@
       <c r="C21">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>137</v>
+      </c>
+      <c r="H21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1633,8 +2953,17 @@
       <c r="C22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1644,8 +2973,17 @@
       <c r="C23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1655,8 +2993,17 @@
       <c r="C24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>143</v>
+      </c>
+      <c r="H24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1666,8 +3013,17 @@
       <c r="C25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1677,8 +3033,17 @@
       <c r="C26">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>147</v>
+      </c>
+      <c r="H26" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1688,8 +3053,17 @@
       <c r="C27">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1699,8 +3073,17 @@
       <c r="C28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" t="s">
+        <v>113</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1710,8 +3093,17 @@
       <c r="C29">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>154</v>
+      </c>
+      <c r="H29" t="s">
+        <v>113</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1721,8 +3113,17 @@
       <c r="C30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" t="s">
+        <v>112</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1732,8 +3133,17 @@
       <c r="C31">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>158</v>
+      </c>
+      <c r="H31" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1743,8 +3153,17 @@
       <c r="C32">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" t="s">
+        <v>113</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1754,8 +3173,17 @@
       <c r="C33">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1765,8 +3193,17 @@
       <c r="C34">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>164</v>
+      </c>
+      <c r="H34" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1776,8 +3213,17 @@
       <c r="C35">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1787,8 +3233,17 @@
       <c r="C36">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H36" t="s">
+        <v>113</v>
+      </c>
+      <c r="I36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1798,8 +3253,17 @@
       <c r="C37">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>168</v>
+      </c>
+      <c r="H37" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="345" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1809,8 +3273,17 @@
       <c r="C38">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1820,8 +3293,17 @@
       <c r="C39">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1831,8 +3313,17 @@
       <c r="C40">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>174</v>
+      </c>
+      <c r="H40" t="s">
+        <v>113</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1842,8 +3333,17 @@
       <c r="C41">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" t="s">
+        <v>177</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1853,8 +3353,17 @@
       <c r="C42">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>179</v>
+      </c>
+      <c r="H42" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -1863,6 +3372,15 @@
       </c>
       <c r="C43">
         <v>43</v>
+      </c>
+      <c r="G43" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" t="s">
+        <v>113</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
studios and producers in for all pending formatting
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\win2k19-dc2.home.lab\home\Angela\Documents\UiPath\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD289C3D-D932-41A9-BC23-15AB4A2D6BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F2D041-40C3-4AC0-92FB-0750F0E791F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="193">
   <si>
     <t>The Equalizer 3</t>
   </si>
@@ -192,21 +192,12 @@
     <t>Farewell My Concubine</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_26</t>
-  </si>
-  <si>
     <t>The Origin of Evil</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_27</t>
-  </si>
-  <si>
     <t>The Kill Room</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_28</t>
-  </si>
-  <si>
     <t>Invisible Beauty</t>
   </si>
   <si>
@@ -216,9 +207,6 @@
     <t>My Sailor, My Love</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_30</t>
-  </si>
-  <si>
     <t>Canary</t>
   </si>
   <si>
@@ -234,13 +222,7 @@
     <t>Uncharitable</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_33</t>
-  </si>
-  <si>
     <t>Radical Wolfe</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1050837761/?ref_=bo_md_table_34</t>
   </si>
   <si>
     <t>Story Ave</t>
@@ -889,27 +871,6 @@
     <t>No studios found</t>
   </si>
   <si>
-    <t>$34,604,229Sep 3, 2023</t>
-  </si>
-  <si>
-    <t>$14,279,529Sep 17, 2023</t>
-  </si>
-  <si>
-    <t>$22,764,354Oct 1, 2023</t>
-  </si>
-  <si>
-    <t>$14,079,512Oct 1, 2023</t>
-  </si>
-  <si>
-    <t>2 hours 49 minutes</t>
-  </si>
-  <si>
-    <t>1 hour 43 minutes</t>
-  </si>
-  <si>
-    <t>2.39:1</t>
-  </si>
-  <si>
     <t>$1,200,000 (estimated)</t>
   </si>
   <si>
@@ -917,9 +878,6 @@
   </si>
   <si>
     <t>Wuershan</t>
-  </si>
-  <si>
-    <t>Dolby Atmos</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1021,9 +979,6 @@
     <t>Aitch Alberto</t>
   </si>
   <si>
-    <t>1 hour 38 minutes</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Aitch Alberto
           ...
@@ -1438,9 +1393,6 @@
     <t>Kaige Chen</t>
   </si>
   <si>
-    <t>$4,000,000 (estimated)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Feng Hsu
           ...
@@ -1466,14 +1418,6 @@
     </t>
   </si>
   <si>
-    <t>Francesco Tesauro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- Harry Manfredini
-    </t>
-  </si>
-  <si>
     <t>Nicol Paone</t>
   </si>
   <si>
@@ -2091,9 +2035,6 @@
     <t>Andrea Di Stefano</t>
   </si>
   <si>
-    <t>2.35 : 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Marco Cohen
           ...
@@ -2155,6 +2096,158 @@
           ...
             producer
     </t>
+  </si>
+  <si>
+    <t>$10,028,675Sep 10, 2023</t>
+  </si>
+  <si>
+    <t>$30,000,000 (estimated)</t>
+  </si>
+  <si>
+    <t>$6,124,963Sep 10, 2023</t>
+  </si>
+  <si>
+    <t>$2,607,665Sep 24, 2023</t>
+  </si>
+  <si>
+    <t>$489,439Sep 17, 2023</t>
+  </si>
+  <si>
+    <t>$230,205Sep 10, 2023</t>
+  </si>
+  <si>
+    <t>$178,176Sep 17, 2023</t>
+  </si>
+  <si>
+    <t>$56,584Sep 10, 2023</t>
+  </si>
+  <si>
+    <t>$190,031Sep 17, 2023</t>
+  </si>
+  <si>
+    <t>$140,005Sep 24, 2023</t>
+  </si>
+  <si>
+    <t>$84,016Sep 3, 2023</t>
+  </si>
+  <si>
+    <t>Sébastien Marnier</t>
+  </si>
+  <si>
+    <t>$47,499Sep 24, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Caroline Bonmarchand
+          ...
+            producer
+ Luc Déry
+          ...
+            co-producer
+ Kim McCraw
+          ...
+            co-producer
+    </t>
+  </si>
+  <si>
+    <t>$12,085Sep 17, 2023</t>
+  </si>
+  <si>
+    <t>Adil El ArbiBilall Fallah</t>
+  </si>
+  <si>
+    <t>$6,500Sep 17, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Anne Berger
+          ...
+            junior producer
+ Brahim Chioua
+          ...
+            co-producer
+ Marc Dujardin
+          ...
+            co-producer
+ Adil El Arbi
+          ...
+            executive producer
+ Diana Elbaum
+          ...
+            co-producer
+ Bilall Fallah
+          ...
+            executive producer
+ Jesus Gonzalez-Elvira
+          ...
+            co-producer
+ Bert Hamelinck
+          ...
+            producer
+ Saïd Hamich
+          ...
+            associate producer
+ Robin Kerremans
+          ...
+            executive producer
+ Vincent Maraval
+          ...
+            co-producer
+ Rula Nasser
+          ...
+            associate producer
+ David Ragonig
+          ...
+            line producer
+ Michael Sagol
+          ...
+            executive producer
+ Laura Scheerlinck
+          ...
+            Junior Producer
+ Dimitri Verbeeck
+          ...
+            producer
+ Clarissa Vermaak
+          ...
+            associate producer
+    </t>
+  </si>
+  <si>
+    <t>$4,913Sep 24, 2023</t>
+  </si>
+  <si>
+    <t>$4,075Oct 1, 2023</t>
+  </si>
+  <si>
+    <t>$2,496Sep 17, 2023</t>
+  </si>
+  <si>
+    <t>Frank Cimière</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_26</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_27</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_28</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_30</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1050837761/?ref_=bo_md_table_33</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_34</t>
+  </si>
+  <si>
+    <t>Production CompaniesColumbia Pictures(presents)Eagle Pictures(in association with)Escape ArtistsZHIV ProductionsSony Pictures Entertainment (SPE)TSG Entertainment(In association with)</t>
+  </si>
+  <si>
+    <t>Production CompaniesNew Line Cinema(presents)Atomic MonsterThe Safran Company</t>
   </si>
 </sst>
 </file>
@@ -2518,7 +2611,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,13 +2627,13 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>114</v>
+        <v>191</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2554,13 +2647,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="3">
-        <v>233100128</v>
+        <v>82</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2574,13 +2667,13 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>115</v>
+        <v>84</v>
+      </c>
+      <c r="H3" s="2">
+        <v>31770191</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2594,13 +2687,13 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="3">
-        <v>34987190</v>
+        <v>86</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2614,13 +2707,13 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2634,13 +2727,13 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H6" s="3">
         <v>19874313</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2654,13 +2747,13 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="H7" s="2">
+        <v>15277372</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2674,13 +2767,13 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2694,13 +2787,13 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>119</v>
+        <v>96</v>
+      </c>
+      <c r="H9" s="2">
+        <v>13508046</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2714,13 +2807,13 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H10" s="3">
-        <v>8288722</v>
+        <v>7428887</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2734,13 +2827,13 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5197594</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2754,13 +2847,13 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2774,13 +2867,13 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H13" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2794,13 +2887,13 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="H14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2814,13 +2907,13 @@
         <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
-      </c>
-      <c r="H15" t="s">
-        <v>124</v>
+        <v>110</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1422011</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2834,13 +2927,13 @@
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="H16" t="s">
+        <v>167</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2854,13 +2947,13 @@
         <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>128</v>
-      </c>
-      <c r="H17" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="H17" s="3">
+        <v>503378</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2874,13 +2967,13 @@
         <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H18" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="255" x14ac:dyDescent="0.25">
@@ -2894,13 +2987,13 @@
         <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>133</v>
-      </c>
-      <c r="H19" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="H19" s="3">
+        <v>380386</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2914,13 +3007,13 @@
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="H20" t="s">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2934,13 +3027,13 @@
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2954,13 +3047,13 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2974,13 +3067,13 @@
         <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="H23" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -2994,13 +3087,13 @@
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>143</v>
-      </c>
-      <c r="H24" t="s">
-        <v>113</v>
+        <v>128</v>
+      </c>
+      <c r="H24" s="3">
+        <v>134825</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -3014,373 +3107,373 @@
         <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="H25" t="s">
-        <v>113</v>
+        <v>173</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="C26">
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>147</v>
-      </c>
-      <c r="H26" t="s">
-        <v>148</v>
+        <v>132</v>
+      </c>
+      <c r="H26" s="3">
+        <v>5311415</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
       <c r="C27">
         <v>27</v>
       </c>
       <c r="G27" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="H27" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
       <c r="C28">
         <v>28</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
-      </c>
-      <c r="H28" t="s">
-        <v>113</v>
+        <v>134</v>
+      </c>
+      <c r="H28" s="3">
+        <v>546081</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>29</v>
       </c>
       <c r="G29" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="H29" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="C30">
         <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>156</v>
-      </c>
-      <c r="H30" t="s">
-        <v>112</v>
+        <v>138</v>
+      </c>
+      <c r="H30" s="3">
+        <v>57960</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C31">
         <v>31</v>
       </c>
       <c r="G31" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="H31" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C32">
         <v>32</v>
       </c>
       <c r="G32" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="H32" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>189</v>
       </c>
       <c r="C33">
         <v>33</v>
       </c>
       <c r="G33" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="C34">
         <v>34</v>
       </c>
       <c r="G34" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="H34" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C35">
         <v>35</v>
       </c>
       <c r="G35" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="H35" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C36">
         <v>36</v>
       </c>
       <c r="G36" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="H36" t="s">
-        <v>113</v>
-      </c>
-      <c r="I36" t="s">
-        <v>113</v>
+        <v>179</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C37">
         <v>37</v>
       </c>
       <c r="G37" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="H37" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="345" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C38">
         <v>38</v>
       </c>
       <c r="G38" t="s">
-        <v>170</v>
-      </c>
-      <c r="H38" t="s">
-        <v>113</v>
+        <v>152</v>
+      </c>
+      <c r="H38" s="3">
+        <v>7082</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C39">
         <v>39</v>
       </c>
       <c r="G39" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H39" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>40</v>
       </c>
       <c r="G40" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="H40" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C41">
         <v>41</v>
       </c>
       <c r="G41" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="H41" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C42">
         <v>42</v>
       </c>
       <c r="G42" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="H42" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C43">
         <v>43</v>
       </c>
       <c r="G43" t="s">
-        <v>113</v>
+        <v>184</v>
       </c>
       <c r="H43" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted first database row
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Group8-300-762-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B79402-C9AC-410A-8481-334D620B69BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7473549D-386B-4397-AA11-4B8C6F4D2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15816" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="5748" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -692,8 +692,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -793,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -807,7 +806,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1169,13 +1167,13 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="2">
         <v>2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="2">
         <v>3</v>
       </c>
       <c r="H2" s="2"/>

</xml_diff>

<commit_message>
Program runs with no problems. Excel changed.
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Group8-300-762-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7473549D-386B-4397-AA11-4B8C6F4D2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D55144-7718-449C-B410-151235831000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5748" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
-    <sheet name="MovieCrew" sheetId="1" r:id="rId2"/>
+    <sheet name="Director's Highest gross Films" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="317">
   <si>
     <t>Film Title</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Worldwide Gross</t>
   </si>
   <si>
-    <t>Cast and Crew</t>
-  </si>
-  <si>
     <t>Film Director</t>
   </si>
   <si>
@@ -686,6 +683,399 @@
   <si>
     <t xml:space="preserve">371,989
 </t>
+  </si>
+  <si>
+    <t>Antoine Fuqua</t>
+  </si>
+  <si>
+    <t>Columbia Pictures(presents)Eagle Pictures(in association with)Escape ArtistsZHIV ProductionsSony Pictures Entertainment (SPE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tarak Ben Ammar ... executive producer  Todd Black ... producer (produced by)(p.g.a.) David Bloomfield ... executive producer  Jason Blumenthal ... producer (produced by)(p.g.a.) Vito Colazzo ... line producer  Tony Eldridge ... producer (produced by) Antoine Fuqua ... producer (produced by)(p.g.a.) Andy Mitchell ... executive producer  Samir M. Patel ... executive producer (as Samir Patel) Guja Quaranta ... line producer  Kat Samick ... executive producer  Alex Siskin ... producer (produced by) Enzo Sisti ... executive producer  Michael Sloan ... producer (produced by) Steve Tisch ... producer (produced by) Clayton Townsend ... producer (produced by)(p.g.a.) Denzel Washington ... producer (produced by) Richard Wenk ... co-producer </t>
+  </si>
+  <si>
+    <t>Michael Chaves</t>
+  </si>
+  <si>
+    <t>New Line Cinema(presents)Atomic MonsterThe Safran Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> John Bernard ... line producer  Richard Brener ... executive producer  Michael Clear ... executive producer  Gary Dauberman ... executive producer  Tricia Miles ... associate producer (as Tricia Miles Tharp) Dave Neustadter ... executive producer  Victoria Palmeri ... executive producer  Michael Polaire ... executive producer  Peter Safran ... producer (produced by)(p.g.a.) Judson Scott ... executive producer  James Wan ... producer (produced by)(p.g.a.)</t>
+  </si>
+  <si>
+    <t>Kenneth Branagh</t>
+  </si>
+  <si>
+    <t>20th Century StudiosKinberg GenreScott Free ProductionsTSG EntertainmentThe Mark Gordon Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrico Ballarin ... line producer: Venice  Kenneth Branagh ... producer (p.g.a.) Martin Curry ... associate producer  Mark Gordon ... executive producer  Judy Hofflund ... producer (p.g.a.) Louise Killin ... executive producer  Simon Kinberg ... producer  James Prichard ... executive producer  Ridley Scott ... producer </t>
+  </si>
+  <si>
+    <t>Cal Brunker</t>
+  </si>
+  <si>
+    <t>Nickelodeon Animation StudiosNickelodeon MoviesParamount AnimationParamount PicturesSpin Master Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bob Barlen ... associate producer  Adam Beder ... executive producer  Laura Clunie ... producer (produced by)(p.g.a.) Andre Coutu ... post producer  Jennifer Dodge ... producer (produced by)(p.g.a.) Pierre Escande ... executive producer: Mikros Animation  Ronnen Harary ... executive producer  Julie Marouzé ... line producer: Mikros Animation  Peter Schlessel ... executive producer  Toni Stevens ... producer (produced by)(p.g.a.) Laurence Vacher ... executive producer: Mikros Animation </t>
+  </si>
+  <si>
+    <t>Nia Vardalos</t>
+  </si>
+  <si>
+    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)Playtone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Brooks ... executive producer  Michael P. Flannigan ... executive producer  Gary Goetzman ... producer  Tom Hanks ... producer  Scott Niemeyer ... executive producer  Eric Quijano ... associate producer  Kostas Raftopoulos ... line producer: Greece  Steve Shareshian ... executive producer  Julie Shimer ... associate producer (as Julie Shimer Lawrence) Jonathan Shore ... co-producer  Nia Vardalos ... executive producer  Rita Wilson ... producer (produced by)(p.g.a)</t>
+  </si>
+  <si>
+    <t>Kevin Greutert</t>
+  </si>
+  <si>
+    <t>Aldea M EstudiosCorazón FilmsLionsgate ProductionsLionsgateTwisted Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mark Burg ... producer  Jason Constantine ... executive producer  Daniel J. Heffner ... executive producer (as Daniel Jason Heffner) Gregg Hoffman ... executive producer  Ketura Kestin ... executive producer  Oren Koules ... producer  Ulrich Maier ... producer: mexico  Mindy Sheldon ... co-producer  Stacey Testro ... executive producer  James Wan ... executive producer  Leigh Whannell ... executive producer </t>
+  </si>
+  <si>
+    <t>Gareth Edwards</t>
+  </si>
+  <si>
+    <t>20th Century StudiosNew Regency ProductionsEntertainment One</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Courtney Cunniff ... co-producer (as Courtney L. Cunniff) Gareth Edwards ... producer (p.g.a.) Zev Foreman ... executive producer  Greig Fraser ... co-producer  Kiri Hart ... producer  Natalie Lehmann ... executive producer  Nick Meyer ... executive producer  Arnon Milchan ... producer  Yariv Milchan ... executive producer  Galileo Mondol ... producer: Los Angeles unit  Chidchanok Plodripu ... line producer: Thailand (as Chidchanok 'Pam' Plodripu) Ace Salvador ... producer: Los Angeles unit  Michael Schaefer ... executive producer  Nicholas Simon ... co-producer  Jim Spencer ... producer (p.g.a.)</t>
+  </si>
+  <si>
+    <t>Atlee</t>
+  </si>
+  <si>
+    <t>Red Chillies Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gauri Khan ... producer  Gaurav Verma ... co-producer </t>
+  </si>
+  <si>
+    <t>Scott Waugh</t>
+  </si>
+  <si>
+    <t>Campbell Grobman FilmsMedia Capital Technologies(in association with)Millennium FilmsNu Boyana Film Studios(production facilities)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vessela Banzourkova ... line producer  Christa Campbell ... executive producer  Guymon Casady ... executive producer  Spenser Cohen ... executive producer  Michael S. Constable ... executive producer  Jason Constantine ... executive producer  Allen Dam ... executive producer  Boaz Davidson ... executive producer  Jon Feltheimer ... executive producer  Claiton Fernandes ... co-executive producer  Vladimir Fernandes ... co-executive producer  Jeffrey Greenstein ... executive producer  Lati Grobman ... executive producer  Victor Hadida ... co-executive producer  Anna Halberg ... executive producer  Basil Iwanyk ... executive producer  K. Blaine Johnston ... executive producer  Eda Kowan ... executive producer  Avi Lerner ... executive producer  Yariv Lerner ... producer  Gisella Marengo ... co-producer  Balan Melarkode ... co-executive producer  Abby Mills ... co-producer  Euzebio Munhoz Jr.... co-executive producer  Matthew O'Toole ... co-producer  Stephen Paul ... executive producer  Lonnie Ramati ... co-executive producer  Trevor Short ... executive producer  Jason Statham ... producer  Kevin King Templeton ... producer  Robert Van Norden ... executive producer  Les Weldon ... producer  Gareth West ... executive producer  Christopher Woodrow ... executive producer  Jonathan Yunger ... executive producer </t>
+  </si>
+  <si>
+    <t>Craig Gillespie</t>
+  </si>
+  <si>
+    <t>Black Bear PicturesColumbia PicturesRyder Picture CompanySony Pictures Entertainment (SPE)Stage 6 Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rebecca Angelo ... executive producer  Lauren Schuker Blum ... executive producer  Loren Brock ... line producer: LA unit  Christopher Casanova ... co-producer  John Friedberg ... executive producer  Craig Gillespie ... producer  Michael Heimler ... executive producer  Johnny Holland ... executive producer  Ben Mezrich ... executive producer  Johnny Pariseau ... co-producer  Aaron Ryder ... producer (produced by)(p.g.a.) Teddy Schwarzman ... producer  Claire Severance ... associate producer  Andrew Swett ... executive producer  Kevin Ulrich ... executive producer  Cameron Winklevoss ... executive producer  Tyler Winklevoss ... executive producer </t>
+  </si>
+  <si>
+    <t>Andrew Hyatt</t>
+  </si>
+  <si>
+    <t>GND Media GroupStacey Films(in association with)Tread Lively</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dan Campbell ... associate producer  Zach Dasher ... producer  Troy Duhon ... executive producer  Bob Katz ... executive producer  Robert Katz ... producer  Jason Melton ... executive producer  Shelley D. Needham ... line producer  Cole Prine ... producer  Korie Robertson ... producer  Willie Robertson ... executive producer  Jeremy John Wells ... executive producer  Brittany Yost ... producer </t>
+  </si>
+  <si>
+    <t>Bishal Dutta</t>
+  </si>
+  <si>
+    <t>Brightlight PicturesNeonQC Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arielle Boisvert ... executive producer  Jeff Deutchman ... executive producer  Ryan Friscia ... executive producer  Edward H. Hamm Jr.... executive producer  Raymond Mansfield ... producer  Sean McKittrick ... producer  Jameson Parker ... executive producer  Tom Quinn ... executive producer  Emily Thomas ... executive producer  Shawn Williamson ... executive producer </t>
+  </si>
+  <si>
+    <t>Jonathan Demme</t>
+  </si>
+  <si>
+    <t>Talking HeadsArnold Stiefel Company(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gary Goetzman ... producer  Gary Kurfirst ... executive producer </t>
+  </si>
+  <si>
+    <t>Matthew Crouch</t>
+  </si>
+  <si>
+    <t>No studios found</t>
+  </si>
+  <si>
+    <t>No producers found</t>
+  </si>
+  <si>
+    <t>Wuershan</t>
+  </si>
+  <si>
+    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
+  </si>
+  <si>
+    <t>Sean Olson</t>
+  </si>
+  <si>
+    <t>Called Higher Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
+  </si>
+  <si>
+    <t>Miles Joris-Peyrafitte</t>
+  </si>
+  <si>
+    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
+  </si>
+  <si>
+    <t>Aitch Alberto</t>
+  </si>
+  <si>
+    <t>Boies Schiller Entertainment3Pas Studios5000 Broadway ProductionsBig Swing ProductionsLimelight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aitch Alberto ... executive producer  Meredith Bagby ... executive producer  David Boies ... executive producer  Eugenio Derbez ... producer  Nicole Flores ... line producer  Lin-Manuel Miranda ... producer  Ben Odell ... producer  Owen Panettieri ... co-producer  Chris Parker ... producer  Zack Schiller ... executive producer  Kyra Sedgwick ... producer  Dylan Sellers ... producer  Valerie Stadler ... producer </t>
+  </si>
+  <si>
+    <t>Rudy Valdez</t>
+  </si>
+  <si>
+    <t>Imagine DocumentariesSony Music Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Santana </t>
+  </si>
+  <si>
+    <t>Michael A. Goorjian</t>
+  </si>
+  <si>
+    <t>People of ArPalodeon Pictures(In Association With)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
+  </si>
+  <si>
+    <t>Michael Jai White</t>
+  </si>
+  <si>
+    <t>Jaigantic Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
+  </si>
+  <si>
+    <t>Jim CapobiancoPierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
+  </si>
+  <si>
+    <t>Tyler Sansom</t>
+  </si>
+  <si>
+    <t>First Capital FilmsKappa Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
+  </si>
+  <si>
+    <t>Nicol Paone</t>
+  </si>
+  <si>
+    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
+  </si>
+  <si>
+    <t>Peter FacinelliNick Lyon</t>
+  </si>
+  <si>
+    <t>Lone Star StorytellersMedia GroupSC Films International</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
+  </si>
+  <si>
+    <t>Peter Lepeniotis</t>
+  </si>
+  <si>
+    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
+  </si>
+  <si>
+    <t>Kaige Chen</t>
+  </si>
+  <si>
+    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
+  </si>
+  <si>
+    <t>Sébastien Marnier</t>
+  </si>
+  <si>
+    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
+  </si>
+  <si>
+    <t>Bethann HardisonFrédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
+  </si>
+  <si>
+    <t>Klaus Härö</t>
+  </si>
+  <si>
+    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
+  </si>
+  <si>
+    <t>Stephen Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Upstream Pictures (II)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
+  </si>
+  <si>
+    <t>Danny O'MalleyAlex Rivest</t>
+  </si>
+  <si>
+    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
+  </si>
+  <si>
+    <t>Joshua TickellRebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Big Picture RanchBenenson Productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
+  </si>
+  <si>
+    <t>Richard Dewey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
+  </si>
+  <si>
+    <t>Aristotle Torres</t>
+  </si>
+  <si>
+    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
+  </si>
+  <si>
+    <t>Adil El ArbiBilall Fallah</t>
+  </si>
+  <si>
+    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
+  </si>
+  <si>
+    <t>Luca Balser</t>
+  </si>
+  <si>
+    <t>Gummy Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
+  </si>
+  <si>
+    <t>Hiroshi Akabane</t>
+  </si>
+  <si>
+    <t>HS ProductionsIRH Press Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
+  </si>
+  <si>
+    <t>John Stalberg Jr.</t>
+  </si>
+  <si>
+    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
+  </si>
+  <si>
+    <t>Jude Okwudiafor Johnson</t>
+  </si>
+  <si>
+    <t>Anchor Media Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
+  </si>
+  <si>
+    <t>Cru EnnisLee Roy Kunz</t>
+  </si>
+  <si>
+    <t>World's Fair Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
+  </si>
+  <si>
+    <t>Andrea Di Stefano</t>
+  </si>
+  <si>
+    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
+  </si>
+  <si>
+    <t>Miguel Ángel Vivas</t>
+  </si>
+  <si>
+    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
+  </si>
+  <si>
+    <t>Frank Cimière</t>
+  </si>
+  <si>
+    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marc Missonnier ... producer </t>
   </si>
 </sst>
 </file>
@@ -792,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -800,12 +1190,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,984 +1520,1319 @@
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="G6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="G9" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="G10" t="s">
+        <v>210</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="G11" t="s">
+        <v>213</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="G12" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="G13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="G14" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" t="s">
+        <v>223</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
+        <v>225</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="G16" t="s">
+        <v>228</v>
+      </c>
+      <c r="H16" t="s">
+        <v>229</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="G17" t="s">
+        <v>231</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="G18" t="s">
+        <v>234</v>
+      </c>
+      <c r="H18" t="s">
+        <v>235</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="G19" t="s">
+        <v>237</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="G20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H20" t="s">
+        <v>241</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+      <c r="G21" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21" t="s">
+        <v>244</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="G22" t="s">
+        <v>246</v>
+      </c>
+      <c r="H22" t="s">
+        <v>247</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
         <v>52</v>
-      </c>
-      <c r="B23" t="s">
-        <v>53</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="G23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H23" t="s">
+        <v>250</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="G24" t="s">
+        <v>252</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="G25" t="s">
+        <v>255</v>
+      </c>
+      <c r="H25" t="s">
+        <v>256</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="G26" t="s">
+        <v>258</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="G27" t="s">
+        <v>261</v>
+      </c>
+      <c r="H27" t="s">
+        <v>262</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="G28" t="s">
+        <v>264</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>65</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="G29" t="s">
+        <v>267</v>
+      </c>
+      <c r="H29" t="s">
+        <v>268</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
         <v>66</v>
-      </c>
-      <c r="B30" t="s">
-        <v>67</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="G30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" t="s">
-        <v>69</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="G31" t="s">
+        <v>273</v>
+      </c>
+      <c r="H31" t="s">
+        <v>274</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
         <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>71</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I32" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="G32" t="s">
+        <v>276</v>
+      </c>
+      <c r="H32" t="s">
+        <v>277</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
         <v>72</v>
-      </c>
-      <c r="B33" t="s">
-        <v>73</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="G33" t="s">
+        <v>279</v>
+      </c>
+      <c r="H33" t="s">
+        <v>280</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
         <v>74</v>
-      </c>
-      <c r="B34" t="s">
-        <v>75</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="G34" t="s">
+        <v>282</v>
+      </c>
+      <c r="H34" t="s">
+        <v>283</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
         <v>76</v>
-      </c>
-      <c r="B35" t="s">
-        <v>77</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="G35" t="s">
+        <v>285</v>
+      </c>
+      <c r="H35" t="s">
+        <v>226</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
         <v>78</v>
-      </c>
-      <c r="B36" t="s">
-        <v>79</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
+        <v>287</v>
+      </c>
+      <c r="H36" t="s">
+        <v>288</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" t="s">
         <v>80</v>
-      </c>
-      <c r="B37" t="s">
-        <v>81</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="G37" t="s">
+        <v>290</v>
+      </c>
+      <c r="H37" t="s">
+        <v>291</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
         <v>82</v>
-      </c>
-      <c r="B38" t="s">
-        <v>83</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="G38" t="s">
+        <v>293</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
         <v>84</v>
-      </c>
-      <c r="B39" t="s">
-        <v>85</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="G39" t="s">
+        <v>296</v>
+      </c>
+      <c r="H39" t="s">
+        <v>297</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
         <v>86</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="G40" t="s">
+        <v>299</v>
+      </c>
+      <c r="H40" t="s">
+        <v>300</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
         <v>88</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="G41" t="s">
+        <v>302</v>
+      </c>
+      <c r="H41" t="s">
+        <v>303</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
         <v>90</v>
-      </c>
-      <c r="B42" t="s">
-        <v>91</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="G42" t="s">
+        <v>305</v>
+      </c>
+      <c r="H42" t="s">
+        <v>306</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
         <v>92</v>
-      </c>
-      <c r="B43" t="s">
-        <v>93</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="G43" t="s">
+        <v>308</v>
+      </c>
+      <c r="H43" t="s">
+        <v>309</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
         <v>94</v>
-      </c>
-      <c r="B44" t="s">
-        <v>95</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I44" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="G44" t="s">
+        <v>311</v>
+      </c>
+      <c r="H44" t="s">
+        <v>312</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="45" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="D46" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E46" t="s">
-        <v>99</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="G45" t="s">
+        <v>314</v>
+      </c>
+      <c r="H45" t="s">
+        <v>315</v>
+      </c>
+      <c r="I45" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D46" s="1"/>
+      <c r="F46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2117,36 +2841,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C8FA34-854C-4FDF-A76D-37677D1C3B05}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="7"/>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First commit, Did annotations for the open box office mojo in edge and changed the titles. Will add a comment to it if necessary
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Group8-300-762-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssre871\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D55144-7718-449C-B410-151235831000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC85F551-9644-4EE7-94CC-9EAE2917A883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -81,27 +81,15 @@
     <t>A Haunting in Venice</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_3</t>
-  </si>
-  <si>
     <t>PAW Patrol: The Mighty Movie</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_4</t>
-  </si>
-  <si>
     <t>My Big Fat Greek Wedding 3</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_5</t>
-  </si>
-  <si>
     <t>Saw X</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_6</t>
-  </si>
-  <si>
     <t>The Creator</t>
   </si>
   <si>
@@ -231,39 +219,21 @@
     <t>The Origin of Evil</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_28</t>
-  </si>
-  <si>
     <t>Invisible Beauty</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_29</t>
-  </si>
-  <si>
     <t>My Sailor, My Love</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_30</t>
-  </si>
-  <si>
     <t>Uncharitable</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_31</t>
-  </si>
-  <si>
     <t>Canary</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_32</t>
-  </si>
-  <si>
     <t>Common Ground</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_33</t>
-  </si>
-  <si>
     <t>Radical Wolfe</t>
   </si>
   <si>
@@ -1076,6 +1046,36 @@
   </si>
   <si>
     <t xml:space="preserve"> Marc Missonnier ... producer </t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
   </si>
 </sst>
 </file>
@@ -1511,21 +1511,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1565,25 +1565,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1594,1243 +1594,1243 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>307</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>308</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>309</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G8" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G12" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G13" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="H13" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G14" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="H14" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G15" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="388.8" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="345" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G18" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H18" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G20" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="H20" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="G21" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="H21" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="H22" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G23" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="H23" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="G24" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="G25" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="H25" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G26" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G27" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H27" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="G28" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="G29" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="H29" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>312</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="G30" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>313</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="G31" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="H31" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G32" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="H32" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>315</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G33" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="H33" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>316</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G34" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="H34" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G35" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="H35" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G36" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H36" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E37" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G37" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="H37" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G38" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E39" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G39" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="H39" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E40" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G40" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="H40" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E41" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G41" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="H41" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G42" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="H42" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G43" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="H43" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="G44" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="H44" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="G45" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="H45" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="I45" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="F46" s="1"/>
     </row>
@@ -2843,20 +2843,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C8FA34-854C-4FDF-A76D-37677D1C3B05}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Played around with datatable for directors - problem with the extraction metadata
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49de3f50b24696c5/Documents/UiPath/Group8-300-762/Movie Search Data Scrape Test 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{73D55144-7718-449C-B410-151235831000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D923D7EE-E4F1-484D-8BE6-EB14732798B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FC91F7-3873-4A8E-B7E8-AE8A3C300DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9615" yWindow="2025" windowWidth="29010" windowHeight="15345" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="304">
   <si>
     <t>Film Title</t>
   </si>
@@ -99,15 +99,9 @@
     <t>Jawan</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl2106360577/?ref_=bo_md_table_8</t>
-  </si>
-  <si>
     <t>Expend4bles</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl2783019777/?ref_=bo_md_table_9</t>
-  </si>
-  <si>
     <t>Dumb Money</t>
   </si>
   <si>
@@ -249,21 +243,12 @@
     <t>Rebel</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3719136001/?ref_=bo_md_table_36</t>
-  </si>
-  <si>
     <t>What Doesn't Float</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1722778369/?ref_=bo_md_table_37</t>
-  </si>
-  <si>
     <t>Before the Sunset</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3568206593/?ref_=bo_md_table_38</t>
-  </si>
-  <si>
     <t>Muzzle</t>
   </si>
   <si>
@@ -519,25 +504,521 @@
 </t>
   </si>
   <si>
-    <t>Antoine Fuqua</t>
-  </si>
-  <si>
     <t>Columbia Pictures(presents)Eagle Pictures(in association with)Escape ArtistsZHIV ProductionsSony Pictures Entertainment (SPE)</t>
   </si>
   <si>
     <t xml:space="preserve"> Tarak Ben Ammar ... executive producer  Todd Black ... producer (produced by)(p.g.a.) David Bloomfield ... executive producer  Jason Blumenthal ... producer (produced by)(p.g.a.) Vito Colazzo ... line producer  Tony Eldridge ... producer (produced by) Antoine Fuqua ... producer (produced by)(p.g.a.) Andy Mitchell ... executive producer  Samir M. Patel ... executive producer (as Samir Patel) Guja Quaranta ... line producer  Kat Samick ... executive producer  Alex Siskin ... producer (produced by) Enzo Sisti ... executive producer  Michael Sloan ... producer (produced by) Steve Tisch ... producer (produced by) Clayton Townsend ... producer (produced by)(p.g.a.) Denzel Washington ... producer (produced by) Richard Wenk ... co-producer </t>
   </si>
   <si>
-    <t>Michael Chaves</t>
-  </si>
-  <si>
     <t>New Line Cinema(presents)Atomic MonsterThe Safran Company</t>
   </si>
   <si>
     <t xml:space="preserve"> John Bernard ... line producer  Richard Brener ... executive producer  Michael Clear ... executive producer  Gary Dauberman ... executive producer  Tricia Miles ... associate producer (as Tricia Miles Tharp) Dave Neustadter ... executive producer  Victoria Palmeri ... executive producer  Michael Polaire ... executive producer  Peter Safran ... producer (produced by)(p.g.a.) Judson Scott ... executive producer  James Wan ... producer (produced by)(p.g.a.)</t>
   </si>
   <si>
-    <t>Kenneth Branagh</t>
+    <t>Nickelodeon Animation StudiosNickelodeon MoviesParamount AnimationParamount PicturesSpin Master Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bob Barlen ... associate producer  Adam Beder ... executive producer  Laura Clunie ... producer (produced by)(p.g.a.) Andre Coutu ... post producer  Jennifer Dodge ... producer (produced by)(p.g.a.) Pierre Escande ... executive producer: Mikros Animation  Ronnen Harary ... executive producer  Julie Marouzé ... line producer: Mikros Animation  Peter Schlessel ... executive producer  Toni Stevens ... producer (produced by)(p.g.a.) Laurence Vacher ... executive producer: Mikros Animation </t>
+  </si>
+  <si>
+    <t>Aldea M EstudiosCorazón FilmsLionsgate ProductionsLionsgateTwisted Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mark Burg ... producer  Jason Constantine ... executive producer  Daniel J. Heffner ... executive producer (as Daniel Jason Heffner) Gregg Hoffman ... executive producer  Ketura Kestin ... executive producer  Oren Koules ... producer  Ulrich Maier ... producer: mexico  Mindy Sheldon ... co-producer  Stacey Testro ... executive producer  James Wan ... executive producer  Leigh Whannell ... executive producer </t>
+  </si>
+  <si>
+    <t>20th Century StudiosNew Regency ProductionsEntertainment One</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Courtney Cunniff ... co-producer (as Courtney L. Cunniff) Gareth Edwards ... producer (p.g.a.) Zev Foreman ... executive producer  Greig Fraser ... co-producer  Kiri Hart ... producer  Natalie Lehmann ... executive producer  Nick Meyer ... executive producer  Arnon Milchan ... producer  Yariv Milchan ... executive producer  Galileo Mondol ... producer: Los Angeles unit  Chidchanok Plodripu ... line producer: Thailand (as Chidchanok 'Pam' Plodripu) Ace Salvador ... producer: Los Angeles unit  Michael Schaefer ... executive producer  Nicholas Simon ... co-producer  Jim Spencer ... producer (p.g.a.)</t>
+  </si>
+  <si>
+    <t>Campbell Grobman FilmsMedia Capital Technologies(in association with)Millennium FilmsNu Boyana Film Studios(production facilities)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vessela Banzourkova ... line producer  Christa Campbell ... executive producer  Guymon Casady ... executive producer  Spenser Cohen ... executive producer  Michael S. Constable ... executive producer  Jason Constantine ... executive producer  Allen Dam ... executive producer  Boaz Davidson ... executive producer  Jon Feltheimer ... executive producer  Claiton Fernandes ... co-executive producer  Vladimir Fernandes ... co-executive producer  Jeffrey Greenstein ... executive producer  Lati Grobman ... executive producer  Victor Hadida ... co-executive producer  Anna Halberg ... executive producer  Basil Iwanyk ... executive producer  K. Blaine Johnston ... executive producer  Eda Kowan ... executive producer  Avi Lerner ... executive producer  Yariv Lerner ... producer  Gisella Marengo ... co-producer  Balan Melarkode ... co-executive producer  Abby Mills ... co-producer  Euzebio Munhoz Jr.... co-executive producer  Matthew O'Toole ... co-producer  Stephen Paul ... executive producer  Lonnie Ramati ... co-executive producer  Trevor Short ... executive producer  Jason Statham ... producer  Kevin King Templeton ... producer  Robert Van Norden ... executive producer  Les Weldon ... producer  Gareth West ... executive producer  Christopher Woodrow ... executive producer  Jonathan Yunger ... executive producer </t>
+  </si>
+  <si>
+    <t>Black Bear PicturesColumbia PicturesRyder Picture CompanySony Pictures Entertainment (SPE)Stage 6 Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rebecca Angelo ... executive producer  Lauren Schuker Blum ... executive producer  Loren Brock ... line producer: LA unit  Christopher Casanova ... co-producer  John Friedberg ... executive producer  Craig Gillespie ... producer  Michael Heimler ... executive producer  Johnny Holland ... executive producer  Ben Mezrich ... executive producer  Johnny Pariseau ... co-producer  Aaron Ryder ... producer (produced by)(p.g.a.) Teddy Schwarzman ... producer  Claire Severance ... associate producer  Andrew Swett ... executive producer  Kevin Ulrich ... executive producer  Cameron Winklevoss ... executive producer  Tyler Winklevoss ... executive producer </t>
+  </si>
+  <si>
+    <t>GND Media GroupStacey Films(in association with)Tread Lively</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dan Campbell ... associate producer  Zach Dasher ... producer  Troy Duhon ... executive producer  Bob Katz ... executive producer  Robert Katz ... producer  Jason Melton ... executive producer  Shelley D. Needham ... line producer  Cole Prine ... producer  Korie Robertson ... producer  Willie Robertson ... executive producer  Jeremy John Wells ... executive producer  Brittany Yost ... producer </t>
+  </si>
+  <si>
+    <t>Brightlight PicturesNeonQC Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arielle Boisvert ... executive producer  Jeff Deutchman ... executive producer  Ryan Friscia ... executive producer  Edward H. Hamm Jr.... executive producer  Raymond Mansfield ... producer  Sean McKittrick ... producer  Jameson Parker ... executive producer  Tom Quinn ... executive producer  Emily Thomas ... executive producer  Shawn Williamson ... executive producer </t>
+  </si>
+  <si>
+    <t>Talking HeadsArnold Stiefel Company(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gary Goetzman ... producer  Gary Kurfirst ... executive producer </t>
+  </si>
+  <si>
+    <t>Matthew Crouch</t>
+  </si>
+  <si>
+    <t>No studios found</t>
+  </si>
+  <si>
+    <t>No producers found</t>
+  </si>
+  <si>
+    <t>Wuershan</t>
+  </si>
+  <si>
+    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
+  </si>
+  <si>
+    <t>Sean Olson</t>
+  </si>
+  <si>
+    <t>Called Higher Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
+  </si>
+  <si>
+    <t>Miles Joris-Peyrafitte</t>
+  </si>
+  <si>
+    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
+  </si>
+  <si>
+    <t>Aitch Alberto</t>
+  </si>
+  <si>
+    <t>Boies Schiller Entertainment3Pas Studios5000 Broadway ProductionsBig Swing ProductionsLimelight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aitch Alberto ... executive producer  Meredith Bagby ... executive producer  David Boies ... executive producer  Eugenio Derbez ... producer  Nicole Flores ... line producer  Lin-Manuel Miranda ... producer  Ben Odell ... producer  Owen Panettieri ... co-producer  Chris Parker ... producer  Zack Schiller ... executive producer  Kyra Sedgwick ... producer  Dylan Sellers ... producer  Valerie Stadler ... producer </t>
+  </si>
+  <si>
+    <t>Rudy Valdez</t>
+  </si>
+  <si>
+    <t>Imagine DocumentariesSony Music Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Santana </t>
+  </si>
+  <si>
+    <t>Michael A. Goorjian</t>
+  </si>
+  <si>
+    <t>People of ArPalodeon Pictures(In Association With)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
+  </si>
+  <si>
+    <t>Michael Jai White</t>
+  </si>
+  <si>
+    <t>Jaigantic Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
+  </si>
+  <si>
+    <t>Jim CapobiancoPierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
+  </si>
+  <si>
+    <t>Tyler Sansom</t>
+  </si>
+  <si>
+    <t>First Capital FilmsKappa Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
+  </si>
+  <si>
+    <t>Nicol Paone</t>
+  </si>
+  <si>
+    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
+  </si>
+  <si>
+    <t>Peter FacinelliNick Lyon</t>
+  </si>
+  <si>
+    <t>Lone Star StorytellersMedia GroupSC Films International</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
+  </si>
+  <si>
+    <t>Peter Lepeniotis</t>
+  </si>
+  <si>
+    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
+  </si>
+  <si>
+    <t>Kaige Chen</t>
+  </si>
+  <si>
+    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
+  </si>
+  <si>
+    <t>Sébastien Marnier</t>
+  </si>
+  <si>
+    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
+  </si>
+  <si>
+    <t>Bethann HardisonFrédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
+  </si>
+  <si>
+    <t>Klaus Härö</t>
+  </si>
+  <si>
+    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
+  </si>
+  <si>
+    <t>Stephen Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Upstream Pictures (II)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
+  </si>
+  <si>
+    <t>Danny O'MalleyAlex Rivest</t>
+  </si>
+  <si>
+    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
+  </si>
+  <si>
+    <t>Joshua TickellRebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Big Picture RanchBenenson Productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
+  </si>
+  <si>
+    <t>Richard Dewey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
+  </si>
+  <si>
+    <t>Aristotle Torres</t>
+  </si>
+  <si>
+    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
+  </si>
+  <si>
+    <t>Adil El ArbiBilall Fallah</t>
+  </si>
+  <si>
+    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
+  </si>
+  <si>
+    <t>Luca Balser</t>
+  </si>
+  <si>
+    <t>Gummy Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
+  </si>
+  <si>
+    <t>Hiroshi Akabane</t>
+  </si>
+  <si>
+    <t>HS ProductionsIRH Press Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
+  </si>
+  <si>
+    <t>John Stalberg Jr.</t>
+  </si>
+  <si>
+    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
+  </si>
+  <si>
+    <t>Jude Okwudiafor Johnson</t>
+  </si>
+  <si>
+    <t>Anchor Media Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
+  </si>
+  <si>
+    <t>Cru EnnisLee Roy Kunz</t>
+  </si>
+  <si>
+    <t>World's Fair Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
+  </si>
+  <si>
+    <t>Andrea Di Stefano</t>
+  </si>
+  <si>
+    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
+  </si>
+  <si>
+    <t>Miguel Ángel Vivas</t>
+  </si>
+  <si>
+    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
+  </si>
+  <si>
+    <t>Frank Cimière</t>
+  </si>
+  <si>
+    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marc Missonnier ... producer </t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,837,275
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">167,037,275
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,059,802
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">248,659,802
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,866,988
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87,066,988
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,653,726
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102,653,726
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,554,793
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43,854,793
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,517,765
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,318,793
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,929,037
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61,829,037
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,366,200
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,094,529
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,635,065
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,048,963
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,486,997
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,486,997
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,600,194
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,482,662
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,000,378
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,388,017
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222,410
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222,410
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,811
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,811
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70,125
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171,840
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,919
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">756,934
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,215
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,215
+</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2783019777/?ref_=bo_md_table_8</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2106360577/?ref_=bo_md_table_9</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3568206593/?ref_=bo_md_table_36</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3719136001/?ref_=bo_md_table_37</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1722778369/?ref_=bo_md_table_38</t>
   </si>
   <si>
     <t>20th Century StudiosKinberg GenreScott Free ProductionsTSG EntertainmentThe Mark Gordon Company</t>
@@ -546,536 +1027,16 @@
     <t xml:space="preserve"> Enrico Ballarin ... line producer: Venice  Kenneth Branagh ... producer (p.g.a.) Martin Curry ... associate producer  Mark Gordon ... executive producer  Judy Hofflund ... producer (p.g.a.) Louise Killin ... executive producer  Simon Kinberg ... producer  James Prichard ... executive producer  Ridley Scott ... producer </t>
   </si>
   <si>
-    <t>Cal Brunker</t>
-  </si>
-  <si>
-    <t>Nickelodeon Animation StudiosNickelodeon MoviesParamount AnimationParamount PicturesSpin Master Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bob Barlen ... associate producer  Adam Beder ... executive producer  Laura Clunie ... producer (produced by)(p.g.a.) Andre Coutu ... post producer  Jennifer Dodge ... producer (produced by)(p.g.a.) Pierre Escande ... executive producer: Mikros Animation  Ronnen Harary ... executive producer  Julie Marouzé ... line producer: Mikros Animation  Peter Schlessel ... executive producer  Toni Stevens ... producer (produced by)(p.g.a.) Laurence Vacher ... executive producer: Mikros Animation </t>
-  </si>
-  <si>
-    <t>Nia Vardalos</t>
-  </si>
-  <si>
     <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)Playtone</t>
   </si>
   <si>
     <t xml:space="preserve"> Paul Brooks ... executive producer  Michael P. Flannigan ... executive producer  Gary Goetzman ... producer  Tom Hanks ... producer  Scott Niemeyer ... executive producer  Eric Quijano ... associate producer  Kostas Raftopoulos ... line producer: Greece  Steve Shareshian ... executive producer  Julie Shimer ... associate producer (as Julie Shimer Lawrence) Jonathan Shore ... co-producer  Nia Vardalos ... executive producer  Rita Wilson ... producer (produced by)(p.g.a)</t>
   </si>
   <si>
-    <t>Kevin Greutert</t>
-  </si>
-  <si>
-    <t>Aldea M EstudiosCorazón FilmsLionsgate ProductionsLionsgateTwisted Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mark Burg ... producer  Jason Constantine ... executive producer  Daniel J. Heffner ... executive producer (as Daniel Jason Heffner) Gregg Hoffman ... executive producer  Ketura Kestin ... executive producer  Oren Koules ... producer  Ulrich Maier ... producer: mexico  Mindy Sheldon ... co-producer  Stacey Testro ... executive producer  James Wan ... executive producer  Leigh Whannell ... executive producer </t>
-  </si>
-  <si>
-    <t>Gareth Edwards</t>
-  </si>
-  <si>
-    <t>20th Century StudiosNew Regency ProductionsEntertainment One</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Courtney Cunniff ... co-producer (as Courtney L. Cunniff) Gareth Edwards ... producer (p.g.a.) Zev Foreman ... executive producer  Greig Fraser ... co-producer  Kiri Hart ... producer  Natalie Lehmann ... executive producer  Nick Meyer ... executive producer  Arnon Milchan ... producer  Yariv Milchan ... executive producer  Galileo Mondol ... producer: Los Angeles unit  Chidchanok Plodripu ... line producer: Thailand (as Chidchanok 'Pam' Plodripu) Ace Salvador ... producer: Los Angeles unit  Michael Schaefer ... executive producer  Nicholas Simon ... co-producer  Jim Spencer ... producer (p.g.a.)</t>
-  </si>
-  <si>
-    <t>Atlee</t>
-  </si>
-  <si>
     <t>Red Chillies Entertainment</t>
   </si>
   <si>
     <t xml:space="preserve"> Gauri Khan ... producer  Gaurav Verma ... co-producer </t>
-  </si>
-  <si>
-    <t>Scott Waugh</t>
-  </si>
-  <si>
-    <t>Campbell Grobman FilmsMedia Capital Technologies(in association with)Millennium FilmsNu Boyana Film Studios(production facilities)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vessela Banzourkova ... line producer  Christa Campbell ... executive producer  Guymon Casady ... executive producer  Spenser Cohen ... executive producer  Michael S. Constable ... executive producer  Jason Constantine ... executive producer  Allen Dam ... executive producer  Boaz Davidson ... executive producer  Jon Feltheimer ... executive producer  Claiton Fernandes ... co-executive producer  Vladimir Fernandes ... co-executive producer  Jeffrey Greenstein ... executive producer  Lati Grobman ... executive producer  Victor Hadida ... co-executive producer  Anna Halberg ... executive producer  Basil Iwanyk ... executive producer  K. Blaine Johnston ... executive producer  Eda Kowan ... executive producer  Avi Lerner ... executive producer  Yariv Lerner ... producer  Gisella Marengo ... co-producer  Balan Melarkode ... co-executive producer  Abby Mills ... co-producer  Euzebio Munhoz Jr.... co-executive producer  Matthew O'Toole ... co-producer  Stephen Paul ... executive producer  Lonnie Ramati ... co-executive producer  Trevor Short ... executive producer  Jason Statham ... producer  Kevin King Templeton ... producer  Robert Van Norden ... executive producer  Les Weldon ... producer  Gareth West ... executive producer  Christopher Woodrow ... executive producer  Jonathan Yunger ... executive producer </t>
-  </si>
-  <si>
-    <t>Craig Gillespie</t>
-  </si>
-  <si>
-    <t>Black Bear PicturesColumbia PicturesRyder Picture CompanySony Pictures Entertainment (SPE)Stage 6 Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rebecca Angelo ... executive producer  Lauren Schuker Blum ... executive producer  Loren Brock ... line producer: LA unit  Christopher Casanova ... co-producer  John Friedberg ... executive producer  Craig Gillespie ... producer  Michael Heimler ... executive producer  Johnny Holland ... executive producer  Ben Mezrich ... executive producer  Johnny Pariseau ... co-producer  Aaron Ryder ... producer (produced by)(p.g.a.) Teddy Schwarzman ... producer  Claire Severance ... associate producer  Andrew Swett ... executive producer  Kevin Ulrich ... executive producer  Cameron Winklevoss ... executive producer  Tyler Winklevoss ... executive producer </t>
-  </si>
-  <si>
-    <t>Andrew Hyatt</t>
-  </si>
-  <si>
-    <t>GND Media GroupStacey Films(in association with)Tread Lively</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dan Campbell ... associate producer  Zach Dasher ... producer  Troy Duhon ... executive producer  Bob Katz ... executive producer  Robert Katz ... producer  Jason Melton ... executive producer  Shelley D. Needham ... line producer  Cole Prine ... producer  Korie Robertson ... producer  Willie Robertson ... executive producer  Jeremy John Wells ... executive producer  Brittany Yost ... producer </t>
-  </si>
-  <si>
-    <t>Bishal Dutta</t>
-  </si>
-  <si>
-    <t>Brightlight PicturesNeonQC Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Arielle Boisvert ... executive producer  Jeff Deutchman ... executive producer  Ryan Friscia ... executive producer  Edward H. Hamm Jr.... executive producer  Raymond Mansfield ... producer  Sean McKittrick ... producer  Jameson Parker ... executive producer  Tom Quinn ... executive producer  Emily Thomas ... executive producer  Shawn Williamson ... executive producer </t>
-  </si>
-  <si>
-    <t>Jonathan Demme</t>
-  </si>
-  <si>
-    <t>Talking HeadsArnold Stiefel Company(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gary Goetzman ... producer  Gary Kurfirst ... executive producer </t>
-  </si>
-  <si>
-    <t>Matthew Crouch</t>
-  </si>
-  <si>
-    <t>No studios found</t>
-  </si>
-  <si>
-    <t>No producers found</t>
-  </si>
-  <si>
-    <t>Wuershan</t>
-  </si>
-  <si>
-    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
-  </si>
-  <si>
-    <t>Sean Olson</t>
-  </si>
-  <si>
-    <t>Called Higher Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
-  </si>
-  <si>
-    <t>Miles Joris-Peyrafitte</t>
-  </si>
-  <si>
-    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
-  </si>
-  <si>
-    <t>Aitch Alberto</t>
-  </si>
-  <si>
-    <t>Boies Schiller Entertainment3Pas Studios5000 Broadway ProductionsBig Swing ProductionsLimelight</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aitch Alberto ... executive producer  Meredith Bagby ... executive producer  David Boies ... executive producer  Eugenio Derbez ... producer  Nicole Flores ... line producer  Lin-Manuel Miranda ... producer  Ben Odell ... producer  Owen Panettieri ... co-producer  Chris Parker ... producer  Zack Schiller ... executive producer  Kyra Sedgwick ... producer  Dylan Sellers ... producer  Valerie Stadler ... producer </t>
-  </si>
-  <si>
-    <t>Rudy Valdez</t>
-  </si>
-  <si>
-    <t>Imagine DocumentariesSony Music Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carlos Santana </t>
-  </si>
-  <si>
-    <t>Michael A. Goorjian</t>
-  </si>
-  <si>
-    <t>People of ArPalodeon Pictures(In Association With)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
-  </si>
-  <si>
-    <t>Michael Jai White</t>
-  </si>
-  <si>
-    <t>Jaigantic Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
-  </si>
-  <si>
-    <t>Jim CapobiancoPierre-Luc Granjon</t>
-  </si>
-  <si>
-    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
-  </si>
-  <si>
-    <t>Tyler Sansom</t>
-  </si>
-  <si>
-    <t>First Capital FilmsKappa Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
-  </si>
-  <si>
-    <t>Nicol Paone</t>
-  </si>
-  <si>
-    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
-  </si>
-  <si>
-    <t>Peter FacinelliNick Lyon</t>
-  </si>
-  <si>
-    <t>Lone Star StorytellersMedia GroupSC Films International</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
-  </si>
-  <si>
-    <t>Peter Lepeniotis</t>
-  </si>
-  <si>
-    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
-  </si>
-  <si>
-    <t>Kaige Chen</t>
-  </si>
-  <si>
-    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
-  </si>
-  <si>
-    <t>Sébastien Marnier</t>
-  </si>
-  <si>
-    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
-  </si>
-  <si>
-    <t>Bethann HardisonFrédéric Tcheng</t>
-  </si>
-  <si>
-    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
-  </si>
-  <si>
-    <t>Klaus Härö</t>
-  </si>
-  <si>
-    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
-  </si>
-  <si>
-    <t>Stephen Gyllenhaal</t>
-  </si>
-  <si>
-    <t>Upstream Pictures (II)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
-  </si>
-  <si>
-    <t>Danny O'MalleyAlex Rivest</t>
-  </si>
-  <si>
-    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
-  </si>
-  <si>
-    <t>Joshua TickellRebecca Harrell Tickell</t>
-  </si>
-  <si>
-    <t>Big Picture RanchBenenson Productions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
-  </si>
-  <si>
-    <t>Richard Dewey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
-  </si>
-  <si>
-    <t>Aristotle Torres</t>
-  </si>
-  <si>
-    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
-  </si>
-  <si>
-    <t>Adil El ArbiBilall Fallah</t>
-  </si>
-  <si>
-    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
-  </si>
-  <si>
-    <t>Luca Balser</t>
-  </si>
-  <si>
-    <t>Gummy Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
-  </si>
-  <si>
-    <t>Hiroshi Akabane</t>
-  </si>
-  <si>
-    <t>HS ProductionsIRH Press Co.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
-  </si>
-  <si>
-    <t>John Stalberg Jr.</t>
-  </si>
-  <si>
-    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
-  </si>
-  <si>
-    <t>Jude Okwudiafor Johnson</t>
-  </si>
-  <si>
-    <t>Anchor Media Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
-  </si>
-  <si>
-    <t>Cru EnnisLee Roy Kunz</t>
-  </si>
-  <si>
-    <t>World's Fair Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
-  </si>
-  <si>
-    <t>Andrea Di Stefano</t>
-  </si>
-  <si>
-    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
-  </si>
-  <si>
-    <t>Miguel Ángel Vivas</t>
-  </si>
-  <si>
-    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
-  </si>
-  <si>
-    <t>Frank Cimière</t>
-  </si>
-  <si>
-    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marc Missonnier ... producer </t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,837,275
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">167,037,275
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81,059,802
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">248,659,802
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38,866,988
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87,066,988
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35,653,726
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102,653,726
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,554,793
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43,854,793
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,517,765
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36,318,793
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,929,037
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61,829,037
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,366,200
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,094,529
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,635,065
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,048,963
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,486,997
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,486,997
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,600,194
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,482,662
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,000,378
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,388,017
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222,410
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222,410
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,811
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,811
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70,125
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">171,840
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,919
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">756,934
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,215
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,215
-</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1171,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1572,22 +1529,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="G2" t="s">
-        <v>142</v>
+        <v>260</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1601,22 +1555,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="G3" t="s">
-        <v>145</v>
+        <v>262</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1624,28 +1575,25 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G4" t="s">
-        <v>148</v>
+        <v>264</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1653,28 +1601,25 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="G5" t="s">
-        <v>151</v>
+        <v>266</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>153</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1682,28 +1627,25 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="G6" t="s">
-        <v>154</v>
+        <v>268</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1711,28 +1653,25 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G7" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>158</v>
+        <v>300</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>159</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1746,834 +1685,813 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="G8" t="s">
-        <v>160</v>
+        <v>272</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>293</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>273</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" t="s">
-        <v>163</v>
+        <v>274</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>294</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>297</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="G10" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>167</v>
+        <v>302</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>168</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G11" t="s">
-        <v>169</v>
+        <v>276</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G12" t="s">
-        <v>172</v>
+        <v>278</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="G13" t="s">
-        <v>175</v>
+        <v>280</v>
       </c>
       <c r="H13" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="G14" t="s">
-        <v>178</v>
+        <v>282</v>
       </c>
       <c r="H14" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="H16" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="H18" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G19" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="H21" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="H22" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G23" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="H23" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="G24" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G25" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="H25" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G26" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G27" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="H27" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="G29" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="H29" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G30" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G31" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="H31" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="G32" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="H32" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G33" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="H33" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G34" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="H34" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G35" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="H35" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G36" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H36" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -2581,260 +2499,260 @@
         <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>295</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>128</v>
+        <v>289</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>129</v>
+        <v>290</v>
       </c>
       <c r="G37" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="H37" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>296</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G38" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>297</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>313</v>
+        <v>125</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>314</v>
+        <v>126</v>
       </c>
       <c r="G39" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="H39" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G40" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="H40" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="E41" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="G41" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="H41" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E42" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G42" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="H42" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G43" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="H43" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G44" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="H44" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G45" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="H45" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="I45" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
transfer all into gross iteration
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Group8-300-762-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C0CD86-0C7A-4A0E-9003-7442918CD1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277884-1C33-4AF8-983E-960B8A651E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="226">
   <si>
     <t>Film Title</t>
   </si>
@@ -327,9 +327,6 @@
     <t>https://www.boxofficemojo.com/release/rl1303282433/?ref_=bo_md_table_44</t>
   </si>
   <si>
-    <t>No directors found</t>
-  </si>
-  <si>
     <t>No producers found</t>
   </si>
   <si>
@@ -709,14 +706,22 @@
   </si>
   <si>
     <t xml:space="preserve"> Marc Missonnier ... producer </t>
+  </si>
+  <si>
+    <t>Antoine Fuqua</t>
+  </si>
+  <si>
+    <t>Columbia Pictures(presents)Eagle Pictures(in association with)Escape ArtistsZHIV ProductionsSony Pictures Entertainment (SPE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tarak Ben Ammar ... executive producer  Todd Black ... producer (produced by)(p.g.a.) David Bloomfield ... executive producer  Jason Blumenthal ... producer (produced by)(p.g.a.) Vito Colazzo ... line producer  Tony Eldridge ... producer (produced by) Antoine Fuqua ... producer (produced by)(p.g.a.) Andy Mitchell ... executive producer  Samir M. Patel ... executive producer (as Samir Patel) Guja Quaranta ... line producer  Kat Samick ... executive producer  Alex Siskin ... producer (produced by) Enzo Sisti ... executive producer  Michael Sloan ... producer (produced by) Steve Tisch ... producer (produced by) Clayton Townsend ... producer (produced by)(p.g.a.) Denzel Washington ... producer (produced by) Richard Wenk ... co-producer </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -826,7 +831,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,16 +1152,16 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1199,14 +1204,16 @@
         <v>167605171</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1223,16 +1230,16 @@
         <v>249149159</v>
       </c>
       <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1249,16 +1256,16 @@
         <v>88950223</v>
       </c>
       <c r="F4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="403.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1275,16 +1282,16 @@
         <v>103116671</v>
       </c>
       <c r="F5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1301,16 +1308,16 @@
         <v>56984243</v>
       </c>
       <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1327,16 +1334,16 @@
         <v>36428526</v>
       </c>
       <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1353,16 +1360,16 @@
         <v>62992122</v>
       </c>
       <c r="F8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1379,16 +1386,16 @@
         <v>27461442</v>
       </c>
       <c r="F9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1405,16 +1412,16 @@
         <v>27514156</v>
       </c>
       <c r="F10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1431,16 +1438,16 @@
         <v>10983467</v>
       </c>
       <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1457,16 +1464,16 @@
         <v>12365832</v>
       </c>
       <c r="F12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1483,16 +1490,16 @@
         <v>5482605</v>
       </c>
       <c r="F13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" t="s">
         <v>128</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1509,16 +1516,16 @@
         <v>4388017</v>
       </c>
       <c r="F14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" t="s">
         <v>131</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1535,14 +1542,14 @@
         <v>1606339</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1559,16 +1566,16 @@
         <v>1973543</v>
       </c>
       <c r="F16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" t="s">
         <v>135</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="288" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" ht="345" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1585,16 +1592,16 @@
         <v>1108247</v>
       </c>
       <c r="F17" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1611,16 +1618,16 @@
         <v>503378</v>
       </c>
       <c r="F18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" t="s">
         <v>141</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1637,16 +1644,16 @@
         <v>423024</v>
       </c>
       <c r="F19" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1663,16 +1670,16 @@
         <v>407838</v>
       </c>
       <c r="F20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" t="s">
         <v>147</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="331.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1689,16 +1696,16 @@
         <v>376719</v>
       </c>
       <c r="F21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" t="s">
         <v>150</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1715,16 +1722,16 @@
         <v>319848</v>
       </c>
       <c r="F22" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" t="s">
         <v>153</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1741,16 +1748,16 @@
         <v>306385</v>
       </c>
       <c r="F23" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" t="s">
         <v>156</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1767,16 +1774,16 @@
         <v>224585</v>
       </c>
       <c r="F24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1793,16 +1800,16 @@
         <v>168926</v>
       </c>
       <c r="F25" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" t="s">
         <v>162</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1819,16 +1826,16 @@
         <v>617143</v>
       </c>
       <c r="F26" t="s">
+        <v>164</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1845,16 +1852,16 @@
         <v>205118</v>
       </c>
       <c r="F27" t="s">
+        <v>167</v>
+      </c>
+      <c r="G27" t="s">
         <v>168</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1871,16 +1878,16 @@
         <v>130802</v>
       </c>
       <c r="F28" t="s">
+        <v>170</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1897,16 +1904,16 @@
         <v>88910</v>
       </c>
       <c r="F29" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" t="s">
         <v>174</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1923,16 +1930,16 @@
         <v>1120899</v>
       </c>
       <c r="F30" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1949,16 +1956,16 @@
         <v>81599</v>
       </c>
       <c r="F31" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" t="s">
         <v>180</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1975,16 +1982,16 @@
         <v>171463</v>
       </c>
       <c r="F32" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" t="s">
         <v>183</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2001,16 +2008,16 @@
         <v>38683</v>
       </c>
       <c r="F33" t="s">
+        <v>185</v>
+      </c>
+      <c r="G33" t="s">
         <v>186</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2027,16 +2034,16 @@
         <v>35563</v>
       </c>
       <c r="F34" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" t="s">
         <v>189</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -2053,13 +2060,13 @@
         <v>32535</v>
       </c>
       <c r="F35" t="s">
+        <v>191</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2076,16 +2083,16 @@
         <v>25570</v>
       </c>
       <c r="F36" t="s">
+        <v>193</v>
+      </c>
+      <c r="G36" t="s">
         <v>194</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -2102,16 +2109,16 @@
         <v>757434</v>
       </c>
       <c r="F37" t="s">
+        <v>196</v>
+      </c>
+      <c r="G37" t="s">
         <v>197</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -2128,16 +2135,16 @@
         <v>13273</v>
       </c>
       <c r="F38" t="s">
+        <v>199</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2154,16 +2161,16 @@
         <v>173121</v>
       </c>
       <c r="F39" t="s">
+        <v>202</v>
+      </c>
+      <c r="G39" t="s">
         <v>203</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2180,16 +2187,16 @@
         <v>7807</v>
       </c>
       <c r="F40" t="s">
+        <v>205</v>
+      </c>
+      <c r="G40" t="s">
         <v>206</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -2206,16 +2213,16 @@
         <v>5300</v>
       </c>
       <c r="F41" t="s">
+        <v>208</v>
+      </c>
+      <c r="G41" t="s">
         <v>209</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -2232,16 +2239,16 @@
         <v>4883</v>
       </c>
       <c r="F42" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" t="s">
         <v>212</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2258,16 +2265,16 @@
         <v>4580566</v>
       </c>
       <c r="F43" t="s">
+        <v>214</v>
+      </c>
+      <c r="G43" t="s">
         <v>215</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -2284,16 +2291,16 @@
         <v>147849</v>
       </c>
       <c r="F44" t="s">
+        <v>217</v>
+      </c>
+      <c r="G44" t="s">
         <v>218</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2310,13 +2317,13 @@
         <v>371989</v>
       </c>
       <c r="F45" t="s">
+        <v>220</v>
+      </c>
+      <c r="G45" t="s">
         <v>221</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>222</v>
-      </c>
-      <c r="H45" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2332,16 +2339,16 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
output of whole solution running
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FC91F7-3873-4A8E-B7E8-AE8A3C300DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCE4C75-241B-42CC-8BF7-BF1F345CE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
-    <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
-    <sheet name="Director's Highest gross Films" sheetId="1" r:id="rId2"/>
+    <sheet name="Directors" sheetId="3" r:id="rId1"/>
+    <sheet name="MovieInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Director's Highest gross Films" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="359">
   <si>
     <t>Film Title</t>
   </si>
@@ -105,15 +106,9 @@
     <t>Dumb Money</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3028583169/?ref_=bo_md_table_10</t>
-  </si>
-  <si>
     <t>The Blind</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl2123662081/?ref_=bo_md_table_11</t>
-  </si>
-  <si>
     <t>It Lives Inside</t>
   </si>
   <si>
@@ -153,15 +148,9 @@
     <t>Aristotle and Dante Discover the Secrets of the Universe</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl984056577/?ref_=bo_md_table_18</t>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3584983809/?ref_=bo_md_table_19</t>
-  </si>
-  <si>
     <t>Amerikatsi</t>
   </si>
   <si>
@@ -189,27 +178,15 @@
     <t>The Kill Room</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_24</t>
-  </si>
-  <si>
     <t>On Fire</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl464618241/?ref_=bo_md_table_25</t>
-  </si>
-  <si>
     <t>Zombie Town</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3182002945/?ref_=bo_md_table_26</t>
-  </si>
-  <si>
     <t>Farewell My Concubine</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_27</t>
-  </si>
-  <si>
     <t>The Origin of Evil</t>
   </si>
   <si>
@@ -304,22 +281,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1,422,011
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,792,566
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,105,059
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,105,059
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">503,378
 </t>
   </si>
@@ -336,22 +297,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">402,275
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">415,986
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">359,516
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">359,516
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">319,848
 </t>
   </si>
@@ -392,14 +337,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">124,936
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">124,936
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">87,344
 </t>
   </si>
@@ -408,14 +345,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">77,265
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77,265
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">38,683
 </t>
   </si>
@@ -432,22 +361,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">30,507
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,507
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,058
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,058
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">10,500
 </t>
   </si>
@@ -456,14 +369,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">9,289
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9,289
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">7,807
 </t>
   </si>
@@ -522,9 +427,6 @@
     <t xml:space="preserve"> Bob Barlen ... associate producer  Adam Beder ... executive producer  Laura Clunie ... producer (produced by)(p.g.a.) Andre Coutu ... post producer  Jennifer Dodge ... producer (produced by)(p.g.a.) Pierre Escande ... executive producer: Mikros Animation  Ronnen Harary ... executive producer  Julie Marouzé ... line producer: Mikros Animation  Peter Schlessel ... executive producer  Toni Stevens ... producer (produced by)(p.g.a.) Laurence Vacher ... executive producer: Mikros Animation </t>
   </si>
   <si>
-    <t>Aldea M EstudiosCorazón FilmsLionsgate ProductionsLionsgateTwisted Pictures</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Mark Burg ... producer  Jason Constantine ... executive producer  Daniel J. Heffner ... executive producer (as Daniel Jason Heffner) Gregg Hoffman ... executive producer  Ketura Kestin ... executive producer  Oren Koules ... producer  Ulrich Maier ... producer: mexico  Mindy Sheldon ... co-producer  Stacey Testro ... executive producer  James Wan ... executive producer  Leigh Whannell ... executive producer </t>
   </si>
   <si>
@@ -540,64 +442,542 @@
     <t xml:space="preserve"> Vessela Banzourkova ... line producer  Christa Campbell ... executive producer  Guymon Casady ... executive producer  Spenser Cohen ... executive producer  Michael S. Constable ... executive producer  Jason Constantine ... executive producer  Allen Dam ... executive producer  Boaz Davidson ... executive producer  Jon Feltheimer ... executive producer  Claiton Fernandes ... co-executive producer  Vladimir Fernandes ... co-executive producer  Jeffrey Greenstein ... executive producer  Lati Grobman ... executive producer  Victor Hadida ... co-executive producer  Anna Halberg ... executive producer  Basil Iwanyk ... executive producer  K. Blaine Johnston ... executive producer  Eda Kowan ... executive producer  Avi Lerner ... executive producer  Yariv Lerner ... producer  Gisella Marengo ... co-producer  Balan Melarkode ... co-executive producer  Abby Mills ... co-producer  Euzebio Munhoz Jr.... co-executive producer  Matthew O'Toole ... co-producer  Stephen Paul ... executive producer  Lonnie Ramati ... co-executive producer  Trevor Short ... executive producer  Jason Statham ... producer  Kevin King Templeton ... producer  Robert Van Norden ... executive producer  Les Weldon ... producer  Gareth West ... executive producer  Christopher Woodrow ... executive producer  Jonathan Yunger ... executive producer </t>
   </si>
   <si>
+    <t>GND Media GroupStacey Films(in association with)Tread Lively</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dan Campbell ... associate producer  Zach Dasher ... producer  Troy Duhon ... executive producer  Bob Katz ... executive producer  Robert Katz ... producer  Jason Melton ... executive producer  Shelley D. Needham ... line producer  Cole Prine ... producer  Korie Robertson ... producer  Willie Robertson ... executive producer  Jeremy John Wells ... executive producer  Brittany Yost ... producer </t>
+  </si>
+  <si>
+    <t>Brightlight PicturesNeonQC Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arielle Boisvert ... executive producer  Jeff Deutchman ... executive producer  Ryan Friscia ... executive producer  Edward H. Hamm Jr.... executive producer  Raymond Mansfield ... producer  Sean McKittrick ... producer  Jameson Parker ... executive producer  Tom Quinn ... executive producer  Emily Thomas ... executive producer  Shawn Williamson ... executive producer </t>
+  </si>
+  <si>
+    <t>Talking HeadsArnold Stiefel Company(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gary Goetzman ... producer  Gary Kurfirst ... executive producer </t>
+  </si>
+  <si>
+    <t>Matthew Crouch</t>
+  </si>
+  <si>
+    <t>No studios found</t>
+  </si>
+  <si>
+    <t>No producers found</t>
+  </si>
+  <si>
+    <t>Wuershan</t>
+  </si>
+  <si>
+    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
+  </si>
+  <si>
+    <t>Sean Olson</t>
+  </si>
+  <si>
+    <t>Called Higher Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
+  </si>
+  <si>
+    <t>Miles Joris-Peyrafitte</t>
+  </si>
+  <si>
+    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
+  </si>
+  <si>
+    <t>Rudy Valdez</t>
+  </si>
+  <si>
+    <t>Imagine DocumentariesSony Music Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Santana </t>
+  </si>
+  <si>
+    <t>Michael A. Goorjian</t>
+  </si>
+  <si>
+    <t>People of ArPalodeon Pictures(In Association With)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
+  </si>
+  <si>
+    <t>Michael Jai White</t>
+  </si>
+  <si>
+    <t>Jaigantic Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
+  </si>
+  <si>
+    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
+  </si>
+  <si>
+    <t>Tyler Sansom</t>
+  </si>
+  <si>
+    <t>First Capital FilmsKappa Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
+  </si>
+  <si>
+    <t>Kaige Chen</t>
+  </si>
+  <si>
+    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
+  </si>
+  <si>
+    <t>Big Picture RanchBenenson Productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
+  </si>
+  <si>
+    <t>Richard Dewey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
+  </si>
+  <si>
+    <t>Aristotle Torres</t>
+  </si>
+  <si>
+    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
+  </si>
+  <si>
+    <t>Luca Balser</t>
+  </si>
+  <si>
+    <t>Gummy Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
+  </si>
+  <si>
+    <t>Hiroshi Akabane</t>
+  </si>
+  <si>
+    <t>HS ProductionsIRH Press Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
+  </si>
+  <si>
+    <t>John Stalberg Jr.</t>
+  </si>
+  <si>
+    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
+  </si>
+  <si>
+    <t>Jude Okwudiafor Johnson</t>
+  </si>
+  <si>
+    <t>Anchor Media Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
+  </si>
+  <si>
+    <t>World's Fair Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
+  </si>
+  <si>
+    <t>Andrea Di Stefano</t>
+  </si>
+  <si>
+    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
+  </si>
+  <si>
+    <t>Miguel Ángel Vivas</t>
+  </si>
+  <si>
+    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
+  </si>
+  <si>
+    <t>Frank Cimière</t>
+  </si>
+  <si>
+    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marc Missonnier ... producer </t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,000,378
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,388,017
+</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2783019777/?ref_=bo_md_table_8</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2106360577/?ref_=bo_md_table_9</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3568206593/?ref_=bo_md_table_36</t>
+  </si>
+  <si>
+    <t>20th Century StudiosKinberg GenreScott Free ProductionsTSG EntertainmentThe Mark Gordon Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrico Ballarin ... line producer: Venice  Kenneth Branagh ... producer (p.g.a.) Martin Curry ... associate producer  Mark Gordon ... executive producer  Judy Hofflund ... producer (p.g.a.) Louise Killin ... executive producer  Simon Kinberg ... producer  James Prichard ... executive producer  Ridley Scott ... producer </t>
+  </si>
+  <si>
+    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)Playtone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Brooks ... executive producer  Michael P. Flannigan ... executive producer  Gary Goetzman ... producer  Tom Hanks ... producer  Scott Niemeyer ... executive producer  Eric Quijano ... associate producer  Kostas Raftopoulos ... line producer: Greece  Steve Shareshian ... executive producer  Julie Shimer ... associate producer (as Julie Shimer Lawrence) Jonathan Shore ... co-producer  Nia Vardalos ... executive producer  Rita Wilson ... producer (produced by)(p.g.a)</t>
+  </si>
+  <si>
+    <t>Red Chillies Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gauri Khan ... producer  Gaurav Verma ... co-producer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">89,060,830
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">167,605,171
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,449,159
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249,149,159
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40,750,223
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,950,223
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,039,951
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103,116,671
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,297,240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56,984,243
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,624,825
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,428,526
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,086,021
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62,992,122
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,526,363
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,461,442
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,983,467
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,983,467
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,937,308
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,365,832
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,600,137
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,482,605
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,602,988
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,973,543
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,108,247
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,108,247
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">409,313
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">423,024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376,719
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376,719
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224,585
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224,585
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">168,926
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">168,926
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,910
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,910
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,599
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81,599
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,748
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171,463
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,535
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,535
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,570
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,570
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,419
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">757,434
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,273
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,273
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,300
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,300
+</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2123662081/?ref_=bo_md_table_10</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3028583169/?ref_=bo_md_table_11</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3584983809/?ref_=bo_md_table_18</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl984056577/?ref_=bo_md_table_19</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_24</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_25</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl464618241/?ref_=bo_md_table_26</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3182002945/?ref_=bo_md_table_27</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1722778369/?ref_=bo_md_table_37</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3719136001/?ref_=bo_md_table_38</t>
+  </si>
+  <si>
+    <t>Antoine Fuqua</t>
+  </si>
+  <si>
+    <t>Michael Chaves</t>
+  </si>
+  <si>
+    <t>Cal Brunker</t>
+  </si>
+  <si>
+    <t>Kenneth Branagh</t>
+  </si>
+  <si>
+    <t>Kevin Greutert</t>
+  </si>
+  <si>
+    <t>Aldea M EstudiosCorazón FilmsLions Gate FilmsLionsgate ProductionsTwisted Pictures</t>
+  </si>
+  <si>
+    <t>Nia Vardalos</t>
+  </si>
+  <si>
+    <t>Gareth Edwards</t>
+  </si>
+  <si>
+    <t>Scott Waugh</t>
+  </si>
+  <si>
+    <t>Atlee</t>
+  </si>
+  <si>
+    <t>Andrew Hyatt</t>
+  </si>
+  <si>
+    <t>Craig Gillespie</t>
+  </si>
+  <si>
     <t>Black Bear PicturesColumbia PicturesRyder Picture CompanySony Pictures Entertainment (SPE)Stage 6 Films</t>
   </si>
   <si>
     <t xml:space="preserve"> Rebecca Angelo ... executive producer  Lauren Schuker Blum ... executive producer  Loren Brock ... line producer: LA unit  Christopher Casanova ... co-producer  John Friedberg ... executive producer  Craig Gillespie ... producer  Michael Heimler ... executive producer  Johnny Holland ... executive producer  Ben Mezrich ... executive producer  Johnny Pariseau ... co-producer  Aaron Ryder ... producer (produced by)(p.g.a.) Teddy Schwarzman ... producer  Claire Severance ... associate producer  Andrew Swett ... executive producer  Kevin Ulrich ... executive producer  Cameron Winklevoss ... executive producer  Tyler Winklevoss ... executive producer </t>
   </si>
   <si>
-    <t>GND Media GroupStacey Films(in association with)Tread Lively</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dan Campbell ... associate producer  Zach Dasher ... producer  Troy Duhon ... executive producer  Bob Katz ... executive producer  Robert Katz ... producer  Jason Melton ... executive producer  Shelley D. Needham ... line producer  Cole Prine ... producer  Korie Robertson ... producer  Willie Robertson ... executive producer  Jeremy John Wells ... executive producer  Brittany Yost ... producer </t>
-  </si>
-  <si>
-    <t>Brightlight PicturesNeonQC Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Arielle Boisvert ... executive producer  Jeff Deutchman ... executive producer  Ryan Friscia ... executive producer  Edward H. Hamm Jr.... executive producer  Raymond Mansfield ... producer  Sean McKittrick ... producer  Jameson Parker ... executive producer  Tom Quinn ... executive producer  Emily Thomas ... executive producer  Shawn Williamson ... executive producer </t>
-  </si>
-  <si>
-    <t>Talking HeadsArnold Stiefel Company(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gary Goetzman ... producer  Gary Kurfirst ... executive producer </t>
-  </si>
-  <si>
-    <t>Matthew Crouch</t>
-  </si>
-  <si>
-    <t>No studios found</t>
-  </si>
-  <si>
-    <t>No producers found</t>
-  </si>
-  <si>
-    <t>Wuershan</t>
-  </si>
-  <si>
-    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
-  </si>
-  <si>
-    <t>Sean Olson</t>
-  </si>
-  <si>
-    <t>Called Higher Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
-  </si>
-  <si>
-    <t>Miles Joris-Peyrafitte</t>
-  </si>
-  <si>
-    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
+    <t>Bishal Dutta</t>
+  </si>
+  <si>
+    <t>Jonathan Demme</t>
   </si>
   <si>
     <t>Aitch Alberto</t>
@@ -609,49 +989,7 @@
     <t xml:space="preserve"> Aitch Alberto ... executive producer  Meredith Bagby ... executive producer  David Boies ... executive producer  Eugenio Derbez ... producer  Nicole Flores ... line producer  Lin-Manuel Miranda ... producer  Ben Odell ... producer  Owen Panettieri ... co-producer  Chris Parker ... producer  Zack Schiller ... executive producer  Kyra Sedgwick ... producer  Dylan Sellers ... producer  Valerie Stadler ... producer </t>
   </si>
   <si>
-    <t>Rudy Valdez</t>
-  </si>
-  <si>
-    <t>Imagine DocumentariesSony Music Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carlos Santana </t>
-  </si>
-  <si>
-    <t>Michael A. Goorjian</t>
-  </si>
-  <si>
-    <t>People of ArPalodeon Pictures(In Association With)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
-  </si>
-  <si>
-    <t>Michael Jai White</t>
-  </si>
-  <si>
-    <t>Jaigantic Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
-  </si>
-  <si>
-    <t>Jim CapobiancoPierre-Luc Granjon</t>
-  </si>
-  <si>
-    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
-  </si>
-  <si>
-    <t>Tyler Sansom</t>
-  </si>
-  <si>
-    <t>First Capital FilmsKappa Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
+    <t>Jim Capobianco, Pierre-Luc Granjon</t>
   </si>
   <si>
     <t>Nicol Paone</t>
@@ -663,7 +1001,7 @@
     <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
   </si>
   <si>
-    <t>Peter FacinelliNick Lyon</t>
+    <t>Peter Facinelli, Nick Lyon</t>
   </si>
   <si>
     <t>Lone Star StorytellersMedia GroupSC Films International</t>
@@ -681,13 +1019,7 @@
     <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
   </si>
   <si>
-    <t>Kaige Chen</t>
-  </si>
-  <si>
-    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
+    <t>Joshua Tickell, Rebecca Harrell Tickell</t>
   </si>
   <si>
     <t>Sébastien Marnier</t>
@@ -699,7 +1031,7 @@
     <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
   </si>
   <si>
-    <t>Bethann HardisonFrédéric Tcheng</t>
+    <t>Bethann Hardison, Frédéric Tcheng</t>
   </si>
   <si>
     <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
@@ -726,7 +1058,7 @@
     <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
   </si>
   <si>
-    <t>Danny O'MalleyAlex Rivest</t>
+    <t>Danny O'Malley, Alex Rivest</t>
   </si>
   <si>
     <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
@@ -735,31 +1067,7 @@
     <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
   </si>
   <si>
-    <t>Joshua TickellRebecca Harrell Tickell</t>
-  </si>
-  <si>
-    <t>Big Picture RanchBenenson Productions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
-  </si>
-  <si>
-    <t>Richard Dewey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
-  </si>
-  <si>
-    <t>Aristotle Torres</t>
-  </si>
-  <si>
-    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
-  </si>
-  <si>
-    <t>Adil El ArbiBilall Fallah</t>
+    <t>Adil El Arbi, Bilall Fallah</t>
   </si>
   <si>
     <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
@@ -768,275 +1076,133 @@
     <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
   </si>
   <si>
-    <t>Luca Balser</t>
-  </si>
-  <si>
-    <t>Gummy Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
-  </si>
-  <si>
-    <t>Hiroshi Akabane</t>
-  </si>
-  <si>
-    <t>HS ProductionsIRH Press Co.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
-  </si>
-  <si>
-    <t>John Stalberg Jr.</t>
-  </si>
-  <si>
-    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
-  </si>
-  <si>
-    <t>Jude Okwudiafor Johnson</t>
-  </si>
-  <si>
-    <t>Anchor Media Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
-  </si>
-  <si>
-    <t>Cru EnnisLee Roy Kunz</t>
-  </si>
-  <si>
-    <t>World's Fair Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
-  </si>
-  <si>
-    <t>Andrea Di Stefano</t>
-  </si>
-  <si>
-    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
-  </si>
-  <si>
-    <t>Miguel Ángel Vivas</t>
-  </si>
-  <si>
-    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
-  </si>
-  <si>
-    <t>Frank Cimière</t>
-  </si>
-  <si>
-    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marc Missonnier ... producer </t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,837,275
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">167,037,275
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81,059,802
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">248,659,802
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38,866,988
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87,066,988
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35,653,726
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102,653,726
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,554,793
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43,854,793
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,517,765
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36,318,793
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,929,037
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61,829,037
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,366,200
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,094,529
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,635,065
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,048,963
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,486,997
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,486,997
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,600,194
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,482,662
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,000,378
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,388,017
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222,410
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222,410
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,811
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,811
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70,125
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">171,840
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,919
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">756,934
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,215
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,215
-</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl2783019777/?ref_=bo_md_table_8</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl2106360577/?ref_=bo_md_table_9</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3568206593/?ref_=bo_md_table_36</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3719136001/?ref_=bo_md_table_37</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1722778369/?ref_=bo_md_table_38</t>
-  </si>
-  <si>
-    <t>20th Century StudiosKinberg GenreScott Free ProductionsTSG EntertainmentThe Mark Gordon Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enrico Ballarin ... line producer: Venice  Kenneth Branagh ... producer (p.g.a.) Martin Curry ... associate producer  Mark Gordon ... executive producer  Judy Hofflund ... producer (p.g.a.) Louise Killin ... executive producer  Simon Kinberg ... producer  James Prichard ... executive producer  Ridley Scott ... producer </t>
-  </si>
-  <si>
-    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)Playtone</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paul Brooks ... executive producer  Michael P. Flannigan ... executive producer  Gary Goetzman ... producer  Tom Hanks ... producer  Scott Niemeyer ... executive producer  Eric Quijano ... associate producer  Kostas Raftopoulos ... line producer: Greece  Steve Shareshian ... executive producer  Julie Shimer ... associate producer (as Julie Shimer Lawrence) Jonathan Shore ... co-producer  Nia Vardalos ... executive producer  Rita Wilson ... producer (produced by)(p.g.a)</t>
-  </si>
-  <si>
-    <t>Red Chillies Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gauri Khan ... producer  Gaurav Verma ... co-producer </t>
+    <t>Cru Ennis, Lee Roy Kunz</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>King Arthur</t>
+  </si>
+  <si>
+    <t>PAW Patrol: The Movie</t>
+  </si>
+  <si>
+    <t>Thor: The Dark World</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>My Big Fat Greek Wedding</t>
+  </si>
+  <si>
+    <t>Rogue One: A Star Wars Story</t>
+  </si>
+  <si>
+    <t>Need for Speed</t>
+  </si>
+  <si>
+    <t>Paul, Apostle of Christ</t>
+  </si>
+  <si>
+    <t>Cruella</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>The Butcher, the Chef, and the Swordsman</t>
+  </si>
+  <si>
+    <t>A Question of Faith</t>
+  </si>
+  <si>
+    <t>Jim Capobianco</t>
+  </si>
+  <si>
+    <t>The Lion King</t>
+  </si>
+  <si>
+    <t>Pierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t>Zibilla</t>
+  </si>
+  <si>
+    <t>The Battle at Lake Changjin</t>
+  </si>
+  <si>
+    <t>Peter Facinelli</t>
+  </si>
+  <si>
+    <t>Nick Lyon</t>
+  </si>
+  <si>
+    <t>Toy Story 2</t>
+  </si>
+  <si>
+    <t>Joshua Tickell</t>
+  </si>
+  <si>
+    <t>Rebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Bethann Hardison</t>
+  </si>
+  <si>
+    <t>Frédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Shortbus</t>
+  </si>
+  <si>
+    <t>Letters to Father Jacob</t>
+  </si>
+  <si>
+    <t>Danny O'Malley</t>
+  </si>
+  <si>
+    <t>Amanda Knox</t>
+  </si>
+  <si>
+    <t>Alex Rivest</t>
+  </si>
+  <si>
+    <t>Uncut Gems</t>
+  </si>
+  <si>
+    <t>Adil El Arbi</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Bilall Fallah</t>
+  </si>
+  <si>
+    <t>Bad Boys for Life</t>
+  </si>
+  <si>
+    <t>High School</t>
+  </si>
+  <si>
+    <t>Cru Ennis</t>
+  </si>
+  <si>
+    <t>Boys of Abu Ghraib</t>
+  </si>
+  <si>
+    <t>Lee Roy Kunz</t>
+  </si>
+  <si>
+    <t>Escobar: Paradise Lost</t>
+  </si>
+  <si>
+    <t>Extinction</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1635,571 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03BAF43-B1E7-49EA-9442-5DB7CCE34CD8}">
+  <dimension ref="A1:C52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C2">
+        <v>203567857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4">
+        <v>144327371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C5">
+        <v>644783140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6">
+        <v>2264743305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C7">
+        <v>368744044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C8">
+        <v>1058682142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C9">
+        <v>203277636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>27514156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11">
+        <v>25915966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12">
+        <v>233503234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>5482605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C14">
+        <v>206678440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1606339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s">
+        <v>328</v>
+      </c>
+      <c r="C16">
+        <v>2089266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>329</v>
+      </c>
+      <c r="C17">
+        <v>2587072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>503378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>423024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>407838</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>376719</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>319848</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>330</v>
+      </c>
+      <c r="B23" t="s">
+        <v>331</v>
+      </c>
+      <c r="C23">
+        <v>968511805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>332</v>
+      </c>
+      <c r="B24" t="s">
+        <v>333</v>
+      </c>
+      <c r="C24">
+        <v>88667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C26">
+        <v>902548476</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>288</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>617143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>335</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>205118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>336</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>205118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>294</v>
+      </c>
+      <c r="B30" t="s">
+        <v>337</v>
+      </c>
+      <c r="C30">
+        <v>497375381</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>338</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31">
+        <v>88910</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>339</v>
+      </c>
+      <c r="B32" t="s">
+        <v>340</v>
+      </c>
+      <c r="C32">
+        <v>89787</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>298</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33">
+        <v>1120899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>341</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>342</v>
+      </c>
+      <c r="B35" t="s">
+        <v>343</v>
+      </c>
+      <c r="C35">
+        <v>5557564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>304</v>
+      </c>
+      <c r="B36" t="s">
+        <v>344</v>
+      </c>
+      <c r="C36">
+        <v>1332577</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>307</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>38683</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>345</v>
+      </c>
+      <c r="B38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C38">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>347</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40">
+        <v>32535</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41">
+        <v>25570</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" t="s">
+        <v>348</v>
+      </c>
+      <c r="C43">
+        <v>50023780</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>349</v>
+      </c>
+      <c r="B44" t="s">
+        <v>350</v>
+      </c>
+      <c r="C44">
+        <v>1692776</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>351</v>
+      </c>
+      <c r="B45" t="s">
+        <v>352</v>
+      </c>
+      <c r="C45">
+        <v>426505244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" t="s">
+        <v>353</v>
+      </c>
+      <c r="C46">
+        <v>221590</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>354</v>
+      </c>
+      <c r="B48" t="s">
+        <v>355</v>
+      </c>
+      <c r="C48">
+        <v>62096</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>356</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49">
+        <v>4883</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>357</v>
+      </c>
+      <c r="C50">
+        <v>6760531</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>181</v>
+      </c>
+      <c r="B51" t="s">
+        <v>358</v>
+      </c>
+      <c r="C51">
+        <v>2350695</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1529,19 +2256,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>259</v>
+        <v>208</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>260</v>
+        <v>209</v>
+      </c>
+      <c r="G2" t="s">
+        <v>268</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1555,19 +2285,22 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>262</v>
+        <v>211</v>
+      </c>
+      <c r="G3" t="s">
+        <v>269</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1575,25 +2308,28 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>263</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>264</v>
+        <v>213</v>
+      </c>
+      <c r="G4" t="s">
+        <v>270</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1601,25 +2337,28 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>188</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>266</v>
+        <v>215</v>
+      </c>
+      <c r="G5" t="s">
+        <v>271</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>298</v>
+        <v>202</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>299</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1627,25 +2366,28 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>189</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>267</v>
+        <v>216</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>268</v>
+        <v>217</v>
+      </c>
+      <c r="G6" t="s">
+        <v>272</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>143</v>
+        <v>273</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1653,25 +2395,28 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>190</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>269</v>
+        <v>218</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>270</v>
+        <v>219</v>
+      </c>
+      <c r="G7" t="s">
+        <v>274</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>300</v>
+        <v>204</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>301</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1685,19 +2430,22 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>271</v>
+        <v>220</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>272</v>
+        <v>221</v>
+      </c>
+      <c r="G8" t="s">
+        <v>275</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="255" x14ac:dyDescent="0.25">
@@ -1705,25 +2453,28 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>293</v>
+        <v>199</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>273</v>
+        <v>222</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>274</v>
+        <v>223</v>
+      </c>
+      <c r="G9" t="s">
+        <v>276</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1731,1028 +2482,1043 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>294</v>
+        <v>200</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
+        <v>277</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>302</v>
+        <v>206</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>258</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>275</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>276</v>
+        <v>225</v>
+      </c>
+      <c r="G11" t="s">
+        <v>278</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>259</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>277</v>
+        <v>226</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>278</v>
+        <v>227</v>
+      </c>
+      <c r="G12" t="s">
+        <v>279</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>151</v>
+        <v>280</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>152</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>280</v>
+        <v>229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>282</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>281</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>282</v>
+        <v>198</v>
+      </c>
+      <c r="G14" t="s">
+        <v>283</v>
       </c>
       <c r="H14" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>88</v>
+        <v>231</v>
       </c>
       <c r="G16" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>89</v>
+        <v>232</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>90</v>
+        <v>233</v>
       </c>
       <c r="G17" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="H18" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>93</v>
+        <v>234</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>94</v>
+        <v>235</v>
       </c>
       <c r="G19" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>284</v>
       </c>
       <c r="H20" t="s">
-        <v>173</v>
+        <v>285</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>174</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="G21" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="H22" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>181</v>
+        <v>287</v>
       </c>
       <c r="H23" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="G24" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="405" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>262</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>103</v>
+        <v>240</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="G25" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="H25" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>263</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>190</v>
+        <v>288</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>264</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="G27" t="s">
-        <v>193</v>
+        <v>291</v>
       </c>
       <c r="H27" t="s">
-        <v>194</v>
+        <v>292</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>265</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="G28" t="s">
-        <v>196</v>
+        <v>294</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>197</v>
+        <v>295</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>253</v>
+        <v>191</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>286</v>
+        <v>243</v>
       </c>
       <c r="G29" t="s">
-        <v>199</v>
+        <v>297</v>
       </c>
       <c r="H29" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>254</v>
+        <v>192</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G30" t="s">
-        <v>202</v>
+        <v>298</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>203</v>
+        <v>299</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>255</v>
+        <v>193</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>113</v>
+        <v>244</v>
       </c>
       <c r="E31" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>114</v>
+        <v>245</v>
       </c>
       <c r="G31" t="s">
-        <v>205</v>
+        <v>301</v>
       </c>
       <c r="H31" t="s">
-        <v>206</v>
+        <v>302</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>207</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
       <c r="G32" t="s">
-        <v>208</v>
+        <v>304</v>
       </c>
       <c r="H32" t="s">
-        <v>209</v>
+        <v>305</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>210</v>
+        <v>306</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>257</v>
+        <v>195</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>211</v>
+        <v>307</v>
       </c>
       <c r="H33" t="s">
-        <v>212</v>
+        <v>308</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>258</v>
+        <v>196</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>214</v>
+        <v>310</v>
       </c>
       <c r="H34" t="s">
-        <v>215</v>
+        <v>311</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>216</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>119</v>
+        <v>248</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>120</v>
+        <v>249</v>
       </c>
       <c r="G35" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="H35" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>121</v>
+        <v>250</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>122</v>
+        <v>251</v>
       </c>
       <c r="G36" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
       <c r="H36" t="s">
-        <v>220</v>
+        <v>162</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>295</v>
+        <v>201</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>289</v>
+        <v>252</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="G37" t="s">
-        <v>222</v>
+        <v>167</v>
       </c>
       <c r="H37" t="s">
-        <v>223</v>
+        <v>168</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>224</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>296</v>
+        <v>266</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>123</v>
+        <v>254</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>124</v>
+        <v>255</v>
       </c>
       <c r="G38" t="s">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>228</v>
+        <v>313</v>
       </c>
       <c r="H39" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>230</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="H40" t="s">
-        <v>232</v>
+        <v>171</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>233</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="G41" t="s">
-        <v>234</v>
+        <v>173</v>
       </c>
       <c r="H41" t="s">
-        <v>235</v>
+        <v>174</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>236</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="E42" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="G42" t="s">
-        <v>237</v>
+        <v>316</v>
       </c>
       <c r="H42" t="s">
-        <v>238</v>
+        <v>176</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>239</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="G43" t="s">
-        <v>240</v>
+        <v>178</v>
       </c>
       <c r="H43" t="s">
-        <v>241</v>
+        <v>179</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>242</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="G44" t="s">
-        <v>243</v>
+        <v>181</v>
       </c>
       <c r="H44" t="s">
-        <v>244</v>
+        <v>182</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>245</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="G45" t="s">
-        <v>246</v>
+        <v>184</v>
       </c>
       <c r="H45" t="s">
-        <v>247</v>
+        <v>185</v>
       </c>
       <c r="I45" t="s">
-        <v>248</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2764,7 +3530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C8FA34-854C-4FDF-A76D-37677D1C3B05}">
   <dimension ref="A1:D1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updating Movie_Data in preparation for merging director branch in
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277884-1C33-4AF8-983E-960B8A651E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A5D6C2-46BC-4BB9-BD9E-6268BB0A3CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
-    <sheet name="Director's Highest gross Films" sheetId="1" r:id="rId2"/>
+    <sheet name="Directors" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="267">
   <si>
     <t>Film Title</t>
   </si>
@@ -715,6 +715,129 @@
   </si>
   <si>
     <t xml:space="preserve"> Tarak Ben Ammar ... executive producer  Todd Black ... producer (produced by)(p.g.a.) David Bloomfield ... executive producer  Jason Blumenthal ... producer (produced by)(p.g.a.) Vito Colazzo ... line producer  Tony Eldridge ... producer (produced by) Antoine Fuqua ... producer (produced by)(p.g.a.) Andy Mitchell ... executive producer  Samir M. Patel ... executive producer (as Samir Patel) Guja Quaranta ... line producer  Kat Samick ... executive producer  Alex Siskin ... producer (produced by) Enzo Sisti ... executive producer  Michael Sloan ... producer (produced by) Steve Tisch ... producer (produced by) Clayton Townsend ... producer (produced by)(p.g.a.) Denzel Washington ... producer (produced by) Richard Wenk ... co-producer </t>
+  </si>
+  <si>
+    <t>King Arthur</t>
+  </si>
+  <si>
+    <t>PAW Patrol: The Movie</t>
+  </si>
+  <si>
+    <t>Thor: The Dark World</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>My Big Fat Greek Wedding</t>
+  </si>
+  <si>
+    <t>Rogue One: A Star Wars Story</t>
+  </si>
+  <si>
+    <t>Need for Speed</t>
+  </si>
+  <si>
+    <t>Paul, Apostle of Christ</t>
+  </si>
+  <si>
+    <t>Cruella</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>The Butcher, the Chef, and the Swordsman</t>
+  </si>
+  <si>
+    <t>A Question of Faith</t>
+  </si>
+  <si>
+    <t>Jim Capobianco</t>
+  </si>
+  <si>
+    <t>The Lion King</t>
+  </si>
+  <si>
+    <t>Pierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t>Zibilla</t>
+  </si>
+  <si>
+    <t>The Battle at Lake Changjin</t>
+  </si>
+  <si>
+    <t>Peter Facinelli</t>
+  </si>
+  <si>
+    <t>Nick Lyon</t>
+  </si>
+  <si>
+    <t>Toy Story 2</t>
+  </si>
+  <si>
+    <t>Joshua Tickell</t>
+  </si>
+  <si>
+    <t>Rebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Bethann Hardison</t>
+  </si>
+  <si>
+    <t>Frédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Shortbus</t>
+  </si>
+  <si>
+    <t>Letters to Father Jacob</t>
+  </si>
+  <si>
+    <t>Danny O'Malley</t>
+  </si>
+  <si>
+    <t>Amanda Knox</t>
+  </si>
+  <si>
+    <t>Alex Rivest</t>
+  </si>
+  <si>
+    <t>Uncut Gems</t>
+  </si>
+  <si>
+    <t>Adil El Arbi</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Bilall Fallah</t>
+  </si>
+  <si>
+    <t>Bad Boys for Life</t>
+  </si>
+  <si>
+    <t>High School</t>
+  </si>
+  <si>
+    <t>Cru Ennis</t>
+  </si>
+  <si>
+    <t>Boys of Abu Ghraib</t>
+  </si>
+  <si>
+    <t>Lee Roy Kunz</t>
+  </si>
+  <si>
+    <t>Escobar: Paradise Lost</t>
+  </si>
+  <si>
+    <t>Extinction</t>
   </si>
 </sst>
 </file>
@@ -753,7 +876,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -794,19 +917,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -821,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -829,8 +939,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,25 +1274,25 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1197,10 +1306,10 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>89060830</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>167605171</v>
       </c>
       <c r="F2" t="s">
@@ -1223,10 +1332,10 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>81449159</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>249149159</v>
       </c>
       <c r="F3" t="s">
@@ -1249,10 +1358,10 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>40750223</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>88950223</v>
       </c>
       <c r="F4" t="s">
@@ -1275,10 +1384,10 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>36039951</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>103116671</v>
       </c>
       <c r="F5" t="s">
@@ -1301,10 +1410,10 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>33297240</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>56984243</v>
       </c>
       <c r="F6" t="s">
@@ -1327,10 +1436,10 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>27624825</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>36428526</v>
       </c>
       <c r="F7" t="s">
@@ -1353,10 +1462,10 @@
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>26086021</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>62992122</v>
       </c>
       <c r="F8" t="s">
@@ -1379,10 +1488,10 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>15526363</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>27461442</v>
       </c>
       <c r="F9" t="s">
@@ -1405,10 +1514,10 @@
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>14735611</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>27514156</v>
       </c>
       <c r="F10" t="s">
@@ -1431,10 +1540,10 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>10983467</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>10983467</v>
       </c>
       <c r="F11" t="s">
@@ -1457,10 +1566,10 @@
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>10937308</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>12365832</v>
       </c>
       <c r="F12" t="s">
@@ -1483,10 +1592,10 @@
       <c r="C13">
         <v>12</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>4600137</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>5482605</v>
       </c>
       <c r="F13" t="s">
@@ -1509,10 +1618,10 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>4000378</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>4388017</v>
       </c>
       <c r="F14" t="s">
@@ -1535,10 +1644,10 @@
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>1606339</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>1606339</v>
       </c>
       <c r="F15" t="s">
@@ -1559,10 +1668,10 @@
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>1602988</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>1973543</v>
       </c>
       <c r="F16" t="s">
@@ -1585,10 +1694,10 @@
       <c r="C17">
         <v>16</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>1108247</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>1108247</v>
       </c>
       <c r="F17" t="s">
@@ -1611,10 +1720,10 @@
       <c r="C18">
         <v>17</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>503378</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>503378</v>
       </c>
       <c r="F18" t="s">
@@ -1637,10 +1746,10 @@
       <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>409313</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>423024</v>
       </c>
       <c r="F19" t="s">
@@ -1663,10 +1772,10 @@
       <c r="C20">
         <v>19</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>407838</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>407838</v>
       </c>
       <c r="F20" t="s">
@@ -1689,10 +1798,10 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>376719</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>376719</v>
       </c>
       <c r="F21" t="s">
@@ -1715,10 +1824,10 @@
       <c r="C22">
         <v>21</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>319848</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>319848</v>
       </c>
       <c r="F22" t="s">
@@ -1741,10 +1850,10 @@
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>306385</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>306385</v>
       </c>
       <c r="F23" t="s">
@@ -1767,10 +1876,10 @@
       <c r="C24">
         <v>23</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>224585</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>224585</v>
       </c>
       <c r="F24" t="s">
@@ -1793,10 +1902,10 @@
       <c r="C25">
         <v>24</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>168926</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>168926</v>
       </c>
       <c r="F25" t="s">
@@ -1819,10 +1928,10 @@
       <c r="C26">
         <v>25</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>139358</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>617143</v>
       </c>
       <c r="F26" t="s">
@@ -1845,10 +1954,10 @@
       <c r="C27">
         <v>26</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>205118</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>205118</v>
       </c>
       <c r="F27" t="s">
@@ -1871,10 +1980,10 @@
       <c r="C28">
         <v>27</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>130802</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>130802</v>
       </c>
       <c r="F28" t="s">
@@ -1897,10 +2006,10 @@
       <c r="C29">
         <v>28</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>88910</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>88910</v>
       </c>
       <c r="F29" t="s">
@@ -1923,10 +2032,10 @@
       <c r="C30">
         <v>29</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>87344</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>1120899</v>
       </c>
       <c r="F30" t="s">
@@ -1949,10 +2058,10 @@
       <c r="C31">
         <v>30</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>81599</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>81599</v>
       </c>
       <c r="F31" t="s">
@@ -1975,10 +2084,10 @@
       <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>69748</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>171463</v>
       </c>
       <c r="F32" t="s">
@@ -2001,10 +2110,10 @@
       <c r="C33">
         <v>32</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>38683</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>38683</v>
       </c>
       <c r="F33" t="s">
@@ -2027,10 +2136,10 @@
       <c r="C34">
         <v>33</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>35563</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>35563</v>
       </c>
       <c r="F34" t="s">
@@ -2053,10 +2162,10 @@
       <c r="C35">
         <v>34</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>32535</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>32535</v>
       </c>
       <c r="F35" t="s">
@@ -2076,10 +2185,10 @@
       <c r="C36">
         <v>35</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>25570</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>25570</v>
       </c>
       <c r="F36" t="s">
@@ -2102,10 +2211,10 @@
       <c r="C37">
         <v>36</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>14419</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>757434</v>
       </c>
       <c r="F37" t="s">
@@ -2128,10 +2237,10 @@
       <c r="C38">
         <v>37</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>13273</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>13273</v>
       </c>
       <c r="F38" t="s">
@@ -2154,10 +2263,10 @@
       <c r="C39">
         <v>38</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <v>10500</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
         <v>173121</v>
       </c>
       <c r="F39" t="s">
@@ -2180,10 +2289,10 @@
       <c r="C40">
         <v>39</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <v>7807</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="6">
         <v>7807</v>
       </c>
       <c r="F40" t="s">
@@ -2206,10 +2315,10 @@
       <c r="C41">
         <v>40</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="6">
         <v>5300</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="6">
         <v>5300</v>
       </c>
       <c r="F41" t="s">
@@ -2232,10 +2341,10 @@
       <c r="C42">
         <v>41</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="6">
         <v>4883</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="6">
         <v>4883</v>
       </c>
       <c r="F42" t="s">
@@ -2258,10 +2367,10 @@
       <c r="C43">
         <v>42</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="6">
         <v>3865</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="6">
         <v>4580566</v>
       </c>
       <c r="F43" t="s">
@@ -2284,10 +2393,10 @@
       <c r="C44">
         <v>43</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="6">
         <v>684</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="6">
         <v>147849</v>
       </c>
       <c r="F44" t="s">
@@ -2310,10 +2419,10 @@
       <c r="C45">
         <v>44</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>539</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>371989</v>
       </c>
       <c r="F45" t="s">
@@ -2332,33 +2441,571 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C8FA34-854C-4FDF-A76D-37677D1C3B05}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91483600-9243-44C6-AC9E-CDA1A8649D8B}">
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2">
+        <v>203567857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4">
+        <v>144327371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5">
+        <v>644783140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6">
+        <v>2264743305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7">
+        <v>368744044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8">
+        <v>1058682142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9">
+        <v>203277636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>27514156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11">
+        <v>25915966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12">
+        <v>233503234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>5482605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14">
+        <v>206678440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>1606339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16">
+        <v>2089266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17">
+        <v>2587072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>503378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>423024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20">
+        <v>407838</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>376719</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22">
+        <v>319848</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23">
+        <v>968511805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24">
+        <v>88667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26">
+        <v>902548476</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>617143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28">
+        <v>205118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29">
+        <v>205118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30">
+        <v>497375381</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>246</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>88910</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32" t="s">
+        <v>248</v>
+      </c>
+      <c r="C32">
+        <v>89787</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33">
+        <v>1120899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>250</v>
+      </c>
+      <c r="B35" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35">
+        <v>5557564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" t="s">
+        <v>252</v>
+      </c>
+      <c r="C36">
+        <v>1332577</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37">
+        <v>38683</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>253</v>
+      </c>
+      <c r="B38" t="s">
+        <v>254</v>
+      </c>
+      <c r="C38">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40">
+        <v>32535</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41">
+        <v>25570</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>199</v>
+      </c>
+      <c r="B43" t="s">
+        <v>256</v>
+      </c>
+      <c r="C43">
+        <v>50023780</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>257</v>
+      </c>
+      <c r="B44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44">
+        <v>1692776</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>259</v>
+      </c>
+      <c r="B45" t="s">
+        <v>260</v>
+      </c>
+      <c r="C45">
+        <v>426505244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>205</v>
+      </c>
+      <c r="B46" t="s">
+        <v>261</v>
+      </c>
+      <c r="C46">
+        <v>221590</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>208</v>
+      </c>
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>262</v>
+      </c>
+      <c r="B48" t="s">
+        <v>263</v>
+      </c>
+      <c r="C48">
+        <v>62096</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>264</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49">
+        <v>4883</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50">
+        <v>6760531</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51">
+        <v>2350695</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Functionality working as expected, all issues solved, number formatting changed to currency.
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\se762\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCE4C75-241B-42CC-8BF7-BF1F345CE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA456FE-1786-4A6B-BD63-1D079FE2538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9360" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="Directors" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="320">
   <si>
     <t>Film Title</t>
   </si>
@@ -178,15 +178,27 @@
     <t>The Kill Room</t>
   </si>
   <si>
+    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_24</t>
+  </si>
+  <si>
     <t>On Fire</t>
   </si>
   <si>
+    <t>https://www.boxofficemojo.com/release/rl464618241/?ref_=bo_md_table_25</t>
+  </si>
+  <si>
     <t>Zombie Town</t>
   </si>
   <si>
+    <t>https://www.boxofficemojo.com/release/rl3182002945/?ref_=bo_md_table_26</t>
+  </si>
+  <si>
     <t>Farewell My Concubine</t>
   </si>
   <si>
+    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_27</t>
+  </si>
+  <si>
     <t>The Origin of Evil</t>
   </si>
   <si>
@@ -442,6 +454,12 @@
     <t xml:space="preserve"> Vessela Banzourkova ... line producer  Christa Campbell ... executive producer  Guymon Casady ... executive producer  Spenser Cohen ... executive producer  Michael S. Constable ... executive producer  Jason Constantine ... executive producer  Allen Dam ... executive producer  Boaz Davidson ... executive producer  Jon Feltheimer ... executive producer  Claiton Fernandes ... co-executive producer  Vladimir Fernandes ... co-executive producer  Jeffrey Greenstein ... executive producer  Lati Grobman ... executive producer  Victor Hadida ... co-executive producer  Anna Halberg ... executive producer  Basil Iwanyk ... executive producer  K. Blaine Johnston ... executive producer  Eda Kowan ... executive producer  Avi Lerner ... executive producer  Yariv Lerner ... producer  Gisella Marengo ... co-producer  Balan Melarkode ... co-executive producer  Abby Mills ... co-producer  Euzebio Munhoz Jr.... co-executive producer  Matthew O'Toole ... co-producer  Stephen Paul ... executive producer  Lonnie Ramati ... co-executive producer  Trevor Short ... executive producer  Jason Statham ... producer  Kevin King Templeton ... producer  Robert Van Norden ... executive producer  Les Weldon ... producer  Gareth West ... executive producer  Christopher Woodrow ... executive producer  Jonathan Yunger ... executive producer </t>
   </si>
   <si>
+    <t>Black Bear PicturesColumbia PicturesRyder Picture CompanySony Pictures Entertainment (SPE)Stage 6 Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rebecca Angelo ... executive producer  Lauren Schuker Blum ... executive producer  Loren Brock ... line producer: LA unit  Christopher Casanova ... co-producer  John Friedberg ... executive producer  Craig Gillespie ... producer  Michael Heimler ... executive producer  Johnny Holland ... executive producer  Ben Mezrich ... executive producer  Johnny Pariseau ... co-producer  Aaron Ryder ... producer (produced by)(p.g.a.) Teddy Schwarzman ... producer  Claire Severance ... associate producer  Andrew Swett ... executive producer  Kevin Ulrich ... executive producer  Cameron Winklevoss ... executive producer  Tyler Winklevoss ... executive producer </t>
+  </si>
+  <si>
     <t>GND Media GroupStacey Films(in association with)Tread Lively</t>
   </si>
   <si>
@@ -460,248 +478,470 @@
     <t xml:space="preserve"> Gary Goetzman ... producer  Gary Kurfirst ... executive producer </t>
   </si>
   <si>
+    <t>No studios found</t>
+  </si>
+  <si>
+    <t>No producers found</t>
+  </si>
+  <si>
+    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
+  </si>
+  <si>
+    <t>Called Higher Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
+  </si>
+  <si>
+    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
+  </si>
+  <si>
+    <t>Imagine DocumentariesSony Music Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Santana </t>
+  </si>
+  <si>
+    <t>People of ArPalodeon Pictures(In Association With)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
+  </si>
+  <si>
+    <t>Jaigantic Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
+  </si>
+  <si>
+    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
+  </si>
+  <si>
+    <t>First Capital FilmsKappa Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
+  </si>
+  <si>
+    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
+  </si>
+  <si>
+    <t>Lone Star StorytellersMedia GroupSC Films International</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
+  </si>
+  <si>
+    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
+  </si>
+  <si>
+    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
+  </si>
+  <si>
+    <t>Big Picture RanchBenenson Productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
+  </si>
+  <si>
+    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
+  </si>
+  <si>
+    <t>Gummy Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
+  </si>
+  <si>
+    <t>HS ProductionsIRH Press Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
+  </si>
+  <si>
+    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
+  </si>
+  <si>
+    <t>Anchor Media Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
+  </si>
+  <si>
+    <t>World's Fair Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
+  </si>
+  <si>
+    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
+  </si>
+  <si>
+    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
+  </si>
+  <si>
+    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marc Missonnier ... producer </t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,000,378
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,388,017
+</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2783019777/?ref_=bo_md_table_8</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl2106360577/?ref_=bo_md_table_9</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3568206593/?ref_=bo_md_table_36</t>
+  </si>
+  <si>
+    <t>20th Century StudiosKinberg GenreScott Free ProductionsTSG EntertainmentThe Mark Gordon Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrico Ballarin ... line producer: Venice  Kenneth Branagh ... producer (p.g.a.) Martin Curry ... associate producer  Mark Gordon ... executive producer  Judy Hofflund ... producer (p.g.a.) Louise Killin ... executive producer  Simon Kinberg ... producer  James Prichard ... executive producer  Ridley Scott ... producer </t>
+  </si>
+  <si>
+    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)Playtone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Brooks ... executive producer  Michael P. Flannigan ... executive producer  Gary Goetzman ... producer  Tom Hanks ... producer  Scott Niemeyer ... executive producer  Eric Quijano ... associate producer  Kostas Raftopoulos ... line producer: Greece  Steve Shareshian ... executive producer  Julie Shimer ... associate producer (as Julie Shimer Lawrence) Jonathan Shore ... co-producer  Nia Vardalos ... executive producer  Rita Wilson ... producer (produced by)(p.g.a)</t>
+  </si>
+  <si>
+    <t>Red Chillies Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gauri Khan ... producer  Gaurav Verma ... co-producer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,600,137
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,482,605
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,602,988
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,973,543
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,108,247
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,108,247
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">409,313
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">423,024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,910
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88,910
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,748
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171,463
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,535
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,535
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,570
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,570
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,273
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,273
+</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3584983809/?ref_=bo_md_table_18</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl984056577/?ref_=bo_md_table_19</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1722778369/?ref_=bo_md_table_37</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3719136001/?ref_=bo_md_table_38</t>
+  </si>
+  <si>
+    <t>Antoine Fuqua</t>
+  </si>
+  <si>
+    <t>Boies Schiller Entertainment3Pas Studios5000 Broadway ProductionsBig Swing ProductionsLimelight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aitch Alberto ... executive producer  Meredith Bagby ... executive producer  David Boies ... executive producer  Eugenio Derbez ... producer  Nicole Flores ... line producer  Lin-Manuel Miranda ... producer  Ben Odell ... producer  Owen Panettieri ... co-producer  Chris Parker ... producer  Zack Schiller ... executive producer  Kyra Sedgwick ... producer  Dylan Sellers ... producer  Valerie Stadler ... producer </t>
+  </si>
+  <si>
+    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
+  </si>
+  <si>
+    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
+  </si>
+  <si>
+    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
+  </si>
+  <si>
+    <t>Upstream Pictures (II)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
+  </si>
+  <si>
+    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
+  </si>
+  <si>
+    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
+  </si>
+  <si>
+    <t>Michael Chaves</t>
+  </si>
+  <si>
+    <t>Cal Brunker</t>
+  </si>
+  <si>
+    <t>Kenneth Branagh</t>
+  </si>
+  <si>
+    <t>Kevin Greutert</t>
+  </si>
+  <si>
+    <t>Nia Vardalos</t>
+  </si>
+  <si>
+    <t>Gareth Edwards</t>
+  </si>
+  <si>
+    <t>Scott Waugh</t>
+  </si>
+  <si>
+    <t>Atlee</t>
+  </si>
+  <si>
+    <t>Craig Gillespie</t>
+  </si>
+  <si>
+    <t>Andrew Hyatt</t>
+  </si>
+  <si>
+    <t>Bishal Dutta</t>
+  </si>
+  <si>
+    <t>Jonathan Demme</t>
+  </si>
+  <si>
     <t>Matthew Crouch</t>
   </si>
   <si>
-    <t>No studios found</t>
-  </si>
-  <si>
-    <t>No producers found</t>
-  </si>
-  <si>
     <t>Wuershan</t>
   </si>
   <si>
-    <t>Tencent PicturesBeijing CultureMongketengri Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yang Du ... executive producer  William Kong ... executive producer  Barrie M. Osborne ... production consultant  Ye Sun ... line producer </t>
-  </si>
-  <si>
     <t>Sean Olson</t>
   </si>
   <si>
-    <t>Called Higher Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jason Lee Brown ... producer  Phillip Glasser ... producer  Brad Goen ... associate producer  Ashley Greyson ... executive producer  Sean Olson ... co-producer  Justin Vesci ... executive producer  Andy Woolard ... associate producer </t>
-  </si>
-  <si>
     <t>Miles Joris-Peyrafitte</t>
   </si>
   <si>
-    <t>SSS EntertainmentArtemisPriority Pictures(in association with)SSS Film Capital(funding, in association with)Votiv Films(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Luke Daniels ... executive producer  Lizzie Friedman ... executive producer  Jeffrey Giles ... executive producer  Richard Goldberg ... executive producer  Peter Jarowey ... executive producer  Karen Lauder ... executive producer  Greg Little ... executive producer  Michael Lurie ... executive producer  Siena Oberman ... producer  Derek Rubin ... co-producer  Shaun Sanghani ... producer  Brent Stiefel ... executive producer  Hilary Swank ... executive producer  Emma Tillinger Koskoff ... producer  Peter Winther ... executive producer </t>
-  </si>
-  <si>
     <t>Rudy Valdez</t>
   </si>
   <si>
-    <t>Imagine DocumentariesSony Music Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carlos Santana </t>
+    <t>Aitch Alberto</t>
   </si>
   <si>
     <t>Michael A. Goorjian</t>
   </si>
   <si>
-    <t>People of ArPalodeon Pictures(In Association With)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vartan Barsoumian ... executive producer  Michael A. Goorjian ... producer  Robert Patrick Malkassian ... producer  Arman Nshanian ... producer  Knarik Sargsyan ... line producer  Serj Tankian ... executive producer  Sol Tryon ... producer  Ani Vorskanyan ... co-producer </t>
-  </si>
-  <si>
     <t>Michael Jai White</t>
   </si>
   <si>
-    <t>Jaigantic Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
-  </si>
-  <si>
-    <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kat Alioshin ... executive producer / line producer  Ali Baghdadi ... executive producer  Olivier Barbier ... executive producer  Joshua A. Bevan ... co-executive producer  Jay Burnley ... executive producer  Ellen Byrne ... co-producer  Chris Capobianco ... executive producer  Jim Capobianco ... producer (produced by) Carmella Casinelli ... executive producer  Justin Chen ... executive producer  Ryan Clarkson ... executive producer  Lorenz Evans ... co-executive producer  Lucas A. Ferrara ... co-executive producer  Raymond Fino ... executive producer  Nicolas Flory ... executive producer  Mimi Polk Gitlin ... executive producer  Don Hahn ... executive producer  Chris Ihlenfeldt ... co-executive producer  Fionnuala Jamison ... executive producer  Nathanaël Karmitz ... executive producer  David Lyons ... executive producer  Christopher Massimine ... executive producer  Keanu Mayo ... executive producer  Vince McCarthy ... co-producer  Rob McGillivray ... executive producer  Martin Metz ... producer  Steve Muench ... executive producer  Habib Paracha ... executive producer  Adrian Politowski ... producer  Robert Rippberger ... producer (produced by)(p.g.a.) Raymond Sandra ... executive producer  Sita Saviolo ... executive producer  Laura Schlessinger ... executive producer  Jacob Michael Silva ... co-executive producer  Ben Stranahan ... executive producer  Kyle Stroud ... executive producer  Chelsea Tieu ... executive producer  Ilan Urroz ... executive producer  Phil Viardo ... executive producer  Eric Vonfeldt ... executive producer  Neuman Vong ... executive producer  Katherine Waddell ... executive producer  Jeremy Walton ... executive producer  Pierce Young ... executive producer  J.D. Zacharias ... executive producer </t>
+    <t>Jim Capobianco, Pierre-Luc Granjon</t>
   </si>
   <si>
     <t>Tyler Sansom</t>
   </si>
   <si>
-    <t>First Capital FilmsKappa Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cameron Arnett ... producer  Ty Carter ... producer  Steve Degrasse ... supervising producer  Brandon Feller ... producer  John French ... producer  Mark Hubbard ... producer  Will Kramer ... executive producer  Paul L. Long ... producer  Evan Mitchum ... producer  Justen Overlander ... executive producer  Eric Pavey ... producer  Mark Richt ... associate producer  Tyler Sansom ... producer  Brad J. Silverman ... producer  Chris Skomra ... associate producer </t>
+    <t>Nicol Paone</t>
+  </si>
+  <si>
+    <t>Peter Facinelli, Nick Lyon</t>
+  </si>
+  <si>
+    <t>Peter Lepeniotis</t>
   </si>
   <si>
     <t>Kaige Chen</t>
   </si>
   <si>
-    <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
-  </si>
-  <si>
-    <t>Big Picture RanchBenenson Productions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
+    <t>Joshua Tickell, Rebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Sébastien Marnier</t>
+  </si>
+  <si>
+    <t>Bethann Hardison, Frédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Klaus Härö</t>
+  </si>
+  <si>
+    <t>Stephen Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Danny O'Malley, Alex Rivest</t>
   </si>
   <si>
     <t>Richard Dewey</t>
   </si>
   <si>
-    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
-  </si>
-  <si>
     <t>Aristotle Torres</t>
   </si>
   <si>
-    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
+    <t>Hiroshi Akabane</t>
   </si>
   <si>
     <t>Luca Balser</t>
   </si>
   <si>
-    <t>Gummy Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
-  </si>
-  <si>
-    <t>Hiroshi Akabane</t>
-  </si>
-  <si>
-    <t>HS ProductionsIRH Press Co.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
+    <t>Adil El Arbi, Bilall Fallah</t>
   </si>
   <si>
     <t>John Stalberg Jr.</t>
   </si>
   <si>
-    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
-  </si>
-  <si>
     <t>Jude Okwudiafor Johnson</t>
   </si>
   <si>
-    <t>Anchor Media Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
-  </si>
-  <si>
-    <t>World's Fair Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
+    <t>Cru Ennis, Lee Roy Kunz</t>
   </si>
   <si>
     <t>Andrea Di Stefano</t>
   </si>
   <si>
-    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
-  </si>
-  <si>
     <t>Miguel Ángel Vivas</t>
   </si>
   <si>
-    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
-  </si>
-  <si>
     <t>Frank Cimière</t>
   </si>
   <si>
-    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marc Missonnier ... producer </t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3038479105/?ref_=bo_md_table_3</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl216040193/?ref_=bo_md_table_4</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1926595329/?ref_=bo_md_table_5</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl780174081/?ref_=bo_md_table_6</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1035043585/?ref_=bo_md_table_28</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3488318209/?ref_=bo_md_table_29</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl866943745/?ref_=bo_md_table_30</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1739555585/?ref_=bo_md_table_31</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1605337857/?ref_=bo_md_table_32</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1436386049/?ref_=bo_md_table_33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,000,378
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,388,017
-</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl2783019777/?ref_=bo_md_table_8</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl2106360577/?ref_=bo_md_table_9</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3568206593/?ref_=bo_md_table_36</t>
-  </si>
-  <si>
-    <t>20th Century StudiosKinberg GenreScott Free ProductionsTSG EntertainmentThe Mark Gordon Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enrico Ballarin ... line producer: Venice  Kenneth Branagh ... producer (p.g.a.) Martin Curry ... associate producer  Mark Gordon ... executive producer  Judy Hofflund ... producer (p.g.a.) Louise Killin ... executive producer  Simon Kinberg ... producer  James Prichard ... executive producer  Ridley Scott ... producer </t>
-  </si>
-  <si>
-    <t>Focus FeaturesGold Circle FilmsHome Box Office (HBO)Playtone</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paul Brooks ... executive producer  Michael P. Flannigan ... executive producer  Gary Goetzman ... producer  Tom Hanks ... producer  Scott Niemeyer ... executive producer  Eric Quijano ... associate producer  Kostas Raftopoulos ... line producer: Greece  Steve Shareshian ... executive producer  Julie Shimer ... associate producer (as Julie Shimer Lawrence) Jonathan Shore ... co-producer  Nia Vardalos ... executive producer  Rita Wilson ... producer (produced by)(p.g.a)</t>
-  </si>
-  <si>
-    <t>Red Chillies Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gauri Khan ... producer  Gaurav Verma ... co-producer </t>
-  </si>
-  <si>
     <t xml:space="preserve">89,060,830
 </t>
   </si>
@@ -782,38 +1022,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">4,600,137
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,482,605
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,602,988
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,973,543
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,108,247
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,108,247
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">409,313
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">423,024
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">376,719
 </t>
   </si>
@@ -838,14 +1046,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">88,910
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88,910
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">81,599
 </t>
   </si>
@@ -854,30 +1054,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">69,748
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">171,463
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,535
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,535
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,570
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,570
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">14,419
 </t>
   </si>
@@ -886,14 +1062,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">13,273
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,273
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">5,300
 </t>
   </si>
@@ -908,301 +1076,16 @@
     <t>https://www.boxofficemojo.com/release/rl3028583169/?ref_=bo_md_table_11</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3584983809/?ref_=bo_md_table_18</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl984056577/?ref_=bo_md_table_19</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_24</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_25</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl464618241/?ref_=bo_md_table_26</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3182002945/?ref_=bo_md_table_27</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl1722778369/?ref_=bo_md_table_37</t>
-  </si>
-  <si>
-    <t>https://www.boxofficemojo.com/release/rl3719136001/?ref_=bo_md_table_38</t>
-  </si>
-  <si>
-    <t>Antoine Fuqua</t>
-  </si>
-  <si>
-    <t>Michael Chaves</t>
-  </si>
-  <si>
-    <t>Cal Brunker</t>
-  </si>
-  <si>
-    <t>Kenneth Branagh</t>
-  </si>
-  <si>
-    <t>Kevin Greutert</t>
-  </si>
-  <si>
     <t>Aldea M EstudiosCorazón FilmsLions Gate FilmsLionsgate ProductionsTwisted Pictures</t>
   </si>
   <si>
-    <t>Nia Vardalos</t>
-  </si>
-  <si>
-    <t>Gareth Edwards</t>
-  </si>
-  <si>
-    <t>Scott Waugh</t>
-  </si>
-  <si>
-    <t>Atlee</t>
-  </si>
-  <si>
-    <t>Andrew Hyatt</t>
-  </si>
-  <si>
-    <t>Craig Gillespie</t>
-  </si>
-  <si>
-    <t>Black Bear PicturesColumbia PicturesRyder Picture CompanySony Pictures Entertainment (SPE)Stage 6 Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rebecca Angelo ... executive producer  Lauren Schuker Blum ... executive producer  Loren Brock ... line producer: LA unit  Christopher Casanova ... co-producer  John Friedberg ... executive producer  Craig Gillespie ... producer  Michael Heimler ... executive producer  Johnny Holland ... executive producer  Ben Mezrich ... executive producer  Johnny Pariseau ... co-producer  Aaron Ryder ... producer (produced by)(p.g.a.) Teddy Schwarzman ... producer  Claire Severance ... associate producer  Andrew Swett ... executive producer  Kevin Ulrich ... executive producer  Cameron Winklevoss ... executive producer  Tyler Winklevoss ... executive producer </t>
-  </si>
-  <si>
-    <t>Bishal Dutta</t>
-  </si>
-  <si>
-    <t>Jonathan Demme</t>
-  </si>
-  <si>
-    <t>Aitch Alberto</t>
-  </si>
-  <si>
-    <t>Boies Schiller Entertainment3Pas Studios5000 Broadway ProductionsBig Swing ProductionsLimelight</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aitch Alberto ... executive producer  Meredith Bagby ... executive producer  David Boies ... executive producer  Eugenio Derbez ... producer  Nicole Flores ... line producer  Lin-Manuel Miranda ... producer  Ben Odell ... producer  Owen Panettieri ... co-producer  Chris Parker ... producer  Zack Schiller ... executive producer  Kyra Sedgwick ... producer  Dylan Sellers ... producer  Valerie Stadler ... producer </t>
-  </si>
-  <si>
-    <t>Jim Capobianco, Pierre-Luc Granjon</t>
-  </si>
-  <si>
-    <t>Nicol Paone</t>
-  </si>
-  <si>
-    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
-  </si>
-  <si>
-    <t>Peter Facinelli, Nick Lyon</t>
-  </si>
-  <si>
-    <t>Lone Star StorytellersMedia GroupSC Films International</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
-  </si>
-  <si>
-    <t>Peter Lepeniotis</t>
-  </si>
-  <si>
-    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
-  </si>
-  <si>
-    <t>Joshua Tickell, Rebecca Harrell Tickell</t>
-  </si>
-  <si>
-    <t>Sébastien Marnier</t>
-  </si>
-  <si>
-    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
-  </si>
-  <si>
-    <t>Bethann Hardison, Frédéric Tcheng</t>
-  </si>
-  <si>
-    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
-  </si>
-  <si>
-    <t>Klaus Härö</t>
-  </si>
-  <si>
-    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
-  </si>
-  <si>
-    <t>Stephen Gyllenhaal</t>
-  </si>
-  <si>
-    <t>Upstream Pictures (II)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
-  </si>
-  <si>
-    <t>Danny O'Malley, Alex Rivest</t>
-  </si>
-  <si>
-    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
-  </si>
-  <si>
-    <t>Adil El Arbi, Bilall Fallah</t>
-  </si>
-  <si>
-    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
-  </si>
-  <si>
-    <t>Cru Ennis, Lee Roy Kunz</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>King Arthur</t>
-  </si>
-  <si>
-    <t>PAW Patrol: The Movie</t>
-  </si>
-  <si>
-    <t>Thor: The Dark World</t>
-  </si>
-  <si>
-    <t>Titanic</t>
-  </si>
-  <si>
-    <t>My Big Fat Greek Wedding</t>
-  </si>
-  <si>
-    <t>Rogue One: A Star Wars Story</t>
-  </si>
-  <si>
-    <t>Need for Speed</t>
-  </si>
-  <si>
-    <t>Paul, Apostle of Christ</t>
-  </si>
-  <si>
-    <t>Cruella</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>The Butcher, the Chef, and the Swordsman</t>
-  </si>
-  <si>
-    <t>A Question of Faith</t>
-  </si>
-  <si>
-    <t>Jim Capobianco</t>
-  </si>
-  <si>
-    <t>The Lion King</t>
-  </si>
-  <si>
-    <t>Pierre-Luc Granjon</t>
-  </si>
-  <si>
-    <t>Zibilla</t>
-  </si>
-  <si>
-    <t>The Battle at Lake Changjin</t>
-  </si>
-  <si>
-    <t>Peter Facinelli</t>
-  </si>
-  <si>
-    <t>Nick Lyon</t>
-  </si>
-  <si>
-    <t>Toy Story 2</t>
-  </si>
-  <si>
-    <t>Joshua Tickell</t>
-  </si>
-  <si>
-    <t>Rebecca Harrell Tickell</t>
-  </si>
-  <si>
-    <t>Pump</t>
-  </si>
-  <si>
-    <t>Bethann Hardison</t>
-  </si>
-  <si>
-    <t>Frédéric Tcheng</t>
-  </si>
-  <si>
-    <t>Shortbus</t>
-  </si>
-  <si>
-    <t>Letters to Father Jacob</t>
-  </si>
-  <si>
-    <t>Danny O'Malley</t>
-  </si>
-  <si>
-    <t>Amanda Knox</t>
-  </si>
-  <si>
-    <t>Alex Rivest</t>
-  </si>
-  <si>
-    <t>Uncut Gems</t>
-  </si>
-  <si>
-    <t>Adil El Arbi</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Bilall Fallah</t>
-  </si>
-  <si>
-    <t>Bad Boys for Life</t>
-  </si>
-  <si>
-    <t>High School</t>
-  </si>
-  <si>
-    <t>Cru Ennis</t>
-  </si>
-  <si>
-    <t>Boys of Abu Ghraib</t>
-  </si>
-  <si>
-    <t>Lee Roy Kunz</t>
-  </si>
-  <si>
-    <t>Escobar: Paradise Lost</t>
-  </si>
-  <si>
-    <t>Extinction</t>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Highest grossing movie</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -1635,559 +1518,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03BAF43-B1E7-49EA-9442-5DB7CCE34CD8}">
-  <dimension ref="A1:C52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681D622B-EB0F-41D0-A912-C092F28EB24E}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
         <v>318</v>
       </c>
-      <c r="C2">
-        <v>203567857</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C1" t="s">
         <v>319</v>
-      </c>
-      <c r="C4">
-        <v>144327371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B5" t="s">
-        <v>320</v>
-      </c>
-      <c r="C5">
-        <v>644783140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>272</v>
-      </c>
-      <c r="B6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6">
-        <v>2264743305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>274</v>
-      </c>
-      <c r="B7" t="s">
-        <v>322</v>
-      </c>
-      <c r="C7">
-        <v>368744044</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C8">
-        <v>1058682142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" t="s">
-        <v>324</v>
-      </c>
-      <c r="C9">
-        <v>203277636</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>277</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>27514156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>278</v>
-      </c>
-      <c r="B11" t="s">
-        <v>325</v>
-      </c>
-      <c r="C11">
-        <v>25915966</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" t="s">
-        <v>326</v>
-      </c>
-      <c r="C12">
-        <v>233503234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>282</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>5482605</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>283</v>
-      </c>
-      <c r="B14" t="s">
-        <v>327</v>
-      </c>
-      <c r="C14">
-        <v>206678440</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15">
-        <v>1606339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" t="s">
-        <v>328</v>
-      </c>
-      <c r="C16">
-        <v>2089266</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" t="s">
-        <v>329</v>
-      </c>
-      <c r="C17">
-        <v>2587072</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18">
-        <v>503378</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19">
-        <v>423024</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>284</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20">
-        <v>407838</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21">
-        <v>376719</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22">
-        <v>319848</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>330</v>
-      </c>
-      <c r="B23" t="s">
-        <v>331</v>
-      </c>
-      <c r="C23">
-        <v>968511805</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>332</v>
-      </c>
-      <c r="B24" t="s">
-        <v>333</v>
-      </c>
-      <c r="C24">
-        <v>88667</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>154</v>
-      </c>
-      <c r="B26" t="s">
-        <v>334</v>
-      </c>
-      <c r="C26">
-        <v>902548476</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>288</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27">
-        <v>617143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>335</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28">
-        <v>205118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>336</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29">
-        <v>205118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>294</v>
-      </c>
-      <c r="B30" t="s">
-        <v>337</v>
-      </c>
-      <c r="C30">
-        <v>497375381</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>338</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31">
-        <v>88910</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>339</v>
-      </c>
-      <c r="B32" t="s">
-        <v>340</v>
-      </c>
-      <c r="C32">
-        <v>89787</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>298</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33">
-        <v>1120899</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>341</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>342</v>
-      </c>
-      <c r="B35" t="s">
-        <v>343</v>
-      </c>
-      <c r="C35">
-        <v>5557564</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>304</v>
-      </c>
-      <c r="B36" t="s">
-        <v>344</v>
-      </c>
-      <c r="C36">
-        <v>1332577</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>307</v>
-      </c>
-      <c r="B37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37">
-        <v>38683</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>345</v>
-      </c>
-      <c r="B38" t="s">
-        <v>346</v>
-      </c>
-      <c r="C38">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>347</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>159</v>
-      </c>
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40">
-        <v>32535</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>161</v>
-      </c>
-      <c r="B41" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41">
-        <v>25570</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>167</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" t="s">
-        <v>348</v>
-      </c>
-      <c r="C43">
-        <v>50023780</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>349</v>
-      </c>
-      <c r="B44" t="s">
-        <v>350</v>
-      </c>
-      <c r="C44">
-        <v>1692776</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>351</v>
-      </c>
-      <c r="B45" t="s">
-        <v>352</v>
-      </c>
-      <c r="C45">
-        <v>426505244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" t="s">
-        <v>353</v>
-      </c>
-      <c r="C46">
-        <v>221590</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>173</v>
-      </c>
-      <c r="B47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47">
-        <v>5300</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>354</v>
-      </c>
-      <c r="B48" t="s">
-        <v>355</v>
-      </c>
-      <c r="C48">
-        <v>62096</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>356</v>
-      </c>
-      <c r="B49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49">
-        <v>4883</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>178</v>
-      </c>
-      <c r="B50" t="s">
-        <v>357</v>
-      </c>
-      <c r="C50">
-        <v>6760531</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" t="s">
-        <v>358</v>
-      </c>
-      <c r="C51">
-        <v>2350695</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>184</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2199,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,22 +1609,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>282</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>209</v>
+        <v>283</v>
       </c>
       <c r="G2" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2285,22 +1638,22 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>210</v>
+        <v>284</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>211</v>
+        <v>285</v>
       </c>
       <c r="G3" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2308,28 +1661,28 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>212</v>
+        <v>286</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>213</v>
+        <v>287</v>
       </c>
       <c r="G4" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2337,28 +1690,28 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>214</v>
+        <v>288</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>215</v>
+        <v>289</v>
       </c>
       <c r="G5" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2366,28 +1719,28 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>216</v>
+        <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>217</v>
+        <v>291</v>
       </c>
       <c r="G6" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2395,28 +1748,28 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>218</v>
+        <v>292</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>219</v>
+        <v>293</v>
       </c>
       <c r="G7" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -2430,22 +1783,22 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>220</v>
+        <v>294</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>221</v>
+        <v>295</v>
       </c>
       <c r="G8" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="255" x14ac:dyDescent="0.25">
@@ -2453,28 +1806,28 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>222</v>
+        <v>296</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>223</v>
+        <v>297</v>
       </c>
       <c r="G9" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2482,28 +1835,28 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2511,28 +1864,28 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>314</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>225</v>
+        <v>299</v>
       </c>
       <c r="G11" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -2540,28 +1893,28 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>315</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>227</v>
+        <v>301</v>
       </c>
       <c r="G12" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>280</v>
+        <v>126</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>281</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2575,22 +1928,22 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="G13" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="H13" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2604,22 +1957,22 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G14" t="s">
-        <v>283</v>
+        <v>250</v>
       </c>
       <c r="H14" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2633,22 +1986,22 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s">
-        <v>128</v>
+        <v>251</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2662,22 +2015,22 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="G16" t="s">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="H16" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2691,22 +2044,22 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="G17" t="s">
-        <v>134</v>
+        <v>253</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -2720,22 +2073,22 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G18" t="s">
-        <v>137</v>
+        <v>254</v>
       </c>
       <c r="H18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2743,28 +2096,28 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>255</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2772,28 +2125,28 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="H20" t="s">
-        <v>285</v>
+        <v>225</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>286</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2807,16 +2160,16 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>236</v>
+        <v>302</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>237</v>
+        <v>303</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="H21" t="s">
         <v>144</v>
@@ -2836,22 +2189,22 @@
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G22" t="s">
+        <v>258</v>
+      </c>
+      <c r="H22" t="s">
         <v>146</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="330" x14ac:dyDescent="0.25">
@@ -2865,22 +2218,22 @@
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="H23" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2894,422 +2247,422 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>238</v>
+        <v>304</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>239</v>
+        <v>305</v>
       </c>
       <c r="G24" t="s">
+        <v>260</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>262</v>
+        <v>46</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>240</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>241</v>
+        <v>92</v>
       </c>
       <c r="G25" t="s">
-        <v>154</v>
+        <v>261</v>
       </c>
       <c r="H25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="405" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>263</v>
+        <v>48</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G26" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>289</v>
+        <v>154</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>50</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="G27" t="s">
-        <v>291</v>
+        <v>263</v>
       </c>
       <c r="H27" t="s">
-        <v>292</v>
+        <v>156</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>265</v>
+        <v>52</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>91</v>
+        <v>306</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
+        <v>307</v>
       </c>
       <c r="G28" t="s">
-        <v>294</v>
+        <v>264</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>295</v>
+        <v>158</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>296</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="G29" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="H29" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>299</v>
+        <v>227</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>300</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>244</v>
+        <v>308</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>245</v>
+        <v>309</v>
       </c>
       <c r="G31" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="H31" t="s">
-        <v>302</v>
+        <v>229</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>303</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="G32" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="H32" t="s">
-        <v>305</v>
+        <v>231</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>306</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="H33" t="s">
-        <v>308</v>
+        <v>233</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>309</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G34" t="s">
-        <v>310</v>
+        <v>270</v>
       </c>
       <c r="H34" t="s">
-        <v>311</v>
+        <v>235</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>312</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="G35" t="s">
-        <v>159</v>
+        <v>271</v>
       </c>
       <c r="H35" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="G36" t="s">
-        <v>161</v>
+        <v>272</v>
       </c>
       <c r="H36" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>252</v>
+        <v>310</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>253</v>
+        <v>311</v>
       </c>
       <c r="G37" t="s">
+        <v>273</v>
+      </c>
+      <c r="H37" t="s">
         <v>167</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>266</v>
+        <v>222</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="G38" t="s">
-        <v>164</v>
+        <v>274</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>165</v>
@@ -3320,205 +2673,205 @@
     </row>
     <row r="39" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>223</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G39" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
       <c r="H39" t="s">
-        <v>314</v>
+        <v>237</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>315</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G40" t="s">
+        <v>276</v>
+      </c>
+      <c r="H40" t="s">
+        <v>169</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="H40" t="s">
-        <v>171</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>256</v>
+        <v>312</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>257</v>
+        <v>313</v>
       </c>
       <c r="G41" t="s">
-        <v>173</v>
+        <v>277</v>
       </c>
       <c r="H41" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G42" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
       <c r="H42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G43" t="s">
-        <v>178</v>
+        <v>279</v>
       </c>
       <c r="H43" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G44" t="s">
-        <v>181</v>
+        <v>280</v>
       </c>
       <c r="H44" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G45" t="s">
-        <v>184</v>
+        <v>281</v>
       </c>
       <c r="H45" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I45" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prepare spreadsheet for merging
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\se762\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA456FE-1786-4A6B-BD63-1D079FE2538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337BD0AD-2507-4262-A7F7-E3BD5A06B94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="Directors" sheetId="3" r:id="rId1"/>
     <sheet name="MovieInfo" sheetId="2" r:id="rId2"/>
-    <sheet name="Director's Highest gross Films" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="315">
   <si>
     <t>Film Title</t>
   </si>
@@ -52,9 +51,6 @@
     <t>Domestic Gross</t>
   </si>
   <si>
-    <t>International Gross</t>
-  </si>
-  <si>
     <t>Worldwide Gross</t>
   </si>
   <si>
@@ -274,9 +270,6 @@
     <t>https://www.boxofficemojo.com/release/rl1303282433/?ref_=bo_md_table_44</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">14,735,611
 </t>
   </si>
@@ -1077,15 +1070,6 @@
   </si>
   <si>
     <t>Aldea M EstudiosCorazón FilmsLions Gate FilmsLionsgate ProductionsTwisted Pictures</t>
-  </si>
-  <si>
-    <t>Director</t>
-  </si>
-  <si>
-    <t>Highest grossing movie</t>
-  </si>
-  <si>
-    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1165,19 +1149,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -1192,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1200,8 +1171,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1522,7 +1492,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,14 +1503,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C1" t="s">
-        <v>319</v>
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1550,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB63AF4-255B-4F4F-A06E-18EAB1273824}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,1357 +1532,1188 @@
     <col min="2" max="2" width="73.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="134.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="134.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="G2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="F2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="G4" t="s">
-        <v>240</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="G6" t="s">
-        <v>242</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G7" t="s">
-        <v>243</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="G8" t="s">
-        <v>244</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="G9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F9" t="s">
+        <v>243</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" t="s">
-        <v>246</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>244</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G11" t="s">
-        <v>248</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="G12" t="s">
-        <v>247</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" t="s">
+        <v>247</v>
       </c>
       <c r="G13" t="s">
-        <v>249</v>
-      </c>
-      <c r="H13" t="s">
-        <v>130</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" t="s">
+        <v>248</v>
       </c>
       <c r="G14" t="s">
-        <v>250</v>
-      </c>
-      <c r="H14" t="s">
-        <v>132</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" t="s">
-        <v>251</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>249</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F16" t="s">
+        <v>250</v>
       </c>
       <c r="G16" t="s">
-        <v>252</v>
-      </c>
-      <c r="H16" t="s">
-        <v>136</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G17" t="s">
-        <v>253</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F17" t="s">
+        <v>251</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>252</v>
       </c>
       <c r="G18" t="s">
-        <v>254</v>
-      </c>
-      <c r="H18" t="s">
-        <v>140</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G19" t="s">
-        <v>255</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F19" t="s">
+        <v>253</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>254</v>
       </c>
       <c r="G20" t="s">
-        <v>256</v>
-      </c>
-      <c r="H20" t="s">
-        <v>225</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
         <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F21" t="s">
+        <v>255</v>
       </c>
       <c r="G21" t="s">
-        <v>257</v>
-      </c>
-      <c r="H21" t="s">
-        <v>144</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" t="s">
+        <v>256</v>
       </c>
       <c r="G22" t="s">
-        <v>258</v>
-      </c>
-      <c r="H22" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
         <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
+        <v>257</v>
       </c>
       <c r="G23" t="s">
-        <v>259</v>
-      </c>
-      <c r="H23" t="s">
-        <v>148</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="G24" t="s">
-        <v>260</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="405" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F24" t="s">
+        <v>258</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="405" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" t="s">
+        <v>259</v>
       </c>
       <c r="G25" t="s">
-        <v>261</v>
-      </c>
-      <c r="H25" t="s">
-        <v>152</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" t="s">
-        <v>262</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
         <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>50</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>261</v>
       </c>
       <c r="G27" t="s">
-        <v>263</v>
-      </c>
-      <c r="H27" t="s">
-        <v>156</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
         <v>51</v>
-      </c>
-      <c r="B28" t="s">
-        <v>52</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E28" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="G28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F28" t="s">
+        <v>262</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F29" t="s">
+        <v>263</v>
       </c>
       <c r="G29" t="s">
-        <v>265</v>
-      </c>
-      <c r="H29" t="s">
-        <v>160</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" t="s">
-        <v>266</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" t="s">
+        <v>264</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E31" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F31" t="s">
+        <v>265</v>
       </c>
       <c r="G31" t="s">
-        <v>267</v>
-      </c>
-      <c r="H31" t="s">
-        <v>229</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" t="s">
+        <v>266</v>
       </c>
       <c r="G32" t="s">
-        <v>268</v>
-      </c>
-      <c r="H32" t="s">
-        <v>231</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" t="s">
+        <v>267</v>
       </c>
       <c r="G33" t="s">
-        <v>269</v>
-      </c>
-      <c r="H33" t="s">
-        <v>233</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>268</v>
       </c>
       <c r="G34" t="s">
-        <v>270</v>
-      </c>
-      <c r="H34" t="s">
-        <v>235</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>60</v>
       </c>
       <c r="C35">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E35" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F35" t="s">
+        <v>269</v>
       </c>
       <c r="G35" t="s">
-        <v>271</v>
-      </c>
-      <c r="H35" t="s">
-        <v>134</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
         <v>61</v>
-      </c>
-      <c r="B36" t="s">
-        <v>62</v>
       </c>
       <c r="C36">
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36" t="s">
-        <v>78</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F36" t="s">
+        <v>270</v>
       </c>
       <c r="G36" t="s">
-        <v>272</v>
-      </c>
-      <c r="H36" t="s">
-        <v>163</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C37">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E37" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F37" t="s">
+        <v>271</v>
       </c>
       <c r="G37" t="s">
-        <v>273</v>
-      </c>
-      <c r="H37" t="s">
-        <v>167</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C38">
         <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E38" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G38" t="s">
-        <v>274</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F38" t="s">
+        <v>272</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C39">
         <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" t="s">
+        <v>273</v>
       </c>
       <c r="G39" t="s">
-        <v>275</v>
-      </c>
-      <c r="H39" t="s">
-        <v>237</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
         <v>66</v>
-      </c>
-      <c r="B40" t="s">
-        <v>67</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" t="s">
+        <v>274</v>
       </c>
       <c r="G40" t="s">
-        <v>276</v>
-      </c>
-      <c r="H40" t="s">
-        <v>169</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
         <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>69</v>
       </c>
       <c r="C41">
         <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E41" t="s">
-        <v>78</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F41" t="s">
+        <v>275</v>
       </c>
       <c r="G41" t="s">
-        <v>277</v>
-      </c>
-      <c r="H41" t="s">
-        <v>171</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
         <v>70</v>
-      </c>
-      <c r="B42" t="s">
-        <v>71</v>
       </c>
       <c r="C42">
         <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E42" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" t="s">
+        <v>276</v>
       </c>
       <c r="G42" t="s">
-        <v>278</v>
-      </c>
-      <c r="H42" t="s">
-        <v>173</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" t="s">
         <v>72</v>
-      </c>
-      <c r="B43" t="s">
-        <v>73</v>
       </c>
       <c r="C43">
         <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" t="s">
+        <v>277</v>
       </c>
       <c r="G43" t="s">
-        <v>279</v>
-      </c>
-      <c r="H43" t="s">
-        <v>175</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" t="s">
         <v>74</v>
-      </c>
-      <c r="B44" t="s">
-        <v>75</v>
       </c>
       <c r="C44">
         <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E44" t="s">
-        <v>78</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" t="s">
+        <v>278</v>
       </c>
       <c r="G44" t="s">
-        <v>280</v>
-      </c>
-      <c r="H44" t="s">
-        <v>177</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" t="s">
         <v>76</v>
-      </c>
-      <c r="B45" t="s">
-        <v>77</v>
       </c>
       <c r="C45">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E45" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" t="s">
+        <v>279</v>
       </c>
       <c r="G45" t="s">
-        <v>281</v>
+        <v>177</v>
       </c>
       <c r="H45" t="s">
-        <v>179</v>
-      </c>
-      <c r="I45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="E46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C8FA34-854C-4FDF-A76D-37677D1C3B05}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
checked and everything works ok + fixed minor bug with inputting studio not found
</commit_message>
<xml_diff>
--- a/Movie_Data.xlsx
+++ b/Movie_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unifiles.uoa.auckland.ac.nz\myhome\Documents\UiPath\Group8-300-762\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154F0C64-A03A-4078-800F-53765561E3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4730C27E-7661-49B3-9FA4-C6440701251F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9360" activeTab="1" xr2:uid="{D64A0BB7-C040-40A0-96DB-DB75B657400A}"/>
   </bookViews>
   <sheets>
     <sheet name="MovieInfo" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="264">
   <si>
     <t>The Equalizer 3</t>
   </si>
@@ -180,27 +180,15 @@
     <t>Farewell My Concubine</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_24</t>
-  </si>
-  <si>
     <t>The Kill Room</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_25</t>
-  </si>
-  <si>
     <t>On Fire</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl464618241/?ref_=bo_md_table_26</t>
-  </si>
-  <si>
     <t>Zombie Town</t>
   </si>
   <si>
-    <t>https://www.boxofficemojo.com/release/rl3182002945/?ref_=bo_md_table_27</t>
-  </si>
-  <si>
     <t>Common Ground</t>
   </si>
   <si>
@@ -480,9 +468,6 @@
     <t xml:space="preserve"> Elliott 'Lee' Cowart ... co-executive producer  Donovan de Boer ... a film produced by  Makasha Dorsey ... associate producer  Grant Gilmore ... producer  Matthew Godbey ... executive producer (as Matthew Grant Godbey) Robert Goldman ... executive producer  Kevin Griffo ... executive producer  Kalon Jackson ... co-executive producer  Herb Kimble ... executive producer  Byron Minns ... producer (as Byron Keith Minns) Oscar Torres ... associate producer  Gillian White ... associate producer  Michael Jai White ... producer </t>
   </si>
   <si>
-    <t>Jim CapobiancoPierre-Luc Granjon</t>
-  </si>
-  <si>
     <t>Leo and KingAerial Contrivance WorkshopAlignCarte Blanche(in association with)Curiosity Rights(in association with)</t>
   </si>
   <si>
@@ -501,353 +486,357 @@
     <t>Kaige Chen</t>
   </si>
   <si>
+    <t>Nicol Paone</t>
+  </si>
+  <si>
+    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
+  </si>
+  <si>
+    <t>Lone Star StorytellersMedia GroupSC Films International</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
+  </si>
+  <si>
+    <t>Peter Lepeniotis</t>
+  </si>
+  <si>
+    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
+  </si>
+  <si>
+    <t>Big Picture RanchBenenson Productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
+  </si>
+  <si>
+    <t>Sébastien Marnier</t>
+  </si>
+  <si>
+    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
+  </si>
+  <si>
+    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
+  </si>
+  <si>
+    <t>Klaus Härö</t>
+  </si>
+  <si>
+    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
+  </si>
+  <si>
+    <t>Stephen Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Upstream Pictures (II)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
+  </si>
+  <si>
+    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
+  </si>
+  <si>
+    <t>Richard Dewey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
+  </si>
+  <si>
+    <t>Aristotle Torres</t>
+  </si>
+  <si>
+    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
+  </si>
+  <si>
+    <t>Hiroshi Akabane</t>
+  </si>
+  <si>
+    <t>HS ProductionsIRH Press Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
+  </si>
+  <si>
+    <t>Luca Balser</t>
+  </si>
+  <si>
+    <t>Gummy Films</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
+  </si>
+  <si>
+    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
+  </si>
+  <si>
+    <t>John Stalberg Jr.</t>
+  </si>
+  <si>
+    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
+  </si>
+  <si>
+    <t>Jude Okwudiafor Johnson</t>
+  </si>
+  <si>
+    <t>Anchor Media Studios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
+  </si>
+  <si>
+    <t>World's Fair Pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
+  </si>
+  <si>
+    <t>Andrea Di Stefano</t>
+  </si>
+  <si>
+    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
+  </si>
+  <si>
+    <t>Miguel Ángel Vivas</t>
+  </si>
+  <si>
+    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
+  </si>
+  <si>
+    <t>Frank Cimière</t>
+  </si>
+  <si>
+    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marc Missonnier ... producer </t>
+  </si>
+  <si>
+    <t>Antoine Fuqua</t>
+  </si>
+  <si>
+    <t>Columbia Pictures(presents)Eagle Pictures(in association with)Escape ArtistsZHIV ProductionsSony Pictures Entertainment (SPE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tarak Ben Ammar ... executive producer  Todd Black ... producer (produced by)(p.g.a.) David Bloomfield ... executive producer  Jason Blumenthal ... producer (produced by)(p.g.a.) Vito Colazzo ... line producer  Tony Eldridge ... producer (produced by) Antoine Fuqua ... producer (produced by)(p.g.a.) Andy Mitchell ... executive producer  Samir M. Patel ... executive producer (as Samir Patel) Guja Quaranta ... line producer  Kat Samick ... executive producer  Alex Siskin ... producer (produced by) Enzo Sisti ... executive producer  Michael Sloan ... producer (produced by) Steve Tisch ... producer (produced by) Clayton Townsend ... producer (produced by)(p.g.a.) Denzel Washington ... producer (produced by) Richard Wenk ... co-producer </t>
+  </si>
+  <si>
+    <t>King Arthur</t>
+  </si>
+  <si>
+    <t>PAW Patrol: The Movie</t>
+  </si>
+  <si>
+    <t>Rogue One: A Star Wars Story</t>
+  </si>
+  <si>
+    <t>Need for Speed</t>
+  </si>
+  <si>
+    <t>Paul, Apostle of Christ</t>
+  </si>
+  <si>
+    <t>Cruella</t>
+  </si>
+  <si>
+    <t>Jim Capobianco</t>
+  </si>
+  <si>
+    <t>Pierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t>The Battle at Lake Changjin</t>
+  </si>
+  <si>
+    <t>Peter Facinelli</t>
+  </si>
+  <si>
+    <t>Nick Lyon</t>
+  </si>
+  <si>
+    <t>Joshua Tickell</t>
+  </si>
+  <si>
+    <t>Rebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Bethann Hardison</t>
+  </si>
+  <si>
+    <t>Frédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Danny O'Malley</t>
+  </si>
+  <si>
+    <t>Alex Rivest</t>
+  </si>
+  <si>
+    <t>Adil El Arbi</t>
+  </si>
+  <si>
+    <t>Bilall Fallah</t>
+  </si>
+  <si>
+    <t>Bad Boys for Life</t>
+  </si>
+  <si>
+    <t>High School</t>
+  </si>
+  <si>
+    <t>Cru Ennis</t>
+  </si>
+  <si>
+    <t>Lee Roy Kunz</t>
+  </si>
+  <si>
+    <t>Escobar: Paradise Lost</t>
+  </si>
+  <si>
+    <t>Extinction</t>
+  </si>
+  <si>
+    <t>Film Title</t>
+  </si>
+  <si>
+    <t>Domestic Gross</t>
+  </si>
+  <si>
+    <t>Worldwide Gross</t>
+  </si>
+  <si>
+    <t>Film Director(s)</t>
+  </si>
+  <si>
+    <t>Film Studios</t>
+  </si>
+  <si>
+    <t>Film Producers</t>
+  </si>
+  <si>
+    <t>Film Director</t>
+  </si>
+  <si>
+    <t>Film URL</t>
+  </si>
+  <si>
+    <t>Film Rank</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl10715905/?ref_=bo_md_table_24</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl464618241/?ref_=bo_md_table_25</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl3182002945/?ref_=bo_md_table_26</t>
+  </si>
+  <si>
+    <t>https://www.boxofficemojo.com/release/rl1387234049/?ref_=bo_md_table_27</t>
+  </si>
+  <si>
+    <t>Jim Capobianco, Pierre-Luc Granjon</t>
+  </si>
+  <si>
+    <t>Peter Facinelli, Nick Lyon</t>
+  </si>
+  <si>
     <t>Beijing Film StudioTomson FilmsChina Film Co-Production Corporation</t>
   </si>
   <si>
     <t xml:space="preserve"> Feng Hsu ... producer  Jade Hsu ... executive producer  Pin Hsu ... executive producer  Zhenduo Li ... line producer  Donald Ranvaud ... associate producer  Sun Ying ... line producer  Xia Zhang ... line producer </t>
   </si>
   <si>
-    <t>Nicol Paone</t>
-  </si>
-  <si>
-    <t>Yale ProductionsBKStudiosBondIt Media Capital(in association with)Bradley Pilz ProductionsBuffalo 8 Productions(post production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cary Anderson ... executive producer  Jordan Beckerman ... producer  David J. Bell ... executive producer  Stephen Braun ... executive producer  Jay Burnley ... executive producer  Ash Christian ... executive producer  Anne Clements ... producer  Neal Cupersmith ... co-executive producer  Michael Day ... co-producer / line producer  James Di Giacomo ... executive producer  Nicholas Donnermeyer ... executive producer  Kahil Dotay ... executive producer  Kurt Ebner ... co-executive producer  Ulf Ek ... executive producer  Pedro Luis Cunha Farias ... co-executive producer  BK Fulton ... executive producer  Marc Fusco ... Creative Producer  Naomi George ... executive producer  David Gilbery ... executive producer  Bill Green ... executive producer  Vishwas Hannurkar ... executive producer  Matthew Helderman ... executive producer  Amanda Homer ... co-producer  Phil Hunt ... executive producer  Robert Kapp ... executive producer  Jon Keeyes ... producer  Megan Kelleher ... co-executive producer  Bill Kenwright ... producer  Tyler W. Konney ... executive producer  Bradley J Korman ... co-executive producer  Jesse Korman ... co-producer  Jason Kringstein ... executive producer  Jeffrey B. Larson ... co-executive producer  Scott Levenson ... executive producer  Jordan Yale Levine ... producer  Marina Masowietsky ... executive producer  Mark Maxey ... executive producer  Kimberly Montini ... co-producer  David Nazar ... executive producer  Ian Niles ... executive producer  Dominic Ottersbach ... co-producer  Jackie Palkovicz ... executive producer  Michael Palkovicz ... executive producer  Nicol Paone ... producer  Bradley Pilz ... executive producer  Vahik Pirhamzei ... Creative Producer  Russ Posternak ... executive producer  William Rosenfeld ... producer  Compton Ross ... executive producer  Michael J. Rothstein ... executive producer  Philip W. Shaltz ... executive producer  Richard Switzer ... executive producer  Luke Taylor ... executive producer  Dannielle Thomas ... producer  Uma Thurman ... producer  Jeffrey Tussi ... executive producer  Paul Wedgwood ... executive producer  Jason Weinberg ... producer  Nicholas Wirth ... executive producer  Jason Zibarras ... executive producer </t>
-  </si>
-  <si>
-    <t>Peter FacinelliNick Lyon</t>
-  </si>
-  <si>
-    <t>Lone Star StorytellersMedia GroupSC Films International</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beth Bruce ... producer  Simon Crowe ... executive producer  Peter Facinelli ... producer  Joe Fernandez ... executive producer  Matthew Joynes ... producer  Nick Lyon ... a film by / producer  Xander McCabe ... line producer  Suzanne Weinert ... producer  Peter Winther ... producer  Rob Witte ... executive producer </t>
-  </si>
-  <si>
-    <t>Peter Lepeniotis</t>
-  </si>
-  <si>
-    <t>Now Entertainment GroupTrimuse Entertainment Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> William Alexander ... associate producer  Dan Bernard ... executive producer  Yvonne M. Bernard ... executive producer  Micheline Blais ... co-producer  Victor Elizalde ... executive producer  John Gillespie ... executive producer / producer  Rakhee Gillespie ... executive producer  Mark Holdom ... executive producer  P. Jayakumar ... executive producer  Mayank Jhalani ... associate producer  Mark Kowalsky ... associate producer  Brendan McNeill ... associate producer  R.L. Stine ... executive producer  Paul Weber ... executive producer  Robert Wertheimer ... co-producer </t>
-  </si>
-  <si>
-    <t>Joshua TickellRebecca Harrell Tickell</t>
-  </si>
-  <si>
-    <t>Big Picture RanchBenenson Productions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jan Ellison Baszucki ... executive producer  Bill Benenson ... executive producer  Laurie Benenson ... executive producer  Corinne Bourdeau ... co-producer  Rosario Dawson ... executive producer  John Paul DeJoria ... executive producer  Eric Dillon ... producer  Ryland Engelhart ... co-producer / executive producer  Pamela B. Green ... executive producer  George Gund IV ... executive producer  Gloriana Gund ... executive producer  Diane Ladd ... executive producer  Julian Lennon ... executive producer  Adam Lewis ... executive producer  Melony Lewis ... executive producer  Christopher Lindstrom ... executive producer  Christiana Musk ... executive producer  Susan Rockefeller ... co-producer  Annie Roney ... executive producer  Regina K. Scully ... executive producer  Ian Somerhalder ... executive producer  Joshua Tickell ... producer  Rebecca Harrell Tickell ... producer </t>
-  </si>
-  <si>
-    <t>Sébastien Marnier</t>
-  </si>
-  <si>
-    <t>Avenue B Productionsmicro_scopemicro_scope(co-production)Poison Productions(co-production)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Caroline Bonmarchand ... producer  Luc Déry ... co-producer  Kim McCraw ... co-producer </t>
-  </si>
-  <si>
-    <t>Bethann HardisonFrédéric Tcheng</t>
-  </si>
-  <si>
-    <t>Cortés FilmworksFord Foundation - Just FilmsLane B ProductionsVogue StudiosWhitewater Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hallee Adelman ... executive producer  John Boccardo ... executive producer  Naomi Campbell ... executive producer  Lisa Cortes ... producer  James Paul Dallas ... Archive Producer / co-producer  Derek Esplin ... executive producer  Ivy Herman ... executive producer  Rebecca H. James ... associate producer  Robina Riccitiello ... co-executive producer  Rick Rosenthal ... executive producer  Nancy Stephens ... executive producer  Nancy Stephens ... executive producer  Chris Stolte ... co-executive producer  Heidi Stolte ... co-executive producer  Andrea van Beuren ... executive producer  Jeff Zimbalist ... executive producer </t>
-  </si>
-  <si>
-    <t>Klaus Härö</t>
-  </si>
-  <si>
-    <t>Making Movies OySamson Films(co-production)WRAP Fund(with the support of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kaarle Aho ... producer  David Collins ... producer  Kai Nordberg ... producer </t>
-  </si>
-  <si>
-    <t>Stephen Gyllenhaal</t>
-  </si>
-  <si>
-    <t>Upstream Pictures (II)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Meredith Blake ... executive producer  Laura Bretscher ... associate producer  Kathleen Man Gyllenhaal ... producer  Stephen Gyllenhaal ... producer  Lindsay Hadley ... executive producer  Melissa Hart ... associate producer  Heather Kahlert ... executive producer  Eric M. Klein ... co-producer  Bri Lageyre ... associate producer  Ambika Leigh ... associate producer  Dina Rahban ... co-producer  Casey Rogers ... co-producer </t>
-  </si>
-  <si>
-    <t>Danny O'MalleyAlex Rivest</t>
-  </si>
-  <si>
-    <t>APU ProductionsAct 4 EntertainmentBoardwalk PicturesEnd of The Road FilmsOscilloscope Laboratories</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paul Doucette  Jeff Russo </t>
-  </si>
-  <si>
-    <t>Richard Dewey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Richard Dewey ... producer  Nathan Epstein ... executive producer  Andy Fortenbacher ... producer  Chris Laszlo ... producer  David Light ... executive producer  Gerry Ohrstrom ... executive producer </t>
-  </si>
-  <si>
-    <t>Aristotle Torres</t>
-  </si>
-  <si>
-    <t>FirstGen Content(produced by)Dark Rabbit ProductionsFoxxhole ProductionsMero Mero ProductionsThe Space Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Robert Aguilar ... executive producer  Claude Amadeo ... executive producer  Martin Cabrera ... executive producer  Justin Cirulli ... associate producer  Michael D'Alto ... executive producer  Gus Deardoff ... executive producer  Jamie Foxx ... producer  Cemí Guzmán ... executive producer  Luis Guzmán ... executive producer  Randal Sandler ... executive producer  Lizzie Shapiro ... producer  Bernie Stern ... line producer  Aristotle Torres ... producer  Chris Triana ... executive producer  Datari Turner ... producer </t>
-  </si>
-  <si>
-    <t>Hiroshi Akabane</t>
-  </si>
-  <si>
-    <t>HS ProductionsIRH Press Co.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ryuho Okawa ... executive producer </t>
-  </si>
-  <si>
-    <t>Luca Balser</t>
-  </si>
-  <si>
-    <t>Gummy Films</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pauline Chalamet ... producer  Rachel Walden ... producer </t>
-  </si>
-  <si>
-    <t>Adil El ArbiBilall Fallah</t>
-  </si>
-  <si>
-    <t>Caviar FilmsCalach Films(co-production)Le Collectif 64(co-production)Beluga Tree(co-production)Vlaamse Radio en Televisie (VRT)(co-production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Anne Berger ... junior producer  Brahim Chioua ... co-producer  Marc Dujardin ... co-producer  Adil El Arbi ... executive producer  Diana Elbaum ... co-producer  Bilall Fallah ... executive producer  Jesus Gonzalez-Elvira ... co-producer  Bert Hamelinck ... producer  Saïd Hamich ... associate producer  Robin Kerremans ... executive producer  Vincent Maraval ... co-producer  Rula Nasser ... associate producer  David Ragonig ... line producer  Michael Sagol ... executive producer  Laura Scheerlinck ... Junior Producer  Dimitri Verbeeck ... producer  Clarissa Vermaak ... associate producer </t>
-  </si>
-  <si>
-    <t>John Stalberg Jr.</t>
-  </si>
-  <si>
-    <t>Slow BurnBroken Open PicturesHighland Film Group (HFG)Studio 507</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adam Beasley ... executive producer  Cindy Bru ... executive producer  Stephen Chrisanthus ... co-executive producer  Ford Corbett ... producer  Jatin Desai ... executive producer  Arianne Fraser ... executive producer  Greg Friedman ... executive producer  David Frigerio ... producer  David Guglielmo ... executive producer  B.D. Gunnell ... line producer / producer  Avi Haas ... executive producer  Joshua Harris ... executive producer  Michael Jefferson ... executive producer  Nathan Klingher ... producer  Roy Scott MacFarland ... executive producer  Tim O'Hair ... executive producer  Delphine Perrier ... executive producer  Scott Powell ... co-executive producer  Kyle Smithson ... executive producer  Dallas Sonnier ... executive producer  John Stalberg Jr.... producer  Anthony Standberry ... executive producer  Caleb Ward ... co-executive producer  Michael Weiss ... executive producer  Ryan Winterstern ... producer </t>
-  </si>
-  <si>
-    <t>Jude Okwudiafor Johnson</t>
-  </si>
-  <si>
-    <t>Anchor Media Studios</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carolyn Bird ... executive producer  Janice Brathwaite ... executive producer  Garfield Bryant ... executive producer  Nicole de Meneses ... line producer  Adam Okwudiafor Johnson ... executive producer  Dee Johnson ... executive producer  Joseph Okwudiafor Johnson ... co-producer / executive producer  Jude Okwudiafor Johnson ... producer  Zina Moore-McGlockton ... executive producer  Jite Okoloko ... executive producer  Angel Omoruan ... coordinating producer  Paresh Raghani ... executive producer  Jerry Stallworth ... executive producer </t>
-  </si>
-  <si>
-    <t>Cru EnnisLee Roy Kunz</t>
-  </si>
-  <si>
-    <t>World's Fair Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isaac Bauman ... producer  Cru Ennis ... producer  Kane Kunz ... producer  Lee Roy Kunz ... producer  Elina Litvinova ... producer  Lili Pilt ... line producer </t>
-  </si>
-  <si>
-    <t>Andrea Di Stefano</t>
-  </si>
-  <si>
-    <t>Indiana ProductionMeMo FilmsAdler EntertainmentVision DistributionSky Italia(in collaboration with)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marco Cohen ... producer  Marco Colombo ... producer  Fabrizio Donvito ... producer  Benedetto Habib ... producer  Fabio Lombardelli ... line producer  Alessandro Mascheroni ... executive producer  Francesco Melzi d'Eril ... producer  Marco Morabito ... executive producer  Daniel Campos Pavoncelli ... producer </t>
-  </si>
-  <si>
-    <t>Miguel Ángel Vivas</t>
-  </si>
-  <si>
-    <t>Amazon Prime VideoApache FilmsComunidad de MadridInstituto de la Cinematografía y de las Artes Audiovisuales (ICAA)México City Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enrique López Lavigne ... producer  Pilar Robla ... executive producer  Miguel Ángel Vivas ... associate producer </t>
-  </si>
-  <si>
-    <t>Frank Cimière</t>
-  </si>
-  <si>
-    <t>Moana FilmsCoupains Production(co-production)France 3 Cinéma(co-production)France Télévisions(participation)Canal+(participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marc Missonnier ... producer </t>
-  </si>
-  <si>
-    <t>Antoine Fuqua</t>
-  </si>
-  <si>
-    <t>Columbia Pictures(presents)Eagle Pictures(in association with)Escape ArtistsZHIV ProductionsSony Pictures Entertainment (SPE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tarak Ben Ammar ... executive producer  Todd Black ... producer (produced by)(p.g.a.) David Bloomfield ... executive producer  Jason Blumenthal ... producer (produced by)(p.g.a.) Vito Colazzo ... line producer  Tony Eldridge ... producer (produced by) Antoine Fuqua ... producer (produced by)(p.g.a.) Andy Mitchell ... executive producer  Samir M. Patel ... executive producer (as Samir Patel) Guja Quaranta ... line producer  Kat Samick ... executive producer  Alex Siskin ... producer (produced by) Enzo Sisti ... executive producer  Michael Sloan ... producer (produced by) Steve Tisch ... producer (produced by) Clayton Townsend ... producer (produced by)(p.g.a.) Denzel Washington ... producer (produced by) Richard Wenk ... co-producer </t>
-  </si>
-  <si>
-    <t>King Arthur</t>
-  </si>
-  <si>
-    <t>PAW Patrol: The Movie</t>
-  </si>
-  <si>
-    <t>Thor: The Dark World</t>
-  </si>
-  <si>
-    <t>Titanic</t>
-  </si>
-  <si>
-    <t>My Big Fat Greek Wedding</t>
-  </si>
-  <si>
-    <t>Rogue One: A Star Wars Story</t>
-  </si>
-  <si>
-    <t>Need for Speed</t>
-  </si>
-  <si>
-    <t>Paul, Apostle of Christ</t>
-  </si>
-  <si>
-    <t>Cruella</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>The Butcher, the Chef, and the Swordsman</t>
-  </si>
-  <si>
-    <t>A Question of Faith</t>
-  </si>
-  <si>
-    <t>Jim Capobianco</t>
-  </si>
-  <si>
-    <t>The Lion King</t>
-  </si>
-  <si>
-    <t>Pierre-Luc Granjon</t>
-  </si>
-  <si>
-    <t>Zibilla</t>
-  </si>
-  <si>
-    <t>The Battle at Lake Changjin</t>
-  </si>
-  <si>
-    <t>Peter Facinelli</t>
-  </si>
-  <si>
-    <t>Nick Lyon</t>
-  </si>
-  <si>
-    <t>Toy Story 2</t>
-  </si>
-  <si>
-    <t>Joshua Tickell</t>
-  </si>
-  <si>
-    <t>Rebecca Harrell Tickell</t>
-  </si>
-  <si>
-    <t>Pump</t>
-  </si>
-  <si>
-    <t>Bethann Hardison</t>
-  </si>
-  <si>
-    <t>Frédéric Tcheng</t>
-  </si>
-  <si>
-    <t>Shortbus</t>
-  </si>
-  <si>
-    <t>Letters to Father Jacob</t>
-  </si>
-  <si>
-    <t>Danny O'Malley</t>
-  </si>
-  <si>
-    <t>Amanda Knox</t>
-  </si>
-  <si>
-    <t>Alex Rivest</t>
-  </si>
-  <si>
-    <t>Uncut Gems</t>
-  </si>
-  <si>
-    <t>Adil El Arbi</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Bilall Fallah</t>
-  </si>
-  <si>
-    <t>Bad Boys for Life</t>
-  </si>
-  <si>
-    <t>High School</t>
-  </si>
-  <si>
-    <t>Cru Ennis</t>
-  </si>
-  <si>
-    <t>Boys of Abu Ghraib</t>
-  </si>
-  <si>
-    <t>Lee Roy Kunz</t>
-  </si>
-  <si>
-    <t>Escobar: Paradise Lost</t>
-  </si>
-  <si>
-    <t>Extinction</t>
-  </si>
-  <si>
-    <t>Film Title</t>
-  </si>
-  <si>
-    <t>Domestic Gross</t>
-  </si>
-  <si>
-    <t>Worldwide Gross</t>
-  </si>
-  <si>
-    <t>Film Director(s)</t>
-  </si>
-  <si>
-    <t>Film Studios</t>
-  </si>
-  <si>
-    <t>Film Producers</t>
-  </si>
-  <si>
-    <t>Film Director</t>
-  </si>
-  <si>
-    <t>Film URL</t>
-  </si>
-  <si>
-    <t>Film Rank</t>
+    <t>Joshua Tickell, Rebecca Harrell Tickell</t>
+  </si>
+  <si>
+    <t>Bethann Hardison, Frédéric Tcheng</t>
+  </si>
+  <si>
+    <t>Danny O'Malley, Alex Rivest</t>
+  </si>
+  <si>
+    <t>Adil El Arbi, Bilall Fallah</t>
+  </si>
+  <si>
+    <t>Cru Ennis, Lee Roy Kunz</t>
+  </si>
+  <si>
+    <t>Cinderella</t>
+  </si>
+  <si>
+    <t>Saw 3D</t>
+  </si>
+  <si>
+    <t>The Silence of the Lambs</t>
+  </si>
+  <si>
+    <t>Mojin: The Lost Legend</t>
+  </si>
+  <si>
+    <t>Titanic 666</t>
+  </si>
+  <si>
+    <t>The Nut Job</t>
+  </si>
+  <si>
+    <t>Dior and I</t>
+  </si>
+  <si>
+    <t>Mother of Mine</t>
+  </si>
+  <si>
+    <t>Losing Isaiah</t>
+  </si>
+  <si>
+    <t>Immortal Hero</t>
+  </si>
+  <si>
+    <t>Operation Portugal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -934,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -944,6 +933,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1275,28 +1265,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1316,13 +1306,13 @@
         <v>167605171</v>
       </c>
       <c r="F2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1342,13 +1332,13 @@
         <v>249149159</v>
       </c>
       <c r="F3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1368,13 +1358,13 @@
         <v>88950223</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1394,13 +1384,13 @@
         <v>103116671</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1420,13 +1410,13 @@
         <v>56984243</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1446,13 +1436,13 @@
         <v>36428526</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1472,13 +1462,13 @@
         <v>62992122</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1498,13 +1488,13 @@
         <v>27461442</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -1524,13 +1514,13 @@
         <v>27514156</v>
       </c>
       <c r="F10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1550,13 +1540,13 @@
         <v>10983467</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1576,13 +1566,13 @@
         <v>12365832</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1602,13 +1592,13 @@
         <v>5482605</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1628,13 +1618,13 @@
         <v>4388017</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1654,11 +1644,11 @@
         <v>1606339</v>
       </c>
       <c r="F15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -1678,13 +1668,13 @@
         <v>1973543</v>
       </c>
       <c r="F16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="345" x14ac:dyDescent="0.25">
@@ -1704,13 +1694,13 @@
         <v>1108247</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1730,13 +1720,13 @@
         <v>503378</v>
       </c>
       <c r="F18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1756,13 +1746,13 @@
         <v>423024</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1782,13 +1772,13 @@
         <v>407838</v>
       </c>
       <c r="F20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G20" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="375" x14ac:dyDescent="0.25">
@@ -1808,13 +1798,13 @@
         <v>376719</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1834,13 +1824,13 @@
         <v>319848</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1860,13 +1850,13 @@
         <v>306385</v>
       </c>
       <c r="F23" t="s">
-        <v>147</v>
+        <v>244</v>
       </c>
       <c r="G23" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1886,39 +1876,39 @@
         <v>224585</v>
       </c>
       <c r="F24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>240</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="4">
-        <v>168926</v>
+        <v>139358</v>
       </c>
       <c r="E25" s="4">
-        <v>168926</v>
+        <v>617143</v>
       </c>
       <c r="F25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G25" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -1926,85 +1916,85 @@
         <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>241</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="4">
-        <v>139358</v>
+        <v>205118</v>
       </c>
       <c r="E26" s="4">
-        <v>617143</v>
+        <v>205118</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
+        <v>245</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>242</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="4">
-        <v>205118</v>
+        <v>130802</v>
       </c>
       <c r="E27" s="4">
-        <v>205118</v>
+        <v>130802</v>
       </c>
       <c r="F27" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G27" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>243</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" s="4">
-        <v>130802</v>
+        <v>168926</v>
       </c>
       <c r="E28" s="4">
-        <v>130802</v>
+        <v>168926</v>
       </c>
       <c r="F28" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>163</v>
+        <v>246</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -2016,21 +2006,21 @@
         <v>88910</v>
       </c>
       <c r="F29" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
       <c r="G29" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -2042,21 +2032,21 @@
         <v>1120899</v>
       </c>
       <c r="F30" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -2068,21 +2058,21 @@
         <v>81599</v>
       </c>
       <c r="F31" t="s">
-        <v>171</v>
+        <v>249</v>
       </c>
       <c r="G31" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -2094,21 +2084,21 @@
         <v>171463</v>
       </c>
       <c r="F32" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G32" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -2120,21 +2110,21 @@
         <v>38683</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G33" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -2146,21 +2136,21 @@
         <v>35563</v>
       </c>
       <c r="F34" t="s">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="G34" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -2172,18 +2162,18 @@
         <v>32535</v>
       </c>
       <c r="F35" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -2195,21 +2185,21 @@
         <v>25570</v>
       </c>
       <c r="F36" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="G36" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -2221,21 +2211,21 @@
         <v>757434</v>
       </c>
       <c r="F37" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G37" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -2247,21 +2237,21 @@
         <v>13273</v>
       </c>
       <c r="F38" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -2273,21 +2263,21 @@
         <v>173121</v>
       </c>
       <c r="F39" t="s">
-        <v>194</v>
+        <v>251</v>
       </c>
       <c r="G39" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -2299,21 +2289,21 @@
         <v>7807</v>
       </c>
       <c r="F40" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="G40" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -2325,21 +2315,21 @@
         <v>5300</v>
       </c>
       <c r="F41" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G41" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -2351,21 +2341,21 @@
         <v>4883</v>
       </c>
       <c r="F42" t="s">
-        <v>203</v>
+        <v>252</v>
       </c>
       <c r="G42" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -2377,21 +2367,21 @@
         <v>4580566</v>
       </c>
       <c r="F43" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="G43" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -2403,21 +2393,21 @@
         <v>147849</v>
       </c>
       <c r="F44" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="G44" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -2429,13 +2419,13 @@
         <v>371989</v>
       </c>
       <c r="F45" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G45" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="H45" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2458,556 +2448,568 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2">
+        <v>205</v>
+      </c>
+      <c r="C2" s="7">
         <v>203567857</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>249149159</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C4">
+        <v>206</v>
+      </c>
+      <c r="C4" s="7">
         <v>144327371</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5">
-        <v>644783140</v>
+        <v>253</v>
+      </c>
+      <c r="C5" s="7">
+        <v>542358331</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6">
-        <v>2264743305</v>
+        <v>254</v>
+      </c>
+      <c r="C6" s="7">
+        <v>136151680</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C7">
-        <v>368744044</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="7">
+        <v>36428526</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C8">
+        <v>207</v>
+      </c>
+      <c r="C8" s="7">
         <v>1058682142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C9">
+        <v>208</v>
+      </c>
+      <c r="C9" s="7">
         <v>203277636</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>27514156</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
-      </c>
-      <c r="C11">
+        <v>209</v>
+      </c>
+      <c r="C11" s="7">
         <v>25915966</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C12">
+        <v>210</v>
+      </c>
+      <c r="C12" s="7">
         <v>233503234</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>5482605</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
-      </c>
-      <c r="C14">
-        <v>206678440</v>
+        <v>255</v>
+      </c>
+      <c r="C14" s="7">
+        <v>272742922</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="7">
         <v>1606339</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>228</v>
-      </c>
-      <c r="C16">
-        <v>2089266</v>
+        <v>256</v>
+      </c>
+      <c r="C16" s="7">
+        <v>259368448</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17">
-        <v>2587072</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1108247</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <v>503378</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <v>423024</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="7">
         <v>407838</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="7">
         <v>376719</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>319848</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B23" t="s">
-        <v>231</v>
-      </c>
-      <c r="C23">
-        <v>968511805</v>
+        <v>42</v>
+      </c>
+      <c r="C23" s="7">
+        <v>306385</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
-      </c>
-      <c r="C24">
-        <v>88667</v>
+        <v>42</v>
+      </c>
+      <c r="C24" s="7">
+        <v>306385</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="7">
+        <v>224585</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>234</v>
-      </c>
-      <c r="C26">
-        <v>902548476</v>
+        <v>47</v>
+      </c>
+      <c r="C26" s="7">
+        <v>617143</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C27">
-        <v>617143</v>
+      <c r="C27" s="7">
+        <v>205118</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28">
-        <v>205118</v>
+        <v>257</v>
+      </c>
+      <c r="C28" s="7">
+        <v>214456</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>236</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29">
-        <v>205118</v>
+        <v>258</v>
+      </c>
+      <c r="C29" s="7">
+        <v>120885527</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
-        <v>237</v>
-      </c>
-      <c r="C30">
-        <v>497375381</v>
+        <v>213</v>
+      </c>
+      <c r="C30" s="7">
+        <v>902548476</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31">
-        <v>88910</v>
+        <v>218</v>
+      </c>
+      <c r="C31" s="7">
+        <v>89787</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="B32" t="s">
-        <v>240</v>
-      </c>
-      <c r="C32">
+        <v>218</v>
+      </c>
+      <c r="C32" s="7">
         <v>89787</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33">
+        <v>52</v>
+      </c>
+      <c r="C33" s="7">
         <v>1120899</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>241</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
+        <v>219</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="7">
+        <v>81599</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
-      </c>
-      <c r="C35">
-        <v>5557564</v>
+        <v>259</v>
+      </c>
+      <c r="C35" s="7">
+        <v>1769832</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B36" t="s">
-        <v>244</v>
-      </c>
-      <c r="C36">
-        <v>1332577</v>
+        <v>260</v>
+      </c>
+      <c r="C36" s="7">
+        <v>2851888</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37">
-        <v>38683</v>
+        <v>261</v>
+      </c>
+      <c r="C37" s="7">
+        <v>7603766</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>245</v>
-      </c>
-      <c r="B38" t="s">
-        <v>246</v>
-      </c>
-      <c r="C38">
-        <v>397</v>
+        <v>221</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>247</v>
-      </c>
-      <c r="C39">
+        <v>222</v>
+      </c>
+      <c r="C39" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40">
+        <v>62</v>
+      </c>
+      <c r="C40" s="7">
         <v>32535</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41">
+        <v>64</v>
+      </c>
+      <c r="C41" s="7">
         <v>25570</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>188</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="B42" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" s="7">
+        <v>6180032</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B43" t="s">
-        <v>248</v>
-      </c>
-      <c r="C43">
-        <v>50023780</v>
+        <v>68</v>
+      </c>
+      <c r="C43" s="7">
+        <v>13273</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="B44" t="s">
-        <v>250</v>
-      </c>
-      <c r="C44">
-        <v>1692776</v>
+        <v>225</v>
+      </c>
+      <c r="C44" s="7">
+        <v>426505244</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="B45" t="s">
-        <v>252</v>
-      </c>
-      <c r="C45">
+        <v>225</v>
+      </c>
+      <c r="C45" s="7">
         <v>426505244</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>253</v>
-      </c>
-      <c r="C46">
+        <v>226</v>
+      </c>
+      <c r="C46" s="7">
         <v>221590</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47">
+        <v>74</v>
+      </c>
+      <c r="C47" s="7">
         <v>5300</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="B48" t="s">
-        <v>255</v>
-      </c>
-      <c r="C48">
-        <v>62096</v>
+        <v>76</v>
+      </c>
+      <c r="C48" s="7">
+        <v>4883</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49">
+        <v>76</v>
+      </c>
+      <c r="C49" s="7">
         <v>4883</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>257</v>
-      </c>
-      <c r="C50">
+        <v>229</v>
+      </c>
+      <c r="C50" s="7">
         <v>6760531</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B51" t="s">
-        <v>258</v>
-      </c>
-      <c r="C51">
+        <v>230</v>
+      </c>
+      <c r="C51" s="7">
         <v>2350695</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>212</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
+        <v>199</v>
+      </c>
+      <c r="B52" t="s">
+        <v>263</v>
+      </c>
+      <c r="C52" s="7">
+        <v>3795575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>